<commit_message>
added oct 2 survival analysis
</commit_message>
<xml_diff>
--- a/data/survival/lab_survival/lab_survival.xlsx
+++ b/data/survival/lab_survival/lab_survival.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/survival/lab_survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC6764-DFBD-284D-BFEA-EFE650886EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A219F07-C342-ED4F-81D1-AB9807DA54C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30440" yWindow="-1120" windowWidth="25800" windowHeight="17440" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
+    <workbookView xWindow="-26980" yWindow="280" windowWidth="25800" windowHeight="17440" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -53,25 +53,13 @@
     <t>oyster</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>B4</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B5</t>
   </si>
   <si>
     <t>B1</t>
   </si>
   <si>
     <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
   </si>
   <si>
     <t>Control</t>
@@ -87,6 +75,9 @@
   </si>
   <si>
     <t>46C</t>
+  </si>
+  <si>
+    <t>18C</t>
   </si>
 </sst>
 </file>
@@ -115,7 +106,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF383A3C"/>
+      <color rgb="FF2A3243"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -480,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7ACAA-9959-8D4E-8E48-CFF679AAAAC5}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -531,34 +522,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B2">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="4">
-        <v>1</v>
+      <c r="J2" s="3">
+        <v>0</v>
       </c>
       <c r="K2" s="4">
         <v>1</v>
@@ -572,27 +563,27 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B3">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
       <c r="I3" s="3">
@@ -601,11 +592,11 @@
       <c r="J3" s="3">
         <v>0</v>
       </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
       </c>
       <c r="M3" s="4">
         <v>1</v>
@@ -613,31 +604,31 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B4">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
       </c>
       <c r="J4" s="4">
         <v>1</v>
@@ -654,27 +645,27 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B5">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
       <c r="I5" s="4">
@@ -695,31 +686,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B6">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
       </c>
       <c r="J6" s="4">
         <v>1</v>
@@ -736,27 +727,27 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B7">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>30</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>0</v>
       </c>
       <c r="I7" s="3">
@@ -765,11 +756,11 @@
       <c r="J7" s="3">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
       </c>
       <c r="M7" s="4">
         <v>1</v>
@@ -777,40 +768,40 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B8">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F8" s="2">
+        <v>33</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
       </c>
       <c r="M8" s="4">
         <v>1</v>
@@ -818,27 +809,27 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B9">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
+      <c r="C9">
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
+        <v>39</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>0</v>
       </c>
       <c r="I9" s="3">
@@ -859,27 +850,27 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B10">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>0</v>
       </c>
       <c r="I10" s="3">
@@ -891,40 +882,40 @@
       <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="4">
-        <v>1</v>
-      </c>
-      <c r="M10" s="4">
-        <v>1</v>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B11">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1</v>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
       </c>
       <c r="J11" s="4">
         <v>1</v>
@@ -941,31 +932,31 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B12">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1</v>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
       </c>
       <c r="J12" s="4">
         <v>1</v>
@@ -982,19 +973,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B13">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2">
         <v>28</v>
@@ -1002,8 +993,8 @@
       <c r="G13" s="2">
         <v>0</v>
       </c>
-      <c r="H13" s="2">
-        <v>0</v>
+      <c r="H13" s="4">
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
@@ -1023,31 +1014,31 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B14">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1</v>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -1064,31 +1055,31 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B15">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F15" s="2">
+        <v>13</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
       </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
@@ -1105,27 +1096,27 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B16">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>0</v>
       </c>
       <c r="I16" s="3">
@@ -1146,19 +1137,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B17">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2">
         <v>26</v>
@@ -1166,11 +1157,11 @@
       <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0</v>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1</v>
       </c>
       <c r="J17" s="4">
         <v>1</v>
@@ -1187,34 +1178,34 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B18">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <v>0</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
-      <c r="J18" s="3">
-        <v>0</v>
+      <c r="J18" s="4">
+        <v>1</v>
       </c>
       <c r="K18" s="4">
         <v>1</v>
@@ -1228,31 +1219,31 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B19">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F19" s="2">
+        <v>6</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1</v>
       </c>
       <c r="J19" s="4">
         <v>1</v>
@@ -1269,28 +1260,28 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B20">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
+      <c r="C20">
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
       </c>
-      <c r="H20" s="2">
-        <v>0</v>
+      <c r="H20" s="4">
+        <v>1</v>
       </c>
       <c r="I20" s="4">
         <v>1</v>
@@ -1310,37 +1301,37 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B21">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
+      <c r="C21">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0</v>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
@@ -1351,27 +1342,27 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
+      <c r="C22">
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="4">
@@ -1392,34 +1383,34 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
-        <v>5</v>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F23" s="2">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="3">
         <v>0</v>
       </c>
-      <c r="J23" s="3">
-        <v>0</v>
+      <c r="J23" s="4">
+        <v>1</v>
       </c>
       <c r="K23" s="4">
         <v>1</v>
@@ -1433,34 +1424,34 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B24">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
       </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1</v>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
       </c>
       <c r="K24" s="4">
         <v>1</v>
@@ -1474,37 +1465,37 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
-        <v>5</v>
+      <c r="C25">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F25" s="2">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>0</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
-      <c r="J25" s="4">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4">
-        <v>1</v>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
@@ -1515,34 +1506,34 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B26">
         <v>21</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F26" s="2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
-      <c r="J26" s="3">
-        <v>0</v>
+      <c r="J26" s="4">
+        <v>1</v>
       </c>
       <c r="K26" s="4">
         <v>1</v>
@@ -1556,27 +1547,27 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B27">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
+      <c r="C27">
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F27" s="2">
+        <v>32</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <v>0</v>
       </c>
       <c r="I27" s="3">
@@ -1585,8 +1576,8 @@
       <c r="J27" s="3">
         <v>0</v>
       </c>
-      <c r="K27" s="4">
-        <v>1</v>
+      <c r="K27" s="3">
+        <v>0</v>
       </c>
       <c r="L27" s="4">
         <v>1</v>
@@ -1597,78 +1588,78 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B28">
         <v>21</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="2">
         <v>16</v>
       </c>
-      <c r="F28" s="2">
-        <v>36</v>
-      </c>
       <c r="G28" s="2">
         <v>0</v>
       </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4">
-        <v>1</v>
-      </c>
-      <c r="K28" s="4">
-        <v>1</v>
-      </c>
-      <c r="L28" s="4">
-        <v>1</v>
-      </c>
-      <c r="M28" s="4">
-        <v>1</v>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B29">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
+      <c r="C29">
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F29" s="2">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
       </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="4">
-        <v>1</v>
-      </c>
-      <c r="K29" s="4">
-        <v>1</v>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
@@ -1679,27 +1670,27 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B30">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
+      <c r="C30">
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F30" s="2">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <v>0</v>
       </c>
       <c r="I30" s="3">
@@ -1711,43 +1702,43 @@
       <c r="K30" s="3">
         <v>0</v>
       </c>
-      <c r="L30" s="4">
-        <v>1</v>
-      </c>
-      <c r="M30" s="4">
-        <v>1</v>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B31">
         <v>21</v>
       </c>
-      <c r="C31" t="s">
-        <v>5</v>
+      <c r="C31">
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F31" s="2">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
       </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1</v>
       </c>
       <c r="K31" s="4">
         <v>1</v>
@@ -1761,27 +1752,27 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B32">
         <v>21</v>
       </c>
-      <c r="C32" t="s">
-        <v>5</v>
+      <c r="C32">
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F32" s="2">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="G32" s="2">
         <v>0</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <v>0</v>
       </c>
       <c r="I32" s="3">
@@ -1802,34 +1793,34 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B33">
         <v>21</v>
       </c>
-      <c r="C33" t="s">
-        <v>5</v>
+      <c r="C33">
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F33" s="2">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
       </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="4">
-        <v>1</v>
-      </c>
-      <c r="J33" s="4">
-        <v>1</v>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
       </c>
       <c r="K33" s="4">
         <v>1</v>
@@ -1843,34 +1834,34 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B34">
         <v>21</v>
       </c>
-      <c r="C34" t="s">
-        <v>5</v>
+      <c r="C34">
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="3">
         <v>0</v>
       </c>
-      <c r="J34" s="3">
-        <v>0</v>
+      <c r="J34" s="4">
+        <v>1</v>
       </c>
       <c r="K34" s="4">
         <v>1</v>
@@ -1884,34 +1875,34 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B35">
         <v>21</v>
       </c>
-      <c r="C35" t="s">
-        <v>5</v>
+      <c r="C35">
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F35" s="2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G35" s="2">
         <v>0</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="3">
         <v>0</v>
       </c>
-      <c r="J35" s="4">
-        <v>1</v>
+      <c r="J35" s="3">
+        <v>0</v>
       </c>
       <c r="K35" s="4">
         <v>1</v>
@@ -1925,27 +1916,27 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B36">
         <v>21</v>
       </c>
-      <c r="C36" t="s">
-        <v>5</v>
+      <c r="C36">
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F36" s="2">
+        <v>38</v>
       </c>
       <c r="G36" s="2">
         <v>0</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <v>0</v>
       </c>
       <c r="I36" s="3">
@@ -1954,11 +1945,11 @@
       <c r="J36" s="3">
         <v>0</v>
       </c>
-      <c r="K36" s="3">
-        <v>0</v>
+      <c r="K36" s="4">
+        <v>1</v>
       </c>
       <c r="L36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="4">
         <v>1</v>
@@ -1966,34 +1957,34 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B37">
         <v>21</v>
       </c>
-      <c r="C37" t="s">
-        <v>5</v>
+      <c r="C37">
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F37" s="2">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G37" s="2">
         <v>0</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>0</v>
       </c>
       <c r="I37" s="3">
         <v>0</v>
       </c>
-      <c r="J37" s="3">
-        <v>0</v>
+      <c r="J37" s="4">
+        <v>1</v>
       </c>
       <c r="K37" s="4">
         <v>1</v>
@@ -2007,34 +1998,34 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B38">
         <v>21</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
+      <c r="C38">
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
       </c>
-      <c r="H38" s="2">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="3">
-        <v>0</v>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1</v>
+      </c>
+      <c r="J38" s="4">
+        <v>1</v>
       </c>
       <c r="K38" s="4">
         <v>1</v>
@@ -2048,34 +2039,34 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B39">
         <v>21</v>
       </c>
-      <c r="C39" t="s">
-        <v>5</v>
+      <c r="C39">
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="F39" s="2">
+        <v>20</v>
       </c>
       <c r="G39" s="2">
         <v>0</v>
       </c>
-      <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
-        <v>0</v>
-      </c>
-      <c r="J39" s="3">
-        <v>0</v>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4">
+        <v>1</v>
       </c>
       <c r="K39" s="4">
         <v>1</v>
@@ -2089,37 +2080,37 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B40">
         <v>21</v>
       </c>
-      <c r="C40" t="s">
-        <v>5</v>
+      <c r="C40">
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F40" s="2">
+        <v>36</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
       </c>
-      <c r="H40" s="2">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <v>0</v>
-      </c>
-      <c r="J40" s="3">
-        <v>0</v>
-      </c>
-      <c r="K40" s="3">
-        <v>0</v>
+      <c r="H40" s="4">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1</v>
+      </c>
+      <c r="J40" s="4">
+        <v>1</v>
+      </c>
+      <c r="K40" s="4">
+        <v>1</v>
       </c>
       <c r="L40" s="4">
         <v>1</v>
@@ -2130,43 +2121,1683 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>45565</v>
+        <v>45567</v>
       </c>
       <c r="B41">
         <v>21</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="2">
+        <v>14</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>1</v>
+      </c>
+      <c r="J41" s="4">
+        <v>1</v>
+      </c>
+      <c r="K41" s="4">
+        <v>1</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B42">
+        <v>38</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="2">
+        <v>20</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B43">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="2">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B44">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="2">
+        <v>10</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B45">
+        <v>38</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="2">
+        <v>23</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="2">
+        <v>22</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B47">
+        <v>38</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="2">
+        <v>27</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B48">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="2">
+        <v>21</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B49">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="2">
+        <v>8</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B50">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="2">
+        <v>38</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0</v>
+      </c>
+      <c r="M50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B51">
+        <v>38</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="2">
+        <v>12</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0</v>
+      </c>
+      <c r="L51" s="3">
+        <v>0</v>
+      </c>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B52">
+        <v>38</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="2">
         <v>16</v>
       </c>
-      <c r="F41" s="2">
+      <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B53">
+        <v>38</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="2">
+        <v>3</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <v>0</v>
+      </c>
+      <c r="L53" s="3">
+        <v>0</v>
+      </c>
+      <c r="M53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B54">
+        <v>38</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="2">
+        <v>14</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B55">
+        <v>38</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="2">
+        <v>6</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0</v>
+      </c>
+      <c r="M55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B56">
+        <v>38</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="2">
+        <v>7</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B57">
+        <v>38</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="2">
+        <v>13</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0</v>
+      </c>
+      <c r="M57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B58">
+        <v>38</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="2">
+        <v>30</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+      <c r="M58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B59">
+        <v>38</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="2">
+        <v>22</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0</v>
+      </c>
+      <c r="M59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B60">
+        <v>38</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0</v>
+      </c>
+      <c r="M60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B61">
+        <v>38</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="2">
+        <v>18</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0</v>
+      </c>
+      <c r="M61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B62">
+        <v>21</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="2">
+        <v>26</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0</v>
+      </c>
+      <c r="M62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B63">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="2">
+        <v>17</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
+        <v>0</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3">
+        <v>0</v>
+      </c>
+      <c r="M63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B64">
+        <v>21</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="2">
+        <v>25</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0</v>
+      </c>
+      <c r="L64" s="3">
+        <v>0</v>
+      </c>
+      <c r="M64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B65">
+        <v>21</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="2">
         <v>37</v>
       </c>
-      <c r="G41" s="2">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0</v>
-      </c>
-      <c r="J41" s="4">
-        <v>1</v>
-      </c>
-      <c r="K41" s="4">
-        <v>1</v>
-      </c>
-      <c r="L41" s="4">
-        <v>1</v>
-      </c>
-      <c r="M41" s="4">
-        <v>1</v>
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+      <c r="M65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B66">
+        <v>21</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="2">
+        <v>16</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
+      </c>
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3">
+        <v>0</v>
+      </c>
+      <c r="M66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B67">
+        <v>21</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="2">
+        <v>21</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0</v>
+      </c>
+      <c r="M67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B68">
+        <v>21</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="2">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+      <c r="J68" s="3">
+        <v>0</v>
+      </c>
+      <c r="K68" s="3">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+      <c r="M68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B69">
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="2">
+        <v>5</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
+      <c r="J69" s="3">
+        <v>0</v>
+      </c>
+      <c r="K69" s="3">
+        <v>0</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B70">
+        <v>21</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="2">
+        <v>34</v>
+      </c>
+      <c r="G70" s="2">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+      <c r="J70" s="3">
+        <v>0</v>
+      </c>
+      <c r="K70" s="3">
+        <v>0</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B71">
+        <v>21</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="2">
+        <v>32</v>
+      </c>
+      <c r="G71" s="2">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0</v>
+      </c>
+      <c r="K71" s="3">
+        <v>0</v>
+      </c>
+      <c r="L71" s="3">
+        <v>0</v>
+      </c>
+      <c r="M71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B72">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="2">
+        <v>19</v>
+      </c>
+      <c r="G72" s="2">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3">
+        <v>0</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
+      <c r="J72" s="3">
+        <v>0</v>
+      </c>
+      <c r="K72" s="3">
+        <v>0</v>
+      </c>
+      <c r="L72" s="3">
+        <v>0</v>
+      </c>
+      <c r="M72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B73">
+        <v>21</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="2">
+        <v>12</v>
+      </c>
+      <c r="G73" s="2">
+        <v>0</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
+      <c r="J73" s="3">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3">
+        <v>0</v>
+      </c>
+      <c r="L73" s="3">
+        <v>0</v>
+      </c>
+      <c r="M73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B74">
+        <v>21</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="2">
+        <v>5</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0</v>
+      </c>
+      <c r="H74" s="3">
+        <v>0</v>
+      </c>
+      <c r="I74" s="3">
+        <v>0</v>
+      </c>
+      <c r="J74" s="3">
+        <v>0</v>
+      </c>
+      <c r="K74" s="3">
+        <v>0</v>
+      </c>
+      <c r="L74" s="3">
+        <v>0</v>
+      </c>
+      <c r="M74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B75">
+        <v>21</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="2">
+        <v>9</v>
+      </c>
+      <c r="G75" s="2">
+        <v>0</v>
+      </c>
+      <c r="H75" s="3">
+        <v>0</v>
+      </c>
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
+      <c r="J75" s="3">
+        <v>0</v>
+      </c>
+      <c r="K75" s="3">
+        <v>0</v>
+      </c>
+      <c r="L75" s="3">
+        <v>0</v>
+      </c>
+      <c r="M75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B76">
+        <v>21</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="2">
+        <v>7</v>
+      </c>
+      <c r="G76" s="2">
+        <v>0</v>
+      </c>
+      <c r="H76" s="3">
+        <v>0</v>
+      </c>
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
+      <c r="J76" s="3">
+        <v>0</v>
+      </c>
+      <c r="K76" s="3">
+        <v>0</v>
+      </c>
+      <c r="L76" s="3">
+        <v>0</v>
+      </c>
+      <c r="M76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B77">
+        <v>21</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="2">
+        <v>13</v>
+      </c>
+      <c r="G77" s="2">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3">
+        <v>0</v>
+      </c>
+      <c r="I77" s="3">
+        <v>0</v>
+      </c>
+      <c r="J77" s="3">
+        <v>0</v>
+      </c>
+      <c r="K77" s="3">
+        <v>0</v>
+      </c>
+      <c r="L77" s="3">
+        <v>0</v>
+      </c>
+      <c r="M77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B78">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="2">
+        <v>0</v>
+      </c>
+      <c r="H78" s="3">
+        <v>0</v>
+      </c>
+      <c r="I78" s="3">
+        <v>0</v>
+      </c>
+      <c r="J78" s="3">
+        <v>0</v>
+      </c>
+      <c r="K78" s="3">
+        <v>0</v>
+      </c>
+      <c r="L78" s="3">
+        <v>0</v>
+      </c>
+      <c r="M78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B79">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="2">
+        <v>112</v>
+      </c>
+      <c r="G79" s="2">
+        <v>0</v>
+      </c>
+      <c r="H79" s="3">
+        <v>0</v>
+      </c>
+      <c r="I79" s="3">
+        <v>0</v>
+      </c>
+      <c r="J79" s="3">
+        <v>0</v>
+      </c>
+      <c r="K79" s="3">
+        <v>0</v>
+      </c>
+      <c r="L79" s="3">
+        <v>0</v>
+      </c>
+      <c r="M79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B80">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="2">
+        <v>20</v>
+      </c>
+      <c r="G80" s="2">
+        <v>0</v>
+      </c>
+      <c r="H80" s="3">
+        <v>0</v>
+      </c>
+      <c r="I80" s="3">
+        <v>0</v>
+      </c>
+      <c r="J80" s="3">
+        <v>0</v>
+      </c>
+      <c r="K80" s="3">
+        <v>0</v>
+      </c>
+      <c r="L80" s="3">
+        <v>0</v>
+      </c>
+      <c r="M80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B81">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="2">
+        <v>31</v>
+      </c>
+      <c r="G81" s="2">
+        <v>0</v>
+      </c>
+      <c r="H81" s="3">
+        <v>0</v>
+      </c>
+      <c r="I81" s="3">
+        <v>0</v>
+      </c>
+      <c r="J81" s="3">
+        <v>0</v>
+      </c>
+      <c r="K81" s="3">
+        <v>0</v>
+      </c>
+      <c r="L81" s="3">
+        <v>0</v>
+      </c>
+      <c r="M81" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated lab survival data
</commit_message>
<xml_diff>
--- a/data/survival/lab_survival/lab_survival.xlsx
+++ b/data/survival/lab_survival/lab_survival.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/survival/lab_survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A219F07-C342-ED4F-81D1-AB9807DA54C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C44FF-6775-9B45-BF1B-02A819BC3721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26980" yWindow="280" windowWidth="25800" windowHeight="17440" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
+    <workbookView xWindow="40520" yWindow="-820" windowWidth="25800" windowHeight="18880" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>18C</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>Effort D</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7ACAA-9959-8D4E-8E48-CFF679AAAAC5}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:N161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,8 +537,8 @@
       <c r="B2">
         <v>38</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -568,8 +578,8 @@
       <c r="B3">
         <v>38</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -609,8 +619,8 @@
       <c r="B4">
         <v>38</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -650,8 +660,8 @@
       <c r="B5">
         <v>38</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -691,8 +701,8 @@
       <c r="B6">
         <v>38</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -732,8 +742,8 @@
       <c r="B7">
         <v>38</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -773,8 +783,8 @@
       <c r="B8">
         <v>38</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -814,8 +824,8 @@
       <c r="B9">
         <v>38</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -855,8 +865,8 @@
       <c r="B10">
         <v>38</v>
       </c>
-      <c r="C10">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -896,8 +906,8 @@
       <c r="B11">
         <v>38</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -937,8 +947,8 @@
       <c r="B12">
         <v>38</v>
       </c>
-      <c r="C12">
-        <v>1</v>
+      <c r="C12" t="s">
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -978,8 +988,8 @@
       <c r="B13">
         <v>38</v>
       </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -1019,8 +1029,8 @@
       <c r="B14">
         <v>38</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -1060,8 +1070,8 @@
       <c r="B15">
         <v>38</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -1101,8 +1111,8 @@
       <c r="B16">
         <v>38</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -1142,8 +1152,8 @@
       <c r="B17">
         <v>38</v>
       </c>
-      <c r="C17">
-        <v>1</v>
+      <c r="C17" t="s">
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -1183,8 +1193,8 @@
       <c r="B18">
         <v>38</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -1224,8 +1234,8 @@
       <c r="B19">
         <v>38</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -1265,8 +1275,8 @@
       <c r="B20">
         <v>38</v>
       </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="C20" t="s">
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -1306,8 +1316,8 @@
       <c r="B21">
         <v>38</v>
       </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="C21" t="s">
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -1347,8 +1357,8 @@
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="C22" t="s">
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1388,8 +1398,8 @@
       <c r="B23">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="C23" t="s">
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1429,8 +1439,8 @@
       <c r="B24">
         <v>21</v>
       </c>
-      <c r="C24">
-        <v>1</v>
+      <c r="C24" t="s">
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
@@ -1470,8 +1480,8 @@
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25">
-        <v>1</v>
+      <c r="C25" t="s">
+        <v>16</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1511,8 +1521,8 @@
       <c r="B26">
         <v>21</v>
       </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>16</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1552,8 +1562,8 @@
       <c r="B27">
         <v>21</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" t="s">
+        <v>16</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1593,8 +1603,8 @@
       <c r="B28">
         <v>21</v>
       </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="C28" t="s">
+        <v>16</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1634,8 +1644,8 @@
       <c r="B29">
         <v>21</v>
       </c>
-      <c r="C29">
-        <v>1</v>
+      <c r="C29" t="s">
+        <v>16</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1675,8 +1685,8 @@
       <c r="B30">
         <v>21</v>
       </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" t="s">
+        <v>16</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1716,8 +1726,8 @@
       <c r="B31">
         <v>21</v>
       </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="C31" t="s">
+        <v>16</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -1757,8 +1767,8 @@
       <c r="B32">
         <v>21</v>
       </c>
-      <c r="C32">
-        <v>1</v>
+      <c r="C32" t="s">
+        <v>16</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1798,8 +1808,8 @@
       <c r="B33">
         <v>21</v>
       </c>
-      <c r="C33">
-        <v>1</v>
+      <c r="C33" t="s">
+        <v>16</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1839,8 +1849,8 @@
       <c r="B34">
         <v>21</v>
       </c>
-      <c r="C34">
-        <v>1</v>
+      <c r="C34" t="s">
+        <v>16</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
@@ -1880,8 +1890,8 @@
       <c r="B35">
         <v>21</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>16</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -1921,8 +1931,8 @@
       <c r="B36">
         <v>21</v>
       </c>
-      <c r="C36">
-        <v>1</v>
+      <c r="C36" t="s">
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -1962,8 +1972,8 @@
       <c r="B37">
         <v>21</v>
       </c>
-      <c r="C37">
-        <v>1</v>
+      <c r="C37" t="s">
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -2003,8 +2013,8 @@
       <c r="B38">
         <v>21</v>
       </c>
-      <c r="C38">
-        <v>1</v>
+      <c r="C38" t="s">
+        <v>16</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -2044,8 +2054,8 @@
       <c r="B39">
         <v>21</v>
       </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="C39" t="s">
+        <v>16</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -2085,8 +2095,8 @@
       <c r="B40">
         <v>21</v>
       </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="C40" t="s">
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -2126,8 +2136,8 @@
       <c r="B41">
         <v>21</v>
       </c>
-      <c r="C41">
-        <v>1</v>
+      <c r="C41" t="s">
+        <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -2167,8 +2177,8 @@
       <c r="B42">
         <v>38</v>
       </c>
-      <c r="C42">
-        <v>1</v>
+      <c r="C42" t="s">
+        <v>16</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
@@ -2208,8 +2218,8 @@
       <c r="B43">
         <v>38</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>16</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -2249,8 +2259,8 @@
       <c r="B44">
         <v>38</v>
       </c>
-      <c r="C44">
-        <v>1</v>
+      <c r="C44" t="s">
+        <v>16</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -2290,8 +2300,8 @@
       <c r="B45">
         <v>38</v>
       </c>
-      <c r="C45">
-        <v>1</v>
+      <c r="C45" t="s">
+        <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
@@ -2331,8 +2341,8 @@
       <c r="B46">
         <v>38</v>
       </c>
-      <c r="C46">
-        <v>1</v>
+      <c r="C46" t="s">
+        <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
@@ -2372,8 +2382,8 @@
       <c r="B47">
         <v>38</v>
       </c>
-      <c r="C47">
-        <v>1</v>
+      <c r="C47" t="s">
+        <v>16</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
@@ -2413,8 +2423,8 @@
       <c r="B48">
         <v>38</v>
       </c>
-      <c r="C48">
-        <v>1</v>
+      <c r="C48" t="s">
+        <v>16</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
@@ -2454,8 +2464,8 @@
       <c r="B49">
         <v>38</v>
       </c>
-      <c r="C49">
-        <v>1</v>
+      <c r="C49" t="s">
+        <v>16</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
@@ -2495,8 +2505,8 @@
       <c r="B50">
         <v>38</v>
       </c>
-      <c r="C50">
-        <v>1</v>
+      <c r="C50" t="s">
+        <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
@@ -2536,8 +2546,8 @@
       <c r="B51">
         <v>38</v>
       </c>
-      <c r="C51">
-        <v>1</v>
+      <c r="C51" t="s">
+        <v>16</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
@@ -2577,8 +2587,8 @@
       <c r="B52">
         <v>38</v>
       </c>
-      <c r="C52">
-        <v>1</v>
+      <c r="C52" t="s">
+        <v>16</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
@@ -2618,8 +2628,8 @@
       <c r="B53">
         <v>38</v>
       </c>
-      <c r="C53">
-        <v>1</v>
+      <c r="C53" t="s">
+        <v>16</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
@@ -2659,8 +2669,8 @@
       <c r="B54">
         <v>38</v>
       </c>
-      <c r="C54">
-        <v>1</v>
+      <c r="C54" t="s">
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
@@ -2700,8 +2710,8 @@
       <c r="B55">
         <v>38</v>
       </c>
-      <c r="C55">
-        <v>1</v>
+      <c r="C55" t="s">
+        <v>16</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
@@ -2741,8 +2751,8 @@
       <c r="B56">
         <v>38</v>
       </c>
-      <c r="C56">
-        <v>1</v>
+      <c r="C56" t="s">
+        <v>16</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
@@ -2782,8 +2792,8 @@
       <c r="B57">
         <v>38</v>
       </c>
-      <c r="C57">
-        <v>1</v>
+      <c r="C57" t="s">
+        <v>16</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
@@ -2823,8 +2833,8 @@
       <c r="B58">
         <v>38</v>
       </c>
-      <c r="C58">
-        <v>1</v>
+      <c r="C58" t="s">
+        <v>16</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
@@ -2864,8 +2874,8 @@
       <c r="B59">
         <v>38</v>
       </c>
-      <c r="C59">
-        <v>1</v>
+      <c r="C59" t="s">
+        <v>16</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -2905,8 +2915,8 @@
       <c r="B60">
         <v>38</v>
       </c>
-      <c r="C60">
-        <v>1</v>
+      <c r="C60" t="s">
+        <v>16</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
@@ -2946,8 +2956,8 @@
       <c r="B61">
         <v>38</v>
       </c>
-      <c r="C61">
-        <v>1</v>
+      <c r="C61" t="s">
+        <v>16</v>
       </c>
       <c r="D61" t="s">
         <v>8</v>
@@ -2987,8 +2997,8 @@
       <c r="B62">
         <v>21</v>
       </c>
-      <c r="C62">
-        <v>1</v>
+      <c r="C62" t="s">
+        <v>16</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -3028,8 +3038,8 @@
       <c r="B63">
         <v>21</v>
       </c>
-      <c r="C63">
-        <v>1</v>
+      <c r="C63" t="s">
+        <v>16</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -3069,8 +3079,8 @@
       <c r="B64">
         <v>21</v>
       </c>
-      <c r="C64">
-        <v>1</v>
+      <c r="C64" t="s">
+        <v>16</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
@@ -3110,8 +3120,8 @@
       <c r="B65">
         <v>21</v>
       </c>
-      <c r="C65">
-        <v>1</v>
+      <c r="C65" t="s">
+        <v>16</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
@@ -3151,8 +3161,8 @@
       <c r="B66">
         <v>21</v>
       </c>
-      <c r="C66">
-        <v>1</v>
+      <c r="C66" t="s">
+        <v>16</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -3192,8 +3202,8 @@
       <c r="B67">
         <v>21</v>
       </c>
-      <c r="C67">
-        <v>1</v>
+      <c r="C67" t="s">
+        <v>16</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
@@ -3233,8 +3243,8 @@
       <c r="B68">
         <v>21</v>
       </c>
-      <c r="C68">
-        <v>1</v>
+      <c r="C68" t="s">
+        <v>16</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
@@ -3274,8 +3284,8 @@
       <c r="B69">
         <v>21</v>
       </c>
-      <c r="C69">
-        <v>1</v>
+      <c r="C69" t="s">
+        <v>16</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -3315,8 +3325,8 @@
       <c r="B70">
         <v>21</v>
       </c>
-      <c r="C70">
-        <v>1</v>
+      <c r="C70" t="s">
+        <v>16</v>
       </c>
       <c r="D70" t="s">
         <v>9</v>
@@ -3356,8 +3366,8 @@
       <c r="B71">
         <v>21</v>
       </c>
-      <c r="C71">
-        <v>1</v>
+      <c r="C71" t="s">
+        <v>16</v>
       </c>
       <c r="D71" t="s">
         <v>9</v>
@@ -3397,8 +3407,8 @@
       <c r="B72">
         <v>21</v>
       </c>
-      <c r="C72">
-        <v>1</v>
+      <c r="C72" t="s">
+        <v>16</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
@@ -3438,8 +3448,8 @@
       <c r="B73">
         <v>21</v>
       </c>
-      <c r="C73">
-        <v>1</v>
+      <c r="C73" t="s">
+        <v>16</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
@@ -3479,8 +3489,8 @@
       <c r="B74">
         <v>21</v>
       </c>
-      <c r="C74">
-        <v>1</v>
+      <c r="C74" t="s">
+        <v>16</v>
       </c>
       <c r="D74" t="s">
         <v>9</v>
@@ -3520,8 +3530,8 @@
       <c r="B75">
         <v>21</v>
       </c>
-      <c r="C75">
-        <v>1</v>
+      <c r="C75" t="s">
+        <v>16</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
@@ -3561,8 +3571,8 @@
       <c r="B76">
         <v>21</v>
       </c>
-      <c r="C76">
-        <v>1</v>
+      <c r="C76" t="s">
+        <v>16</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -3602,8 +3612,8 @@
       <c r="B77">
         <v>21</v>
       </c>
-      <c r="C77">
-        <v>1</v>
+      <c r="C77" t="s">
+        <v>16</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
@@ -3643,8 +3653,8 @@
       <c r="B78">
         <v>21</v>
       </c>
-      <c r="C78">
-        <v>1</v>
+      <c r="C78" t="s">
+        <v>16</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
@@ -3684,8 +3694,8 @@
       <c r="B79">
         <v>21</v>
       </c>
-      <c r="C79">
-        <v>1</v>
+      <c r="C79" t="s">
+        <v>16</v>
       </c>
       <c r="D79" t="s">
         <v>9</v>
@@ -3725,8 +3735,8 @@
       <c r="B80">
         <v>21</v>
       </c>
-      <c r="C80">
-        <v>1</v>
+      <c r="C80" t="s">
+        <v>16</v>
       </c>
       <c r="D80" t="s">
         <v>9</v>
@@ -3759,15 +3769,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>45567</v>
       </c>
       <c r="B81">
         <v>21</v>
       </c>
-      <c r="C81">
-        <v>1</v>
+      <c r="C81" t="s">
+        <v>16</v>
       </c>
       <c r="D81" t="s">
         <v>9</v>
@@ -3798,6 +3808,3287 @@
       </c>
       <c r="M81" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B82">
+        <v>22</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="2">
+        <v>19</v>
+      </c>
+      <c r="G82" s="2">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2">
+        <v>0</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2">
+        <v>0</v>
+      </c>
+      <c r="M82" s="2">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B83">
+        <v>22</v>
+      </c>
+      <c r="C83" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="2">
+        <v>4</v>
+      </c>
+      <c r="G83" s="2">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <v>0</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2">
+        <v>0</v>
+      </c>
+      <c r="K83" s="2">
+        <v>0</v>
+      </c>
+      <c r="L83" s="2">
+        <v>0</v>
+      </c>
+      <c r="M83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B84">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="2">
+        <v>8</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="2">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2">
+        <v>0</v>
+      </c>
+      <c r="K84" s="2">
+        <v>0</v>
+      </c>
+      <c r="L84" s="2">
+        <v>0</v>
+      </c>
+      <c r="M84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B85">
+        <v>22</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="2">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2">
+        <v>0</v>
+      </c>
+      <c r="I85" s="2">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2">
+        <v>0</v>
+      </c>
+      <c r="K85" s="2">
+        <v>0</v>
+      </c>
+      <c r="L85" s="2">
+        <v>0</v>
+      </c>
+      <c r="M85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B86">
+        <v>22</v>
+      </c>
+      <c r="C86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="2">
+        <v>19</v>
+      </c>
+      <c r="G86" s="2">
+        <v>0</v>
+      </c>
+      <c r="H86" s="2">
+        <v>0</v>
+      </c>
+      <c r="I86" s="2">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2">
+        <v>0</v>
+      </c>
+      <c r="K86" s="2">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2">
+        <v>0</v>
+      </c>
+      <c r="M86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B87">
+        <v>22</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="2">
+        <v>8</v>
+      </c>
+      <c r="G87" s="2">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2">
+        <v>0</v>
+      </c>
+      <c r="I87" s="2">
+        <v>0</v>
+      </c>
+      <c r="J87" s="2">
+        <v>0</v>
+      </c>
+      <c r="K87" s="2">
+        <v>0</v>
+      </c>
+      <c r="L87" s="2">
+        <v>0</v>
+      </c>
+      <c r="M87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B88">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" s="2">
+        <v>2</v>
+      </c>
+      <c r="G88" s="2">
+        <v>0</v>
+      </c>
+      <c r="H88" s="2">
+        <v>0</v>
+      </c>
+      <c r="I88" s="2">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2">
+        <v>0</v>
+      </c>
+      <c r="K88" s="2">
+        <v>0</v>
+      </c>
+      <c r="L88" s="2">
+        <v>0</v>
+      </c>
+      <c r="M88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B89">
+        <v>22</v>
+      </c>
+      <c r="C89" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="2">
+        <v>23</v>
+      </c>
+      <c r="G89" s="2">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2">
+        <v>0</v>
+      </c>
+      <c r="I89" s="2">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2">
+        <v>0</v>
+      </c>
+      <c r="K89" s="2">
+        <v>0</v>
+      </c>
+      <c r="L89" s="2">
+        <v>0</v>
+      </c>
+      <c r="M89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B90">
+        <v>22</v>
+      </c>
+      <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s">
+        <v>13</v>
+      </c>
+      <c r="F90" s="2">
+        <v>24</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2">
+        <v>0</v>
+      </c>
+      <c r="I90" s="2">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2">
+        <v>0</v>
+      </c>
+      <c r="K90" s="2">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2">
+        <v>0</v>
+      </c>
+      <c r="M90" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B91">
+        <v>22</v>
+      </c>
+      <c r="C91" t="s">
+        <v>16</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="2">
+        <v>5</v>
+      </c>
+      <c r="G91" s="2">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0</v>
+      </c>
+      <c r="I91" s="2">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2">
+        <v>0</v>
+      </c>
+      <c r="K91" s="2">
+        <v>0</v>
+      </c>
+      <c r="L91" s="2">
+        <v>0</v>
+      </c>
+      <c r="M91" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B92">
+        <v>22</v>
+      </c>
+      <c r="C92" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="2">
+        <v>37</v>
+      </c>
+      <c r="G92" s="2">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2">
+        <v>0</v>
+      </c>
+      <c r="I92" s="2">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2">
+        <v>0</v>
+      </c>
+      <c r="K92" s="2">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2">
+        <v>0</v>
+      </c>
+      <c r="M92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B93">
+        <v>22</v>
+      </c>
+      <c r="C93" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" s="2">
+        <v>40</v>
+      </c>
+      <c r="G93" s="2">
+        <v>0</v>
+      </c>
+      <c r="H93" s="2">
+        <v>0</v>
+      </c>
+      <c r="I93" s="2">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2">
+        <v>0</v>
+      </c>
+      <c r="K93" s="2">
+        <v>0</v>
+      </c>
+      <c r="L93" s="2">
+        <v>0</v>
+      </c>
+      <c r="M93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B94">
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" s="2">
+        <v>2</v>
+      </c>
+      <c r="G94" s="2">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2">
+        <v>0</v>
+      </c>
+      <c r="I94" s="2">
+        <v>0</v>
+      </c>
+      <c r="J94" s="2">
+        <v>0</v>
+      </c>
+      <c r="K94" s="2">
+        <v>0</v>
+      </c>
+      <c r="L94" s="2">
+        <v>0</v>
+      </c>
+      <c r="M94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B95">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="2">
+        <v>38</v>
+      </c>
+      <c r="G95" s="2">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2">
+        <v>0</v>
+      </c>
+      <c r="K95" s="2">
+        <v>0</v>
+      </c>
+      <c r="L95" s="2">
+        <v>0</v>
+      </c>
+      <c r="M95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B96">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="2">
+        <v>20</v>
+      </c>
+      <c r="G96" s="2">
+        <v>0</v>
+      </c>
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+      <c r="I96" s="2">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2">
+        <v>0</v>
+      </c>
+      <c r="K96" s="2">
+        <v>0</v>
+      </c>
+      <c r="L96" s="2">
+        <v>0</v>
+      </c>
+      <c r="M96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B97">
+        <v>22</v>
+      </c>
+      <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="2">
+        <v>24</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>0</v>
+      </c>
+      <c r="K97" s="2">
+        <v>0</v>
+      </c>
+      <c r="L97" s="2">
+        <v>0</v>
+      </c>
+      <c r="M97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B98">
+        <v>22</v>
+      </c>
+      <c r="C98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="2">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2">
+        <v>0</v>
+      </c>
+      <c r="K98" s="2">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2">
+        <v>0</v>
+      </c>
+      <c r="M98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B99">
+        <v>22</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="2">
+        <v>15</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2">
+        <v>0</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2">
+        <v>0</v>
+      </c>
+      <c r="K99" s="2">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2">
+        <v>0</v>
+      </c>
+      <c r="M99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B100">
+        <v>22</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="2">
+        <v>16</v>
+      </c>
+      <c r="G100" s="2">
+        <v>0</v>
+      </c>
+      <c r="H100" s="2">
+        <v>0</v>
+      </c>
+      <c r="I100" s="2">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2">
+        <v>0</v>
+      </c>
+      <c r="K100" s="2">
+        <v>0</v>
+      </c>
+      <c r="L100" s="2">
+        <v>0</v>
+      </c>
+      <c r="M100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B101">
+        <v>22</v>
+      </c>
+      <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="2">
+        <v>33</v>
+      </c>
+      <c r="G101" s="2">
+        <v>0</v>
+      </c>
+      <c r="H101" s="2">
+        <v>0</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0</v>
+      </c>
+      <c r="J101" s="2">
+        <v>0</v>
+      </c>
+      <c r="K101" s="2">
+        <v>0</v>
+      </c>
+      <c r="L101" s="2">
+        <v>0</v>
+      </c>
+      <c r="M101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B102">
+        <v>39</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="2">
+        <v>32</v>
+      </c>
+      <c r="G102" s="2">
+        <v>0</v>
+      </c>
+      <c r="H102" s="2">
+        <v>0</v>
+      </c>
+      <c r="I102" s="2">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2">
+        <v>0</v>
+      </c>
+      <c r="K102" s="2">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2">
+        <v>0</v>
+      </c>
+      <c r="M102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B103">
+        <v>39</v>
+      </c>
+      <c r="C103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" s="2">
+        <v>33</v>
+      </c>
+      <c r="G103" s="2">
+        <v>0</v>
+      </c>
+      <c r="H103" s="2">
+        <v>0</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2">
+        <v>0</v>
+      </c>
+      <c r="K103" s="2">
+        <v>0</v>
+      </c>
+      <c r="L103" s="2">
+        <v>0</v>
+      </c>
+      <c r="M103" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B104">
+        <v>39</v>
+      </c>
+      <c r="C104" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="2">
+        <v>17</v>
+      </c>
+      <c r="G104" s="2">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2">
+        <v>0</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0</v>
+      </c>
+      <c r="K104" s="2">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2">
+        <v>0</v>
+      </c>
+      <c r="M104" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B105">
+        <v>39</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="2">
+        <v>222</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2">
+        <v>0</v>
+      </c>
+      <c r="K105" s="2">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2">
+        <v>0</v>
+      </c>
+      <c r="M105" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B106">
+        <v>39</v>
+      </c>
+      <c r="C106" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="2">
+        <v>29</v>
+      </c>
+      <c r="G106" s="2">
+        <v>0</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2">
+        <v>0</v>
+      </c>
+      <c r="K106" s="2">
+        <v>0</v>
+      </c>
+      <c r="L106" s="2">
+        <v>0</v>
+      </c>
+      <c r="M106" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B107">
+        <v>39</v>
+      </c>
+      <c r="C107" t="s">
+        <v>16</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="2">
+        <v>152</v>
+      </c>
+      <c r="G107" s="2">
+        <v>0</v>
+      </c>
+      <c r="H107" s="2">
+        <v>0</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0</v>
+      </c>
+      <c r="J107" s="2">
+        <v>0</v>
+      </c>
+      <c r="K107" s="2">
+        <v>0</v>
+      </c>
+      <c r="L107" s="2">
+        <v>0</v>
+      </c>
+      <c r="M107" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B108">
+        <v>39</v>
+      </c>
+      <c r="C108" t="s">
+        <v>16</v>
+      </c>
+      <c r="D108" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="2">
+        <v>112</v>
+      </c>
+      <c r="G108" s="2">
+        <v>0</v>
+      </c>
+      <c r="H108" s="2">
+        <v>0</v>
+      </c>
+      <c r="I108" s="2">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2">
+        <v>0</v>
+      </c>
+      <c r="K108" s="2">
+        <v>0</v>
+      </c>
+      <c r="L108" s="2">
+        <v>0</v>
+      </c>
+      <c r="M108" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B109">
+        <v>39</v>
+      </c>
+      <c r="C109" t="s">
+        <v>16</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" s="2">
+        <v>38</v>
+      </c>
+      <c r="G109" s="2">
+        <v>0</v>
+      </c>
+      <c r="H109" s="2">
+        <v>0</v>
+      </c>
+      <c r="I109" s="2">
+        <v>0</v>
+      </c>
+      <c r="J109" s="2">
+        <v>0</v>
+      </c>
+      <c r="K109" s="2">
+        <v>0</v>
+      </c>
+      <c r="L109" s="2">
+        <v>0</v>
+      </c>
+      <c r="M109" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B110">
+        <v>39</v>
+      </c>
+      <c r="C110" t="s">
+        <v>16</v>
+      </c>
+      <c r="D110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" s="2">
+        <v>18</v>
+      </c>
+      <c r="G110" s="2">
+        <v>0</v>
+      </c>
+      <c r="H110" s="2">
+        <v>0</v>
+      </c>
+      <c r="I110" s="2">
+        <v>0</v>
+      </c>
+      <c r="J110" s="2">
+        <v>0</v>
+      </c>
+      <c r="K110" s="2">
+        <v>0</v>
+      </c>
+      <c r="L110" s="2">
+        <v>0</v>
+      </c>
+      <c r="M110" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B111">
+        <v>39</v>
+      </c>
+      <c r="C111" t="s">
+        <v>16</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" s="2">
+        <v>26</v>
+      </c>
+      <c r="G111" s="2">
+        <v>0</v>
+      </c>
+      <c r="H111" s="2">
+        <v>0</v>
+      </c>
+      <c r="I111" s="2">
+        <v>0</v>
+      </c>
+      <c r="J111" s="2">
+        <v>0</v>
+      </c>
+      <c r="K111" s="2">
+        <v>0</v>
+      </c>
+      <c r="L111" s="2">
+        <v>0</v>
+      </c>
+      <c r="M111" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B112">
+        <v>39</v>
+      </c>
+      <c r="C112" t="s">
+        <v>16</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" t="s">
+        <v>13</v>
+      </c>
+      <c r="F112" s="2">
+        <v>19</v>
+      </c>
+      <c r="G112" s="2">
+        <v>0</v>
+      </c>
+      <c r="H112" s="2">
+        <v>0</v>
+      </c>
+      <c r="I112" s="2">
+        <v>0</v>
+      </c>
+      <c r="J112" s="2">
+        <v>0</v>
+      </c>
+      <c r="K112" s="2">
+        <v>0</v>
+      </c>
+      <c r="L112" s="2">
+        <v>0</v>
+      </c>
+      <c r="M112" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B113">
+        <v>39</v>
+      </c>
+      <c r="C113" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+      <c r="F113" s="2">
+        <v>2</v>
+      </c>
+      <c r="G113" s="2">
+        <v>0</v>
+      </c>
+      <c r="H113" s="2">
+        <v>0</v>
+      </c>
+      <c r="I113" s="2">
+        <v>0</v>
+      </c>
+      <c r="J113" s="2">
+        <v>0</v>
+      </c>
+      <c r="K113" s="2">
+        <v>0</v>
+      </c>
+      <c r="L113" s="2">
+        <v>0</v>
+      </c>
+      <c r="M113" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B114">
+        <v>39</v>
+      </c>
+      <c r="C114" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" s="2">
+        <v>36</v>
+      </c>
+      <c r="G114" s="2">
+        <v>0</v>
+      </c>
+      <c r="H114" s="2">
+        <v>0</v>
+      </c>
+      <c r="I114" s="2">
+        <v>0</v>
+      </c>
+      <c r="J114" s="2">
+        <v>0</v>
+      </c>
+      <c r="K114" s="2">
+        <v>0</v>
+      </c>
+      <c r="L114" s="2">
+        <v>0</v>
+      </c>
+      <c r="M114" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B115">
+        <v>39</v>
+      </c>
+      <c r="C115" t="s">
+        <v>16</v>
+      </c>
+      <c r="D115" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" t="s">
+        <v>13</v>
+      </c>
+      <c r="F115" s="2">
+        <v>33</v>
+      </c>
+      <c r="G115" s="2">
+        <v>0</v>
+      </c>
+      <c r="H115" s="2">
+        <v>0</v>
+      </c>
+      <c r="I115" s="2">
+        <v>0</v>
+      </c>
+      <c r="J115" s="2">
+        <v>0</v>
+      </c>
+      <c r="K115" s="2">
+        <v>0</v>
+      </c>
+      <c r="L115" s="2">
+        <v>0</v>
+      </c>
+      <c r="M115" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B116">
+        <v>39</v>
+      </c>
+      <c r="C116" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" t="s">
+        <v>13</v>
+      </c>
+      <c r="F116" s="2">
+        <v>10</v>
+      </c>
+      <c r="G116" s="2">
+        <v>0</v>
+      </c>
+      <c r="H116" s="2">
+        <v>0</v>
+      </c>
+      <c r="I116" s="2">
+        <v>0</v>
+      </c>
+      <c r="J116" s="2">
+        <v>0</v>
+      </c>
+      <c r="K116" s="2">
+        <v>0</v>
+      </c>
+      <c r="L116" s="2">
+        <v>0</v>
+      </c>
+      <c r="M116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B117">
+        <v>39</v>
+      </c>
+      <c r="C117" t="s">
+        <v>16</v>
+      </c>
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" t="s">
+        <v>13</v>
+      </c>
+      <c r="F117" s="2">
+        <v>34</v>
+      </c>
+      <c r="G117" s="2">
+        <v>0</v>
+      </c>
+      <c r="H117" s="2">
+        <v>0</v>
+      </c>
+      <c r="I117" s="2">
+        <v>0</v>
+      </c>
+      <c r="J117" s="2">
+        <v>0</v>
+      </c>
+      <c r="K117" s="2">
+        <v>0</v>
+      </c>
+      <c r="L117" s="2">
+        <v>0</v>
+      </c>
+      <c r="M117" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B118">
+        <v>39</v>
+      </c>
+      <c r="C118" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" t="s">
+        <v>13</v>
+      </c>
+      <c r="F118" s="2">
+        <v>3</v>
+      </c>
+      <c r="G118" s="2">
+        <v>0</v>
+      </c>
+      <c r="H118" s="2">
+        <v>0</v>
+      </c>
+      <c r="I118" s="2">
+        <v>0</v>
+      </c>
+      <c r="J118" s="2">
+        <v>0</v>
+      </c>
+      <c r="K118" s="2">
+        <v>0</v>
+      </c>
+      <c r="L118" s="2">
+        <v>0</v>
+      </c>
+      <c r="M118" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B119">
+        <v>39</v>
+      </c>
+      <c r="C119" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" t="s">
+        <v>13</v>
+      </c>
+      <c r="F119" s="2">
+        <v>31</v>
+      </c>
+      <c r="G119" s="2">
+        <v>0</v>
+      </c>
+      <c r="H119" s="2">
+        <v>0</v>
+      </c>
+      <c r="I119" s="2">
+        <v>0</v>
+      </c>
+      <c r="J119" s="2">
+        <v>0</v>
+      </c>
+      <c r="K119" s="2">
+        <v>0</v>
+      </c>
+      <c r="L119" s="2">
+        <v>0</v>
+      </c>
+      <c r="M119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B120">
+        <v>39</v>
+      </c>
+      <c r="C120" t="s">
+        <v>16</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s">
+        <v>13</v>
+      </c>
+      <c r="F120" s="2">
+        <v>40</v>
+      </c>
+      <c r="G120" s="2">
+        <v>0</v>
+      </c>
+      <c r="H120" s="2">
+        <v>0</v>
+      </c>
+      <c r="I120" s="2">
+        <v>0</v>
+      </c>
+      <c r="J120" s="2">
+        <v>0</v>
+      </c>
+      <c r="K120" s="2">
+        <v>0</v>
+      </c>
+      <c r="L120" s="2">
+        <v>0</v>
+      </c>
+      <c r="M120" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B121">
+        <v>39</v>
+      </c>
+      <c r="C121" t="s">
+        <v>16</v>
+      </c>
+      <c r="D121" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" t="s">
+        <v>13</v>
+      </c>
+      <c r="F121" s="2">
+        <v>21</v>
+      </c>
+      <c r="G121" s="2">
+        <v>0</v>
+      </c>
+      <c r="H121" s="2">
+        <v>0</v>
+      </c>
+      <c r="I121" s="2">
+        <v>0</v>
+      </c>
+      <c r="J121" s="2">
+        <v>0</v>
+      </c>
+      <c r="K121" s="2">
+        <v>0</v>
+      </c>
+      <c r="L121" s="2">
+        <v>0</v>
+      </c>
+      <c r="M121" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B122">
+        <v>22</v>
+      </c>
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0</v>
+      </c>
+      <c r="H122" s="3">
+        <v>0</v>
+      </c>
+      <c r="I122" s="3">
+        <v>0</v>
+      </c>
+      <c r="J122" s="4">
+        <v>1</v>
+      </c>
+      <c r="K122" s="4">
+        <v>1</v>
+      </c>
+      <c r="L122" s="4">
+        <v>1</v>
+      </c>
+      <c r="M122" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B123">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>16</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" t="s">
+        <v>12</v>
+      </c>
+      <c r="F123" s="2">
+        <v>19</v>
+      </c>
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
+      <c r="H123" s="3">
+        <v>0</v>
+      </c>
+      <c r="I123" s="3">
+        <v>0</v>
+      </c>
+      <c r="J123" s="3">
+        <v>0</v>
+      </c>
+      <c r="K123" s="3">
+        <v>0</v>
+      </c>
+      <c r="L123" s="3">
+        <v>0</v>
+      </c>
+      <c r="M123" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B124">
+        <v>22</v>
+      </c>
+      <c r="C124" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="2">
+        <v>3</v>
+      </c>
+      <c r="G124" s="2">
+        <v>0</v>
+      </c>
+      <c r="H124" s="3">
+        <v>0</v>
+      </c>
+      <c r="I124" s="3">
+        <v>0</v>
+      </c>
+      <c r="J124" s="3">
+        <v>0</v>
+      </c>
+      <c r="K124" s="3">
+        <v>0</v>
+      </c>
+      <c r="L124" s="4">
+        <v>1</v>
+      </c>
+      <c r="M124" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B125">
+        <v>22</v>
+      </c>
+      <c r="C125" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" t="s">
+        <v>12</v>
+      </c>
+      <c r="F125" s="2">
+        <v>35</v>
+      </c>
+      <c r="G125" s="2">
+        <v>0</v>
+      </c>
+      <c r="H125" s="3">
+        <v>0</v>
+      </c>
+      <c r="I125" s="3">
+        <v>0</v>
+      </c>
+      <c r="J125" s="3">
+        <v>0</v>
+      </c>
+      <c r="K125" s="4">
+        <v>1</v>
+      </c>
+      <c r="L125" s="4">
+        <v>1</v>
+      </c>
+      <c r="M125" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B126">
+        <v>22</v>
+      </c>
+      <c r="C126" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
+        <v>12</v>
+      </c>
+      <c r="F126" s="2">
+        <v>27</v>
+      </c>
+      <c r="G126" s="2">
+        <v>0</v>
+      </c>
+      <c r="H126" s="3">
+        <v>0</v>
+      </c>
+      <c r="I126" s="3">
+        <v>0</v>
+      </c>
+      <c r="J126" s="3">
+        <v>0</v>
+      </c>
+      <c r="K126" s="4">
+        <v>1</v>
+      </c>
+      <c r="L126" s="4">
+        <v>1</v>
+      </c>
+      <c r="M126" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B127">
+        <v>22</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" t="s">
+        <v>12</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G127" s="2">
+        <v>0</v>
+      </c>
+      <c r="H127" s="3">
+        <v>0</v>
+      </c>
+      <c r="I127" s="3">
+        <v>0</v>
+      </c>
+      <c r="J127" s="3">
+        <v>0</v>
+      </c>
+      <c r="K127" s="4">
+        <v>1</v>
+      </c>
+      <c r="L127" s="4">
+        <v>1</v>
+      </c>
+      <c r="M127" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B128">
+        <v>22</v>
+      </c>
+      <c r="C128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" t="s">
+        <v>12</v>
+      </c>
+      <c r="F128" s="2">
+        <v>1</v>
+      </c>
+      <c r="G128" s="2">
+        <v>0</v>
+      </c>
+      <c r="H128" s="3">
+        <v>0</v>
+      </c>
+      <c r="I128" s="3">
+        <v>0</v>
+      </c>
+      <c r="J128" s="3">
+        <v>0</v>
+      </c>
+      <c r="K128" s="3">
+        <v>0</v>
+      </c>
+      <c r="L128" s="3">
+        <v>0</v>
+      </c>
+      <c r="M128" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B129">
+        <v>22</v>
+      </c>
+      <c r="C129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" t="s">
+        <v>12</v>
+      </c>
+      <c r="F129" s="2">
+        <v>8</v>
+      </c>
+      <c r="G129" s="2">
+        <v>0</v>
+      </c>
+      <c r="H129" s="3">
+        <v>0</v>
+      </c>
+      <c r="I129" s="3">
+        <v>0</v>
+      </c>
+      <c r="J129" s="4">
+        <v>1</v>
+      </c>
+      <c r="K129" s="4">
+        <v>1</v>
+      </c>
+      <c r="L129" s="4">
+        <v>1</v>
+      </c>
+      <c r="M129" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B130">
+        <v>22</v>
+      </c>
+      <c r="C130" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" t="s">
+        <v>12</v>
+      </c>
+      <c r="F130" s="2">
+        <v>10</v>
+      </c>
+      <c r="G130" s="2">
+        <v>0</v>
+      </c>
+      <c r="H130" s="3">
+        <v>0</v>
+      </c>
+      <c r="I130" s="3">
+        <v>0</v>
+      </c>
+      <c r="J130" s="3">
+        <v>0</v>
+      </c>
+      <c r="K130" s="4">
+        <v>1</v>
+      </c>
+      <c r="L130" s="4">
+        <v>1</v>
+      </c>
+      <c r="M130" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B131">
+        <v>22</v>
+      </c>
+      <c r="C131" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" t="s">
+        <v>12</v>
+      </c>
+      <c r="F131" s="2">
+        <v>13</v>
+      </c>
+      <c r="G131" s="2">
+        <v>0</v>
+      </c>
+      <c r="H131" s="3">
+        <v>0</v>
+      </c>
+      <c r="I131" s="3">
+        <v>0</v>
+      </c>
+      <c r="J131" s="4">
+        <v>1</v>
+      </c>
+      <c r="K131" s="4">
+        <v>1</v>
+      </c>
+      <c r="L131" s="4">
+        <v>1</v>
+      </c>
+      <c r="M131" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B132">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>16</v>
+      </c>
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" t="s">
+        <v>12</v>
+      </c>
+      <c r="F132" s="2">
+        <v>4</v>
+      </c>
+      <c r="G132" s="2">
+        <v>0</v>
+      </c>
+      <c r="H132" s="3">
+        <v>0</v>
+      </c>
+      <c r="I132" s="3">
+        <v>0</v>
+      </c>
+      <c r="J132" s="3">
+        <v>0</v>
+      </c>
+      <c r="K132" s="3">
+        <v>0</v>
+      </c>
+      <c r="L132" s="3">
+        <v>0</v>
+      </c>
+      <c r="M132" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B133">
+        <v>22</v>
+      </c>
+      <c r="C133" t="s">
+        <v>16</v>
+      </c>
+      <c r="D133" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" t="s">
+        <v>12</v>
+      </c>
+      <c r="F133" s="2">
+        <v>32</v>
+      </c>
+      <c r="G133" s="2">
+        <v>0</v>
+      </c>
+      <c r="H133" s="3">
+        <v>0</v>
+      </c>
+      <c r="I133" s="3">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3">
+        <v>0</v>
+      </c>
+      <c r="K133" s="4">
+        <v>1</v>
+      </c>
+      <c r="L133" s="4">
+        <v>1</v>
+      </c>
+      <c r="M133" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B134">
+        <v>22</v>
+      </c>
+      <c r="C134" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" t="s">
+        <v>12</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G134" s="2">
+        <v>0</v>
+      </c>
+      <c r="H134" s="3">
+        <v>0</v>
+      </c>
+      <c r="I134" s="3">
+        <v>0</v>
+      </c>
+      <c r="J134" s="3">
+        <v>0</v>
+      </c>
+      <c r="K134" s="4">
+        <v>1</v>
+      </c>
+      <c r="L134" s="4">
+        <v>1</v>
+      </c>
+      <c r="M134" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B135">
+        <v>22</v>
+      </c>
+      <c r="C135" t="s">
+        <v>16</v>
+      </c>
+      <c r="D135" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" t="s">
+        <v>12</v>
+      </c>
+      <c r="F135" s="2">
+        <v>12</v>
+      </c>
+      <c r="G135" s="2">
+        <v>0</v>
+      </c>
+      <c r="H135" s="3">
+        <v>0</v>
+      </c>
+      <c r="I135" s="4">
+        <v>1</v>
+      </c>
+      <c r="J135" s="4">
+        <v>1</v>
+      </c>
+      <c r="K135" s="4">
+        <v>1</v>
+      </c>
+      <c r="L135" s="4">
+        <v>1</v>
+      </c>
+      <c r="M135" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B136">
+        <v>22</v>
+      </c>
+      <c r="C136" t="s">
+        <v>16</v>
+      </c>
+      <c r="D136" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" t="s">
+        <v>12</v>
+      </c>
+      <c r="F136" s="2">
+        <v>16</v>
+      </c>
+      <c r="G136" s="2">
+        <v>0</v>
+      </c>
+      <c r="H136" s="3">
+        <v>0</v>
+      </c>
+      <c r="I136" s="4">
+        <v>1</v>
+      </c>
+      <c r="J136" s="4">
+        <v>1</v>
+      </c>
+      <c r="K136" s="4">
+        <v>1</v>
+      </c>
+      <c r="L136" s="4">
+        <v>1</v>
+      </c>
+      <c r="M136" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B137">
+        <v>22</v>
+      </c>
+      <c r="C137" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" t="s">
+        <v>12</v>
+      </c>
+      <c r="F137" s="2">
+        <v>18</v>
+      </c>
+      <c r="G137" s="2">
+        <v>0</v>
+      </c>
+      <c r="H137" s="3">
+        <v>0</v>
+      </c>
+      <c r="I137" s="3">
+        <v>0</v>
+      </c>
+      <c r="J137" s="3">
+        <v>0</v>
+      </c>
+      <c r="K137" s="3">
+        <v>0</v>
+      </c>
+      <c r="L137" s="3">
+        <v>0</v>
+      </c>
+      <c r="M137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B138">
+        <v>22</v>
+      </c>
+      <c r="C138" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" t="s">
+        <v>12</v>
+      </c>
+      <c r="F138" s="2">
+        <v>38</v>
+      </c>
+      <c r="G138" s="2">
+        <v>0</v>
+      </c>
+      <c r="H138" s="3">
+        <v>0</v>
+      </c>
+      <c r="I138" s="3">
+        <v>0</v>
+      </c>
+      <c r="J138" s="3">
+        <v>0</v>
+      </c>
+      <c r="K138" s="4">
+        <v>1</v>
+      </c>
+      <c r="L138" s="4">
+        <v>1</v>
+      </c>
+      <c r="M138" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B139">
+        <v>22</v>
+      </c>
+      <c r="C139" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" t="s">
+        <v>12</v>
+      </c>
+      <c r="F139" s="2">
+        <v>26</v>
+      </c>
+      <c r="G139" s="2">
+        <v>0</v>
+      </c>
+      <c r="H139" s="3">
+        <v>0</v>
+      </c>
+      <c r="I139" s="3">
+        <v>0</v>
+      </c>
+      <c r="J139" s="3">
+        <v>0</v>
+      </c>
+      <c r="K139" s="3">
+        <v>0</v>
+      </c>
+      <c r="L139" s="4">
+        <v>1</v>
+      </c>
+      <c r="M139" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B140">
+        <v>22</v>
+      </c>
+      <c r="C140" t="s">
+        <v>16</v>
+      </c>
+      <c r="D140" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" t="s">
+        <v>12</v>
+      </c>
+      <c r="F140" s="2">
+        <v>5</v>
+      </c>
+      <c r="G140" s="2">
+        <v>0</v>
+      </c>
+      <c r="H140" s="3">
+        <v>0</v>
+      </c>
+      <c r="I140" s="3">
+        <v>0</v>
+      </c>
+      <c r="J140" s="3">
+        <v>0</v>
+      </c>
+      <c r="K140" s="4">
+        <v>1</v>
+      </c>
+      <c r="L140" s="4">
+        <v>1</v>
+      </c>
+      <c r="M140" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B141">
+        <v>22</v>
+      </c>
+      <c r="C141" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141" t="s">
+        <v>9</v>
+      </c>
+      <c r="E141" t="s">
+        <v>12</v>
+      </c>
+      <c r="F141" s="2">
+        <v>40</v>
+      </c>
+      <c r="G141" s="2">
+        <v>0</v>
+      </c>
+      <c r="H141" s="3">
+        <v>0</v>
+      </c>
+      <c r="I141" s="3">
+        <v>0</v>
+      </c>
+      <c r="J141" s="4">
+        <v>1</v>
+      </c>
+      <c r="K141" s="4">
+        <v>1</v>
+      </c>
+      <c r="L141" s="4">
+        <v>1</v>
+      </c>
+      <c r="M141" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B142">
+        <v>39</v>
+      </c>
+      <c r="C142" t="s">
+        <v>16</v>
+      </c>
+      <c r="D142" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" t="s">
+        <v>12</v>
+      </c>
+      <c r="F142" s="2">
+        <v>3</v>
+      </c>
+      <c r="G142" s="2">
+        <v>0</v>
+      </c>
+      <c r="H142" s="3">
+        <v>0</v>
+      </c>
+      <c r="I142" s="3">
+        <v>0</v>
+      </c>
+      <c r="J142" s="3">
+        <v>0</v>
+      </c>
+      <c r="K142" s="3">
+        <v>0</v>
+      </c>
+      <c r="L142" s="4">
+        <v>1</v>
+      </c>
+      <c r="M142" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B143">
+        <v>39</v>
+      </c>
+      <c r="C143" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" t="s">
+        <v>12</v>
+      </c>
+      <c r="F143" s="2">
+        <v>6</v>
+      </c>
+      <c r="G143" s="2">
+        <v>0</v>
+      </c>
+      <c r="H143" s="3">
+        <v>0</v>
+      </c>
+      <c r="I143" s="3">
+        <v>0</v>
+      </c>
+      <c r="J143" s="3">
+        <v>0</v>
+      </c>
+      <c r="K143" s="3">
+        <v>0</v>
+      </c>
+      <c r="L143" s="3">
+        <v>0</v>
+      </c>
+      <c r="M143" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B144">
+        <v>39</v>
+      </c>
+      <c r="C144" t="s">
+        <v>16</v>
+      </c>
+      <c r="D144" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" t="s">
+        <v>12</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G144" s="2">
+        <v>0</v>
+      </c>
+      <c r="H144" s="3">
+        <v>0</v>
+      </c>
+      <c r="I144" s="3">
+        <v>0</v>
+      </c>
+      <c r="J144" s="3">
+        <v>0</v>
+      </c>
+      <c r="K144" s="4">
+        <v>1</v>
+      </c>
+      <c r="L144" s="3">
+        <v>0</v>
+      </c>
+      <c r="M144" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B145">
+        <v>39</v>
+      </c>
+      <c r="C145" t="s">
+        <v>16</v>
+      </c>
+      <c r="D145" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" t="s">
+        <v>12</v>
+      </c>
+      <c r="F145" s="2">
+        <v>22</v>
+      </c>
+      <c r="G145" s="2">
+        <v>0</v>
+      </c>
+      <c r="H145" s="3">
+        <v>0</v>
+      </c>
+      <c r="I145" s="4">
+        <v>1</v>
+      </c>
+      <c r="J145" s="4">
+        <v>1</v>
+      </c>
+      <c r="K145" s="4">
+        <v>1</v>
+      </c>
+      <c r="L145" s="4">
+        <v>1</v>
+      </c>
+      <c r="M145" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B146">
+        <v>39</v>
+      </c>
+      <c r="C146" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" t="s">
+        <v>12</v>
+      </c>
+      <c r="F146" s="2">
+        <v>1</v>
+      </c>
+      <c r="G146" s="2">
+        <v>0</v>
+      </c>
+      <c r="H146" s="3">
+        <v>0</v>
+      </c>
+      <c r="I146" s="3">
+        <v>0</v>
+      </c>
+      <c r="J146" s="3">
+        <v>0</v>
+      </c>
+      <c r="K146" s="4">
+        <v>1</v>
+      </c>
+      <c r="L146" s="3">
+        <v>0</v>
+      </c>
+      <c r="M146" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B147">
+        <v>39</v>
+      </c>
+      <c r="C147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D147" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" t="s">
+        <v>12</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G147" s="2">
+        <v>0</v>
+      </c>
+      <c r="H147" s="3">
+        <v>0</v>
+      </c>
+      <c r="I147" s="3">
+        <v>0</v>
+      </c>
+      <c r="J147" s="3">
+        <v>0</v>
+      </c>
+      <c r="K147" s="3">
+        <v>0</v>
+      </c>
+      <c r="L147" s="4">
+        <v>1</v>
+      </c>
+      <c r="M147" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B148">
+        <v>39</v>
+      </c>
+      <c r="C148" t="s">
+        <v>16</v>
+      </c>
+      <c r="D148" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" t="s">
+        <v>12</v>
+      </c>
+      <c r="F148" s="2">
+        <v>16</v>
+      </c>
+      <c r="G148" s="2">
+        <v>0</v>
+      </c>
+      <c r="H148" s="3">
+        <v>0</v>
+      </c>
+      <c r="I148" s="3">
+        <v>0</v>
+      </c>
+      <c r="J148" s="3">
+        <v>0</v>
+      </c>
+      <c r="K148" s="4">
+        <v>1</v>
+      </c>
+      <c r="L148" s="3">
+        <v>0</v>
+      </c>
+      <c r="M148" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B149">
+        <v>39</v>
+      </c>
+      <c r="C149" t="s">
+        <v>16</v>
+      </c>
+      <c r="D149" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" t="s">
+        <v>12</v>
+      </c>
+      <c r="F149" s="2">
+        <v>35</v>
+      </c>
+      <c r="G149" s="2">
+        <v>0</v>
+      </c>
+      <c r="H149" s="3">
+        <v>0</v>
+      </c>
+      <c r="I149" s="3">
+        <v>0</v>
+      </c>
+      <c r="J149" s="4">
+        <v>1</v>
+      </c>
+      <c r="K149" s="4">
+        <v>1</v>
+      </c>
+      <c r="L149" s="4">
+        <v>1</v>
+      </c>
+      <c r="M149" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B150">
+        <v>39</v>
+      </c>
+      <c r="C150" t="s">
+        <v>16</v>
+      </c>
+      <c r="D150" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" t="s">
+        <v>12</v>
+      </c>
+      <c r="F150" s="2">
+        <v>14</v>
+      </c>
+      <c r="G150" s="2">
+        <v>0</v>
+      </c>
+      <c r="H150" s="3">
+        <v>0</v>
+      </c>
+      <c r="I150" s="3">
+        <v>0</v>
+      </c>
+      <c r="J150" s="3">
+        <v>0</v>
+      </c>
+      <c r="K150" s="4">
+        <v>1</v>
+      </c>
+      <c r="L150" s="3">
+        <v>0</v>
+      </c>
+      <c r="M150" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B151">
+        <v>39</v>
+      </c>
+      <c r="C151" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" t="s">
+        <v>12</v>
+      </c>
+      <c r="F151" s="2">
+        <v>25</v>
+      </c>
+      <c r="G151" s="2">
+        <v>0</v>
+      </c>
+      <c r="H151" s="4">
+        <v>1</v>
+      </c>
+      <c r="I151" s="4">
+        <v>1</v>
+      </c>
+      <c r="J151" s="4">
+        <v>1</v>
+      </c>
+      <c r="K151" s="4">
+        <v>1</v>
+      </c>
+      <c r="L151" s="4">
+        <v>1</v>
+      </c>
+      <c r="M151" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B152">
+        <v>39</v>
+      </c>
+      <c r="C152" t="s">
+        <v>16</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" t="s">
+        <v>12</v>
+      </c>
+      <c r="F152" s="2">
+        <v>6</v>
+      </c>
+      <c r="G152" s="2">
+        <v>0</v>
+      </c>
+      <c r="H152" s="3">
+        <v>0</v>
+      </c>
+      <c r="I152" s="3">
+        <v>0</v>
+      </c>
+      <c r="J152" s="3">
+        <v>0</v>
+      </c>
+      <c r="K152" s="3">
+        <v>0</v>
+      </c>
+      <c r="L152" s="3">
+        <v>0</v>
+      </c>
+      <c r="M152" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B153">
+        <v>39</v>
+      </c>
+      <c r="C153" t="s">
+        <v>16</v>
+      </c>
+      <c r="D153" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" t="s">
+        <v>12</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G153" s="2">
+        <v>0</v>
+      </c>
+      <c r="H153" s="3">
+        <v>0</v>
+      </c>
+      <c r="I153" s="3">
+        <v>0</v>
+      </c>
+      <c r="J153" s="3">
+        <v>0</v>
+      </c>
+      <c r="K153" s="4">
+        <v>1</v>
+      </c>
+      <c r="L153" s="3">
+        <v>0</v>
+      </c>
+      <c r="M153" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B154">
+        <v>39</v>
+      </c>
+      <c r="C154" t="s">
+        <v>16</v>
+      </c>
+      <c r="D154" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" t="s">
+        <v>12</v>
+      </c>
+      <c r="F154" s="2">
+        <v>14</v>
+      </c>
+      <c r="G154" s="2">
+        <v>0</v>
+      </c>
+      <c r="H154" s="3">
+        <v>0</v>
+      </c>
+      <c r="I154" s="3">
+        <v>0</v>
+      </c>
+      <c r="J154" s="3">
+        <v>0</v>
+      </c>
+      <c r="K154" s="4">
+        <v>1</v>
+      </c>
+      <c r="L154" s="3">
+        <v>0</v>
+      </c>
+      <c r="M154" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B155">
+        <v>39</v>
+      </c>
+      <c r="C155" t="s">
+        <v>16</v>
+      </c>
+      <c r="D155" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" t="s">
+        <v>12</v>
+      </c>
+      <c r="F155" s="2">
+        <v>17</v>
+      </c>
+      <c r="G155" s="2">
+        <v>0</v>
+      </c>
+      <c r="H155" s="3">
+        <v>0</v>
+      </c>
+      <c r="I155" s="3">
+        <v>0</v>
+      </c>
+      <c r="J155" s="3">
+        <v>0</v>
+      </c>
+      <c r="K155" s="4">
+        <v>1</v>
+      </c>
+      <c r="L155" s="3">
+        <v>0</v>
+      </c>
+      <c r="M155" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B156">
+        <v>39</v>
+      </c>
+      <c r="C156" t="s">
+        <v>16</v>
+      </c>
+      <c r="D156" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" s="2">
+        <v>20</v>
+      </c>
+      <c r="G156" s="2">
+        <v>0</v>
+      </c>
+      <c r="H156" s="3">
+        <v>0</v>
+      </c>
+      <c r="I156" s="3">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3">
+        <v>0</v>
+      </c>
+      <c r="K156" s="4">
+        <v>1</v>
+      </c>
+      <c r="L156" s="3">
+        <v>0</v>
+      </c>
+      <c r="M156" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B157">
+        <v>39</v>
+      </c>
+      <c r="C157" t="s">
+        <v>16</v>
+      </c>
+      <c r="D157" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+      <c r="F157" s="2">
+        <v>13</v>
+      </c>
+      <c r="G157" s="2">
+        <v>0</v>
+      </c>
+      <c r="H157" s="3">
+        <v>0</v>
+      </c>
+      <c r="I157" s="3">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3">
+        <v>0</v>
+      </c>
+      <c r="K157" s="3">
+        <v>0</v>
+      </c>
+      <c r="L157" s="3">
+        <v>0</v>
+      </c>
+      <c r="M157" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B158">
+        <v>39</v>
+      </c>
+      <c r="C158" t="s">
+        <v>16</v>
+      </c>
+      <c r="D158" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" t="s">
+        <v>12</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G158" s="2">
+        <v>0</v>
+      </c>
+      <c r="H158" s="3">
+        <v>0</v>
+      </c>
+      <c r="I158" s="3">
+        <v>0</v>
+      </c>
+      <c r="J158" s="4">
+        <v>1</v>
+      </c>
+      <c r="K158" s="4">
+        <v>1</v>
+      </c>
+      <c r="L158" s="4">
+        <v>1</v>
+      </c>
+      <c r="M158" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B159">
+        <v>39</v>
+      </c>
+      <c r="C159" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" t="s">
+        <v>12</v>
+      </c>
+      <c r="F159" s="2">
+        <v>18</v>
+      </c>
+      <c r="G159" s="2">
+        <v>0</v>
+      </c>
+      <c r="H159" s="3">
+        <v>0</v>
+      </c>
+      <c r="I159" s="4">
+        <v>1</v>
+      </c>
+      <c r="J159" s="4">
+        <v>1</v>
+      </c>
+      <c r="K159" s="4">
+        <v>1</v>
+      </c>
+      <c r="L159" s="4">
+        <v>1</v>
+      </c>
+      <c r="M159" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B160">
+        <v>39</v>
+      </c>
+      <c r="C160" t="s">
+        <v>16</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" t="s">
+        <v>12</v>
+      </c>
+      <c r="F160" s="2">
+        <v>12</v>
+      </c>
+      <c r="G160" s="2">
+        <v>0</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0</v>
+      </c>
+      <c r="I160" s="3">
+        <v>0</v>
+      </c>
+      <c r="J160" s="3">
+        <v>0</v>
+      </c>
+      <c r="K160" s="3">
+        <v>0</v>
+      </c>
+      <c r="L160" s="3">
+        <v>0</v>
+      </c>
+      <c r="M160" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B161">
+        <v>39</v>
+      </c>
+      <c r="C161" t="s">
+        <v>16</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
+      </c>
+      <c r="F161" s="2">
+        <v>6</v>
+      </c>
+      <c r="G161" s="2">
+        <v>0</v>
+      </c>
+      <c r="H161" s="3">
+        <v>0</v>
+      </c>
+      <c r="I161" s="3">
+        <v>0</v>
+      </c>
+      <c r="J161" s="4">
+        <v>1</v>
+      </c>
+      <c r="K161" s="4">
+        <v>1</v>
+      </c>
+      <c r="L161" s="4">
+        <v>1</v>
+      </c>
+      <c r="M161" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with 10/16 survival
</commit_message>
<xml_diff>
--- a/data/survival/lab_survival/lab_survival.xlsx
+++ b/data/survival/lab_survival/lab_survival.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/survival/lab_survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5924A3E8-4B1F-FD4F-B347-E37DA3E9F6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6192593F-75EF-0845-B468-C3496A1A0815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17720" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
+    <workbookView xWindow="-33880" yWindow="-1460" windowWidth="20700" windowHeight="18300" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -483,11 +483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7ACAA-9959-8D4E-8E48-CFF679AAAAC5}">
-  <dimension ref="A1:N321"/>
+  <dimension ref="A1:N401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F327" sqref="F327"/>
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J389" sqref="J389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12868,7 +12868,10 @@
       <c r="K302" s="3">
         <v>0</v>
       </c>
-      <c r="L302" s="4">
+      <c r="L302" s="3">
+        <v>0</v>
+      </c>
+      <c r="M302" s="4">
         <v>1</v>
       </c>
     </row>
@@ -12897,8 +12900,8 @@
       <c r="H303" s="3">
         <v>0</v>
       </c>
-      <c r="I303" s="4">
-        <v>1</v>
+      <c r="I303" s="3">
+        <v>0</v>
       </c>
       <c r="J303" s="4">
         <v>1</v>
@@ -12907,6 +12910,9 @@
         <v>1</v>
       </c>
       <c r="L303" s="4">
+        <v>1</v>
+      </c>
+      <c r="M303" s="4">
         <v>1</v>
       </c>
     </row>
@@ -12935,8 +12941,8 @@
       <c r="H304" s="3">
         <v>0</v>
       </c>
-      <c r="I304" s="4">
-        <v>1</v>
+      <c r="I304" s="3">
+        <v>0</v>
       </c>
       <c r="J304" s="4">
         <v>1</v>
@@ -12947,8 +12953,11 @@
       <c r="L304" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M304" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>45579</v>
       </c>
@@ -12973,8 +12982,8 @@
       <c r="H305" s="3">
         <v>0</v>
       </c>
-      <c r="I305" s="4">
-        <v>1</v>
+      <c r="I305" s="3">
+        <v>0</v>
       </c>
       <c r="J305" s="4">
         <v>1</v>
@@ -12985,8 +12994,11 @@
       <c r="L305" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M305" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>45579</v>
       </c>
@@ -13011,8 +13023,8 @@
       <c r="H306" s="3">
         <v>0</v>
       </c>
-      <c r="I306" s="4">
-        <v>1</v>
+      <c r="I306" s="3">
+        <v>0</v>
       </c>
       <c r="J306" s="4">
         <v>1</v>
@@ -13023,8 +13035,11 @@
       <c r="L306" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M306" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>45579</v>
       </c>
@@ -13052,8 +13067,8 @@
       <c r="I307" s="3">
         <v>0</v>
       </c>
-      <c r="J307" s="4">
-        <v>1</v>
+      <c r="J307" s="3">
+        <v>0</v>
       </c>
       <c r="K307" s="4">
         <v>1</v>
@@ -13061,8 +13076,11 @@
       <c r="L307" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M307" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>45579</v>
       </c>
@@ -13090,8 +13108,8 @@
       <c r="I308" s="3">
         <v>0</v>
       </c>
-      <c r="J308" s="4">
-        <v>1</v>
+      <c r="J308" s="3">
+        <v>0</v>
       </c>
       <c r="K308" s="4">
         <v>1</v>
@@ -13099,8 +13117,11 @@
       <c r="L308" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M308" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>45579</v>
       </c>
@@ -13128,8 +13149,8 @@
       <c r="I309" s="3">
         <v>0</v>
       </c>
-      <c r="J309" s="4">
-        <v>1</v>
+      <c r="J309" s="3">
+        <v>0</v>
       </c>
       <c r="K309" s="4">
         <v>1</v>
@@ -13137,8 +13158,11 @@
       <c r="L309" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M309" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>45579</v>
       </c>
@@ -13172,11 +13196,14 @@
       <c r="K310" s="3">
         <v>0</v>
       </c>
-      <c r="L310" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L310" s="3">
+        <v>0</v>
+      </c>
+      <c r="M310" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>45579</v>
       </c>
@@ -13207,14 +13234,17 @@
       <c r="J311" s="3">
         <v>0</v>
       </c>
-      <c r="K311" s="4">
-        <v>1</v>
+      <c r="K311" s="3">
+        <v>0</v>
       </c>
       <c r="L311" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M311" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>45579</v>
       </c>
@@ -13236,8 +13266,8 @@
       <c r="G312" s="3">
         <v>0</v>
       </c>
-      <c r="H312" s="4">
-        <v>1</v>
+      <c r="H312" s="3">
+        <v>0</v>
       </c>
       <c r="I312" s="4">
         <v>1</v>
@@ -13251,8 +13281,11 @@
       <c r="L312" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M312" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>45579</v>
       </c>
@@ -13286,11 +13319,14 @@
       <c r="K313" s="3">
         <v>0</v>
       </c>
-      <c r="L313" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L313" s="3">
+        <v>0</v>
+      </c>
+      <c r="M313" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>45579</v>
       </c>
@@ -13315,8 +13351,8 @@
       <c r="H314" s="3">
         <v>0</v>
       </c>
-      <c r="I314" s="4">
-        <v>1</v>
+      <c r="I314" s="3">
+        <v>0</v>
       </c>
       <c r="J314" s="4">
         <v>1</v>
@@ -13327,8 +13363,11 @@
       <c r="L314" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M314" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>45579</v>
       </c>
@@ -13350,8 +13389,8 @@
       <c r="G315" s="3">
         <v>0</v>
       </c>
-      <c r="H315" s="4">
-        <v>1</v>
+      <c r="H315" s="3">
+        <v>0</v>
       </c>
       <c r="I315" s="4">
         <v>1</v>
@@ -13365,8 +13404,11 @@
       <c r="L315" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M315" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>45579</v>
       </c>
@@ -13391,8 +13433,8 @@
       <c r="H316" s="3">
         <v>0</v>
       </c>
-      <c r="I316" s="4">
-        <v>1</v>
+      <c r="I316" s="3">
+        <v>0</v>
       </c>
       <c r="J316" s="4">
         <v>1</v>
@@ -13403,8 +13445,11 @@
       <c r="L316" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M316" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>45579</v>
       </c>
@@ -13429,8 +13474,8 @@
       <c r="H317" s="3">
         <v>0</v>
       </c>
-      <c r="I317" s="4">
-        <v>1</v>
+      <c r="I317" s="3">
+        <v>0</v>
       </c>
       <c r="J317" s="4">
         <v>1</v>
@@ -13441,8 +13486,11 @@
       <c r="L317" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M317" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>45579</v>
       </c>
@@ -13470,8 +13518,8 @@
       <c r="I318" s="3">
         <v>0</v>
       </c>
-      <c r="J318" s="4">
-        <v>1</v>
+      <c r="J318" s="3">
+        <v>0</v>
       </c>
       <c r="K318" s="4">
         <v>1</v>
@@ -13479,8 +13527,11 @@
       <c r="L318" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M318" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>45579</v>
       </c>
@@ -13505,8 +13556,8 @@
       <c r="H319" s="3">
         <v>0</v>
       </c>
-      <c r="I319" s="4">
-        <v>1</v>
+      <c r="I319" s="3">
+        <v>0</v>
       </c>
       <c r="J319" s="4">
         <v>1</v>
@@ -13517,8 +13568,11 @@
       <c r="L319" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M319" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>45579</v>
       </c>
@@ -13546,8 +13600,8 @@
       <c r="I320" s="3">
         <v>0</v>
       </c>
-      <c r="J320" s="4">
-        <v>1</v>
+      <c r="J320" s="3">
+        <v>0</v>
       </c>
       <c r="K320" s="4">
         <v>1</v>
@@ -13555,8 +13609,11 @@
       <c r="L320" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M320" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>45579</v>
       </c>
@@ -13590,7 +13647,3290 @@
       <c r="K321" s="3">
         <v>0</v>
       </c>
-      <c r="L321" s="4">
+      <c r="L321" s="3">
+        <v>0</v>
+      </c>
+      <c r="M321" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B322">
+        <v>8</v>
+      </c>
+      <c r="C322" t="s">
+        <v>17</v>
+      </c>
+      <c r="D322" t="s">
+        <v>8</v>
+      </c>
+      <c r="E322" t="s">
+        <v>13</v>
+      </c>
+      <c r="F322" s="2">
+        <v>19</v>
+      </c>
+      <c r="G322" s="3">
+        <v>0</v>
+      </c>
+      <c r="H322" s="3">
+        <v>0</v>
+      </c>
+      <c r="I322" s="3">
+        <v>0</v>
+      </c>
+      <c r="J322" s="3">
+        <v>0</v>
+      </c>
+      <c r="K322" s="3">
+        <v>0</v>
+      </c>
+      <c r="L322" s="3">
+        <v>0</v>
+      </c>
+      <c r="M322" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B323">
+        <v>8</v>
+      </c>
+      <c r="C323" t="s">
+        <v>17</v>
+      </c>
+      <c r="D323" t="s">
+        <v>8</v>
+      </c>
+      <c r="E323" t="s">
+        <v>13</v>
+      </c>
+      <c r="F323" s="2">
+        <v>4</v>
+      </c>
+      <c r="G323" s="3">
+        <v>0</v>
+      </c>
+      <c r="H323" s="3">
+        <v>0</v>
+      </c>
+      <c r="I323" s="3">
+        <v>0</v>
+      </c>
+      <c r="J323" s="3">
+        <v>0</v>
+      </c>
+      <c r="K323" s="3">
+        <v>0</v>
+      </c>
+      <c r="L323" s="3">
+        <v>0</v>
+      </c>
+      <c r="M323" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B324">
+        <v>8</v>
+      </c>
+      <c r="C324" t="s">
+        <v>17</v>
+      </c>
+      <c r="D324" t="s">
+        <v>8</v>
+      </c>
+      <c r="E324" t="s">
+        <v>13</v>
+      </c>
+      <c r="F324" s="2">
+        <v>8</v>
+      </c>
+      <c r="G324" s="3">
+        <v>0</v>
+      </c>
+      <c r="H324" s="3">
+        <v>0</v>
+      </c>
+      <c r="I324" s="3">
+        <v>0</v>
+      </c>
+      <c r="J324" s="3">
+        <v>0</v>
+      </c>
+      <c r="K324" s="3">
+        <v>0</v>
+      </c>
+      <c r="L324" s="3">
+        <v>0</v>
+      </c>
+      <c r="M324" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B325">
+        <v>8</v>
+      </c>
+      <c r="C325" t="s">
+        <v>17</v>
+      </c>
+      <c r="D325" t="s">
+        <v>8</v>
+      </c>
+      <c r="E325" t="s">
+        <v>13</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G325" s="3">
+        <v>0</v>
+      </c>
+      <c r="H325" s="3">
+        <v>0</v>
+      </c>
+      <c r="I325" s="3">
+        <v>0</v>
+      </c>
+      <c r="J325" s="3">
+        <v>0</v>
+      </c>
+      <c r="K325" s="3">
+        <v>0</v>
+      </c>
+      <c r="L325" s="3">
+        <v>0</v>
+      </c>
+      <c r="M325" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B326">
+        <v>8</v>
+      </c>
+      <c r="C326" t="s">
+        <v>17</v>
+      </c>
+      <c r="D326" t="s">
+        <v>8</v>
+      </c>
+      <c r="E326" t="s">
+        <v>13</v>
+      </c>
+      <c r="F326" s="2">
+        <v>19</v>
+      </c>
+      <c r="G326" s="3">
+        <v>0</v>
+      </c>
+      <c r="H326" s="3">
+        <v>0</v>
+      </c>
+      <c r="I326" s="3">
+        <v>0</v>
+      </c>
+      <c r="J326" s="3">
+        <v>0</v>
+      </c>
+      <c r="K326" s="3">
+        <v>0</v>
+      </c>
+      <c r="L326" s="3">
+        <v>0</v>
+      </c>
+      <c r="M326" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B327">
+        <v>8</v>
+      </c>
+      <c r="C327" t="s">
+        <v>17</v>
+      </c>
+      <c r="D327" t="s">
+        <v>8</v>
+      </c>
+      <c r="E327" t="s">
+        <v>13</v>
+      </c>
+      <c r="F327" s="2">
+        <v>8</v>
+      </c>
+      <c r="G327" s="3">
+        <v>0</v>
+      </c>
+      <c r="H327" s="3">
+        <v>0</v>
+      </c>
+      <c r="I327" s="3">
+        <v>0</v>
+      </c>
+      <c r="J327" s="3">
+        <v>0</v>
+      </c>
+      <c r="K327" s="3">
+        <v>0</v>
+      </c>
+      <c r="L327" s="3">
+        <v>0</v>
+      </c>
+      <c r="M327" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B328">
+        <v>8</v>
+      </c>
+      <c r="C328" t="s">
+        <v>17</v>
+      </c>
+      <c r="D328" t="s">
+        <v>8</v>
+      </c>
+      <c r="E328" t="s">
+        <v>13</v>
+      </c>
+      <c r="F328" s="2">
+        <v>2</v>
+      </c>
+      <c r="G328" s="3">
+        <v>0</v>
+      </c>
+      <c r="H328" s="3">
+        <v>0</v>
+      </c>
+      <c r="I328" s="3">
+        <v>0</v>
+      </c>
+      <c r="J328" s="3">
+        <v>0</v>
+      </c>
+      <c r="K328" s="3">
+        <v>0</v>
+      </c>
+      <c r="L328" s="3">
+        <v>0</v>
+      </c>
+      <c r="M328" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B329">
+        <v>8</v>
+      </c>
+      <c r="C329" t="s">
+        <v>17</v>
+      </c>
+      <c r="D329" t="s">
+        <v>8</v>
+      </c>
+      <c r="E329" t="s">
+        <v>13</v>
+      </c>
+      <c r="F329" s="2">
+        <v>23</v>
+      </c>
+      <c r="G329" s="3">
+        <v>0</v>
+      </c>
+      <c r="H329" s="3">
+        <v>0</v>
+      </c>
+      <c r="I329" s="3">
+        <v>0</v>
+      </c>
+      <c r="J329" s="3">
+        <v>0</v>
+      </c>
+      <c r="K329" s="3">
+        <v>0</v>
+      </c>
+      <c r="L329" s="3">
+        <v>0</v>
+      </c>
+      <c r="M329" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B330">
+        <v>8</v>
+      </c>
+      <c r="C330" t="s">
+        <v>17</v>
+      </c>
+      <c r="D330" t="s">
+        <v>8</v>
+      </c>
+      <c r="E330" t="s">
+        <v>13</v>
+      </c>
+      <c r="F330" s="2">
+        <v>24</v>
+      </c>
+      <c r="G330" s="3">
+        <v>0</v>
+      </c>
+      <c r="H330" s="3">
+        <v>0</v>
+      </c>
+      <c r="I330" s="3">
+        <v>0</v>
+      </c>
+      <c r="J330" s="3">
+        <v>0</v>
+      </c>
+      <c r="K330" s="3">
+        <v>0</v>
+      </c>
+      <c r="L330" s="3">
+        <v>0</v>
+      </c>
+      <c r="M330" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B331">
+        <v>8</v>
+      </c>
+      <c r="C331" t="s">
+        <v>17</v>
+      </c>
+      <c r="D331" t="s">
+        <v>8</v>
+      </c>
+      <c r="E331" t="s">
+        <v>13</v>
+      </c>
+      <c r="F331" s="2">
+        <v>5</v>
+      </c>
+      <c r="G331" s="3">
+        <v>0</v>
+      </c>
+      <c r="H331" s="3">
+        <v>0</v>
+      </c>
+      <c r="I331" s="3">
+        <v>0</v>
+      </c>
+      <c r="J331" s="3">
+        <v>0</v>
+      </c>
+      <c r="K331" s="3">
+        <v>0</v>
+      </c>
+      <c r="L331" s="3">
+        <v>0</v>
+      </c>
+      <c r="M331" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B332">
+        <v>8</v>
+      </c>
+      <c r="C332" t="s">
+        <v>17</v>
+      </c>
+      <c r="D332" t="s">
+        <v>8</v>
+      </c>
+      <c r="E332" t="s">
+        <v>13</v>
+      </c>
+      <c r="F332" s="2">
+        <v>37</v>
+      </c>
+      <c r="G332" s="3">
+        <v>0</v>
+      </c>
+      <c r="H332" s="3">
+        <v>0</v>
+      </c>
+      <c r="I332" s="3">
+        <v>0</v>
+      </c>
+      <c r="J332" s="3">
+        <v>0</v>
+      </c>
+      <c r="K332" s="3">
+        <v>0</v>
+      </c>
+      <c r="L332" s="3">
+        <v>0</v>
+      </c>
+      <c r="M332" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B333">
+        <v>8</v>
+      </c>
+      <c r="C333" t="s">
+        <v>17</v>
+      </c>
+      <c r="D333" t="s">
+        <v>8</v>
+      </c>
+      <c r="E333" t="s">
+        <v>13</v>
+      </c>
+      <c r="F333" s="2">
+        <v>40</v>
+      </c>
+      <c r="G333" s="3">
+        <v>0</v>
+      </c>
+      <c r="H333" s="3">
+        <v>0</v>
+      </c>
+      <c r="I333" s="3">
+        <v>0</v>
+      </c>
+      <c r="J333" s="3">
+        <v>0</v>
+      </c>
+      <c r="K333" s="3">
+        <v>0</v>
+      </c>
+      <c r="L333" s="3">
+        <v>0</v>
+      </c>
+      <c r="M333" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B334">
+        <v>8</v>
+      </c>
+      <c r="C334" t="s">
+        <v>17</v>
+      </c>
+      <c r="D334" t="s">
+        <v>8</v>
+      </c>
+      <c r="E334" t="s">
+        <v>13</v>
+      </c>
+      <c r="F334" s="2">
+        <v>2</v>
+      </c>
+      <c r="G334" s="3">
+        <v>0</v>
+      </c>
+      <c r="H334" s="3">
+        <v>0</v>
+      </c>
+      <c r="I334" s="3">
+        <v>0</v>
+      </c>
+      <c r="J334" s="3">
+        <v>0</v>
+      </c>
+      <c r="K334" s="3">
+        <v>0</v>
+      </c>
+      <c r="L334" s="3">
+        <v>0</v>
+      </c>
+      <c r="M334" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B335">
+        <v>8</v>
+      </c>
+      <c r="C335" t="s">
+        <v>17</v>
+      </c>
+      <c r="D335" t="s">
+        <v>8</v>
+      </c>
+      <c r="E335" t="s">
+        <v>13</v>
+      </c>
+      <c r="F335" s="2">
+        <v>38</v>
+      </c>
+      <c r="G335" s="3">
+        <v>0</v>
+      </c>
+      <c r="H335" s="3">
+        <v>0</v>
+      </c>
+      <c r="I335" s="3">
+        <v>0</v>
+      </c>
+      <c r="J335" s="3">
+        <v>0</v>
+      </c>
+      <c r="K335" s="3">
+        <v>0</v>
+      </c>
+      <c r="L335" s="3">
+        <v>0</v>
+      </c>
+      <c r="M335" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A336" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B336">
+        <v>8</v>
+      </c>
+      <c r="C336" t="s">
+        <v>17</v>
+      </c>
+      <c r="D336" t="s">
+        <v>8</v>
+      </c>
+      <c r="E336" t="s">
+        <v>13</v>
+      </c>
+      <c r="F336" s="2">
+        <v>20</v>
+      </c>
+      <c r="G336" s="3">
+        <v>0</v>
+      </c>
+      <c r="H336" s="3">
+        <v>0</v>
+      </c>
+      <c r="I336" s="3">
+        <v>0</v>
+      </c>
+      <c r="J336" s="3">
+        <v>0</v>
+      </c>
+      <c r="K336" s="3">
+        <v>0</v>
+      </c>
+      <c r="L336" s="3">
+        <v>0</v>
+      </c>
+      <c r="M336" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B337">
+        <v>8</v>
+      </c>
+      <c r="C337" t="s">
+        <v>17</v>
+      </c>
+      <c r="D337" t="s">
+        <v>8</v>
+      </c>
+      <c r="E337" t="s">
+        <v>13</v>
+      </c>
+      <c r="F337" s="2">
+        <v>24</v>
+      </c>
+      <c r="G337" s="3">
+        <v>0</v>
+      </c>
+      <c r="H337" s="3">
+        <v>0</v>
+      </c>
+      <c r="I337" s="3">
+        <v>0</v>
+      </c>
+      <c r="J337" s="3">
+        <v>0</v>
+      </c>
+      <c r="K337" s="3">
+        <v>0</v>
+      </c>
+      <c r="L337" s="3">
+        <v>0</v>
+      </c>
+      <c r="M337" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A338" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B338">
+        <v>8</v>
+      </c>
+      <c r="C338" t="s">
+        <v>17</v>
+      </c>
+      <c r="D338" t="s">
+        <v>8</v>
+      </c>
+      <c r="E338" t="s">
+        <v>13</v>
+      </c>
+      <c r="F338" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G338" s="3">
+        <v>0</v>
+      </c>
+      <c r="H338" s="3">
+        <v>0</v>
+      </c>
+      <c r="I338" s="3">
+        <v>0</v>
+      </c>
+      <c r="J338" s="3">
+        <v>0</v>
+      </c>
+      <c r="K338" s="3">
+        <v>0</v>
+      </c>
+      <c r="L338" s="3">
+        <v>0</v>
+      </c>
+      <c r="M338" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A339" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B339">
+        <v>8</v>
+      </c>
+      <c r="C339" t="s">
+        <v>17</v>
+      </c>
+      <c r="D339" t="s">
+        <v>8</v>
+      </c>
+      <c r="E339" t="s">
+        <v>13</v>
+      </c>
+      <c r="F339" s="2">
+        <v>15</v>
+      </c>
+      <c r="G339" s="3">
+        <v>0</v>
+      </c>
+      <c r="H339" s="3">
+        <v>0</v>
+      </c>
+      <c r="I339" s="3">
+        <v>0</v>
+      </c>
+      <c r="J339" s="3">
+        <v>0</v>
+      </c>
+      <c r="K339" s="3">
+        <v>0</v>
+      </c>
+      <c r="L339" s="3">
+        <v>0</v>
+      </c>
+      <c r="M339" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A340" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B340">
+        <v>8</v>
+      </c>
+      <c r="C340" t="s">
+        <v>17</v>
+      </c>
+      <c r="D340" t="s">
+        <v>8</v>
+      </c>
+      <c r="E340" t="s">
+        <v>13</v>
+      </c>
+      <c r="F340" s="2">
+        <v>16</v>
+      </c>
+      <c r="G340" s="3">
+        <v>0</v>
+      </c>
+      <c r="H340" s="3">
+        <v>0</v>
+      </c>
+      <c r="I340" s="3">
+        <v>0</v>
+      </c>
+      <c r="J340" s="3">
+        <v>0</v>
+      </c>
+      <c r="K340" s="3">
+        <v>0</v>
+      </c>
+      <c r="L340" s="3">
+        <v>0</v>
+      </c>
+      <c r="M340" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A341" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B341">
+        <v>8</v>
+      </c>
+      <c r="C341" t="s">
+        <v>17</v>
+      </c>
+      <c r="D341" t="s">
+        <v>8</v>
+      </c>
+      <c r="E341" t="s">
+        <v>13</v>
+      </c>
+      <c r="F341" s="2">
+        <v>33</v>
+      </c>
+      <c r="G341" s="3">
+        <v>0</v>
+      </c>
+      <c r="H341" s="3">
+        <v>0</v>
+      </c>
+      <c r="I341" s="3">
+        <v>0</v>
+      </c>
+      <c r="J341" s="3">
+        <v>0</v>
+      </c>
+      <c r="K341" s="3">
+        <v>0</v>
+      </c>
+      <c r="L341" s="3">
+        <v>0</v>
+      </c>
+      <c r="M341" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A342" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B342">
+        <v>8</v>
+      </c>
+      <c r="C342" t="s">
+        <v>17</v>
+      </c>
+      <c r="D342" t="s">
+        <v>8</v>
+      </c>
+      <c r="E342" t="s">
+        <v>12</v>
+      </c>
+      <c r="F342" s="2">
+        <v>1</v>
+      </c>
+      <c r="G342" s="3">
+        <v>0</v>
+      </c>
+      <c r="H342" s="3">
+        <v>0</v>
+      </c>
+      <c r="I342" s="3">
+        <v>0</v>
+      </c>
+      <c r="J342" s="3">
+        <v>0</v>
+      </c>
+      <c r="K342" s="4">
+        <v>1</v>
+      </c>
+      <c r="L342" s="4">
+        <v>1</v>
+      </c>
+      <c r="M342" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A343" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B343">
+        <v>8</v>
+      </c>
+      <c r="C343" t="s">
+        <v>17</v>
+      </c>
+      <c r="D343" t="s">
+        <v>8</v>
+      </c>
+      <c r="E343" t="s">
+        <v>12</v>
+      </c>
+      <c r="F343" s="2">
+        <v>34</v>
+      </c>
+      <c r="G343" s="3">
+        <v>0</v>
+      </c>
+      <c r="H343" s="3">
+        <v>0</v>
+      </c>
+      <c r="I343" s="3">
+        <v>0</v>
+      </c>
+      <c r="J343" s="4">
+        <v>1</v>
+      </c>
+      <c r="K343" s="4">
+        <v>1</v>
+      </c>
+      <c r="L343" s="4">
+        <v>1</v>
+      </c>
+      <c r="M343" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A344" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B344">
+        <v>8</v>
+      </c>
+      <c r="C344" t="s">
+        <v>17</v>
+      </c>
+      <c r="D344" t="s">
+        <v>8</v>
+      </c>
+      <c r="E344" t="s">
+        <v>12</v>
+      </c>
+      <c r="F344" s="2">
+        <v>26</v>
+      </c>
+      <c r="G344" s="3">
+        <v>0</v>
+      </c>
+      <c r="H344" s="3">
+        <v>0</v>
+      </c>
+      <c r="I344" s="3">
+        <v>0</v>
+      </c>
+      <c r="J344" s="3">
+        <v>0</v>
+      </c>
+      <c r="K344" s="3">
+        <v>0</v>
+      </c>
+      <c r="L344" s="3">
+        <v>0</v>
+      </c>
+      <c r="M344" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A345" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B345">
+        <v>8</v>
+      </c>
+      <c r="C345" t="s">
+        <v>17</v>
+      </c>
+      <c r="D345" t="s">
+        <v>8</v>
+      </c>
+      <c r="E345" t="s">
+        <v>12</v>
+      </c>
+      <c r="F345" s="2">
+        <v>22</v>
+      </c>
+      <c r="G345" s="3">
+        <v>0</v>
+      </c>
+      <c r="H345" s="3">
+        <v>0</v>
+      </c>
+      <c r="I345" s="3">
+        <v>0</v>
+      </c>
+      <c r="J345" s="3">
+        <v>0</v>
+      </c>
+      <c r="K345" s="3">
+        <v>0</v>
+      </c>
+      <c r="L345" s="3">
+        <v>0</v>
+      </c>
+      <c r="M345" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A346" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B346">
+        <v>8</v>
+      </c>
+      <c r="C346" t="s">
+        <v>17</v>
+      </c>
+      <c r="D346" t="s">
+        <v>8</v>
+      </c>
+      <c r="E346" t="s">
+        <v>12</v>
+      </c>
+      <c r="F346" s="2">
+        <v>16</v>
+      </c>
+      <c r="G346" s="3">
+        <v>0</v>
+      </c>
+      <c r="H346" s="3">
+        <v>0</v>
+      </c>
+      <c r="I346" s="3">
+        <v>0</v>
+      </c>
+      <c r="J346" s="4">
+        <v>1</v>
+      </c>
+      <c r="K346" s="4">
+        <v>1</v>
+      </c>
+      <c r="L346" s="4">
+        <v>1</v>
+      </c>
+      <c r="M346" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A347" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B347">
+        <v>8</v>
+      </c>
+      <c r="C347" t="s">
+        <v>17</v>
+      </c>
+      <c r="D347" t="s">
+        <v>8</v>
+      </c>
+      <c r="E347" t="s">
+        <v>12</v>
+      </c>
+      <c r="F347" s="2">
+        <v>25</v>
+      </c>
+      <c r="G347" s="3">
+        <v>0</v>
+      </c>
+      <c r="H347" s="3">
+        <v>0</v>
+      </c>
+      <c r="I347" s="3">
+        <v>0</v>
+      </c>
+      <c r="J347" s="3">
+        <v>0</v>
+      </c>
+      <c r="K347" s="3">
+        <v>0</v>
+      </c>
+      <c r="L347" s="3">
+        <v>0</v>
+      </c>
+      <c r="M347" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A348" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B348">
+        <v>8</v>
+      </c>
+      <c r="C348" t="s">
+        <v>17</v>
+      </c>
+      <c r="D348" t="s">
+        <v>8</v>
+      </c>
+      <c r="E348" t="s">
+        <v>12</v>
+      </c>
+      <c r="F348" s="2">
+        <v>35</v>
+      </c>
+      <c r="G348" s="3">
+        <v>0</v>
+      </c>
+      <c r="H348" s="3">
+        <v>0</v>
+      </c>
+      <c r="I348" s="3">
+        <v>0</v>
+      </c>
+      <c r="J348" s="3">
+        <v>0</v>
+      </c>
+      <c r="K348" s="4">
+        <v>1</v>
+      </c>
+      <c r="L348" s="4">
+        <v>1</v>
+      </c>
+      <c r="M348" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A349" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B349">
+        <v>8</v>
+      </c>
+      <c r="C349" t="s">
+        <v>17</v>
+      </c>
+      <c r="D349" t="s">
+        <v>8</v>
+      </c>
+      <c r="E349" t="s">
+        <v>12</v>
+      </c>
+      <c r="F349" s="2">
+        <v>19</v>
+      </c>
+      <c r="G349" s="3">
+        <v>0</v>
+      </c>
+      <c r="H349" s="3">
+        <v>0</v>
+      </c>
+      <c r="I349" s="3">
+        <v>0</v>
+      </c>
+      <c r="J349" s="3">
+        <v>0</v>
+      </c>
+      <c r="K349" s="3">
+        <v>0</v>
+      </c>
+      <c r="L349" s="4">
+        <v>1</v>
+      </c>
+      <c r="M349" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A350" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B350">
+        <v>8</v>
+      </c>
+      <c r="C350" t="s">
+        <v>17</v>
+      </c>
+      <c r="D350" t="s">
+        <v>8</v>
+      </c>
+      <c r="E350" t="s">
+        <v>12</v>
+      </c>
+      <c r="F350" s="2">
+        <v>10</v>
+      </c>
+      <c r="G350" s="3">
+        <v>0</v>
+      </c>
+      <c r="H350" s="3">
+        <v>0</v>
+      </c>
+      <c r="I350" s="3">
+        <v>0</v>
+      </c>
+      <c r="J350" s="4">
+        <v>1</v>
+      </c>
+      <c r="K350" s="4">
+        <v>1</v>
+      </c>
+      <c r="L350" s="4">
+        <v>1</v>
+      </c>
+      <c r="M350" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A351" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B351">
+        <v>8</v>
+      </c>
+      <c r="C351" t="s">
+        <v>17</v>
+      </c>
+      <c r="D351" t="s">
+        <v>8</v>
+      </c>
+      <c r="E351" t="s">
+        <v>12</v>
+      </c>
+      <c r="F351" s="2">
+        <v>13</v>
+      </c>
+      <c r="G351" s="3">
+        <v>0</v>
+      </c>
+      <c r="H351" s="3">
+        <v>0</v>
+      </c>
+      <c r="I351" s="3">
+        <v>0</v>
+      </c>
+      <c r="J351" s="4">
+        <v>1</v>
+      </c>
+      <c r="K351" s="4">
+        <v>1</v>
+      </c>
+      <c r="L351" s="4">
+        <v>1</v>
+      </c>
+      <c r="M351" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B352">
+        <v>8</v>
+      </c>
+      <c r="C352" t="s">
+        <v>17</v>
+      </c>
+      <c r="D352" t="s">
+        <v>8</v>
+      </c>
+      <c r="E352" t="s">
+        <v>12</v>
+      </c>
+      <c r="F352" s="2">
+        <v>18</v>
+      </c>
+      <c r="G352" s="3">
+        <v>0</v>
+      </c>
+      <c r="H352" s="3">
+        <v>0</v>
+      </c>
+      <c r="I352" s="3">
+        <v>0</v>
+      </c>
+      <c r="J352" s="3">
+        <v>0</v>
+      </c>
+      <c r="K352" s="3">
+        <v>0</v>
+      </c>
+      <c r="L352" s="3">
+        <v>0</v>
+      </c>
+      <c r="M352" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A353" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B353">
+        <v>8</v>
+      </c>
+      <c r="C353" t="s">
+        <v>17</v>
+      </c>
+      <c r="D353" t="s">
+        <v>8</v>
+      </c>
+      <c r="E353" t="s">
+        <v>12</v>
+      </c>
+      <c r="F353" s="2">
+        <v>14</v>
+      </c>
+      <c r="G353" s="3">
+        <v>0</v>
+      </c>
+      <c r="H353" s="3">
+        <v>0</v>
+      </c>
+      <c r="I353" s="3">
+        <v>0</v>
+      </c>
+      <c r="J353" s="4">
+        <v>1</v>
+      </c>
+      <c r="K353" s="4">
+        <v>1</v>
+      </c>
+      <c r="L353" s="4">
+        <v>1</v>
+      </c>
+      <c r="M353" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A354" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B354">
+        <v>8</v>
+      </c>
+      <c r="C354" t="s">
+        <v>17</v>
+      </c>
+      <c r="D354" t="s">
+        <v>8</v>
+      </c>
+      <c r="E354" t="s">
+        <v>12</v>
+      </c>
+      <c r="F354" s="2">
+        <v>17</v>
+      </c>
+      <c r="G354" s="3">
+        <v>0</v>
+      </c>
+      <c r="H354" s="3">
+        <v>0</v>
+      </c>
+      <c r="I354" s="4">
+        <v>1</v>
+      </c>
+      <c r="J354" s="4">
+        <v>1</v>
+      </c>
+      <c r="K354" s="4">
+        <v>1</v>
+      </c>
+      <c r="L354" s="4">
+        <v>1</v>
+      </c>
+      <c r="M354" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A355" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B355">
+        <v>8</v>
+      </c>
+      <c r="C355" t="s">
+        <v>17</v>
+      </c>
+      <c r="D355" t="s">
+        <v>8</v>
+      </c>
+      <c r="E355" t="s">
+        <v>12</v>
+      </c>
+      <c r="F355" s="2">
+        <v>39</v>
+      </c>
+      <c r="G355" s="3">
+        <v>0</v>
+      </c>
+      <c r="H355" s="3">
+        <v>0</v>
+      </c>
+      <c r="I355" s="3">
+        <v>0</v>
+      </c>
+      <c r="J355" s="3">
+        <v>0</v>
+      </c>
+      <c r="K355" s="4">
+        <v>1</v>
+      </c>
+      <c r="L355" s="4">
+        <v>1</v>
+      </c>
+      <c r="M355" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A356" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B356">
+        <v>8</v>
+      </c>
+      <c r="C356" t="s">
+        <v>17</v>
+      </c>
+      <c r="D356" t="s">
+        <v>8</v>
+      </c>
+      <c r="E356" t="s">
+        <v>12</v>
+      </c>
+      <c r="F356" s="2">
+        <v>3</v>
+      </c>
+      <c r="G356" s="3">
+        <v>0</v>
+      </c>
+      <c r="H356" s="3">
+        <v>0</v>
+      </c>
+      <c r="I356" s="4">
+        <v>1</v>
+      </c>
+      <c r="J356" s="4">
+        <v>1</v>
+      </c>
+      <c r="K356" s="4">
+        <v>1</v>
+      </c>
+      <c r="L356" s="4">
+        <v>1</v>
+      </c>
+      <c r="M356" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A357" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B357">
+        <v>8</v>
+      </c>
+      <c r="C357" t="s">
+        <v>17</v>
+      </c>
+      <c r="D357" t="s">
+        <v>8</v>
+      </c>
+      <c r="E357" t="s">
+        <v>12</v>
+      </c>
+      <c r="F357" s="2">
+        <v>27</v>
+      </c>
+      <c r="G357" s="3">
+        <v>0</v>
+      </c>
+      <c r="H357" s="3">
+        <v>0</v>
+      </c>
+      <c r="I357" s="3">
+        <v>0</v>
+      </c>
+      <c r="J357" s="3">
+        <v>0</v>
+      </c>
+      <c r="K357" s="3">
+        <v>0</v>
+      </c>
+      <c r="L357" s="3">
+        <v>0</v>
+      </c>
+      <c r="M357" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A358" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B358">
+        <v>8</v>
+      </c>
+      <c r="C358" t="s">
+        <v>17</v>
+      </c>
+      <c r="D358" t="s">
+        <v>8</v>
+      </c>
+      <c r="E358" t="s">
+        <v>12</v>
+      </c>
+      <c r="F358" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G358" s="3">
+        <v>0</v>
+      </c>
+      <c r="H358" s="3">
+        <v>0</v>
+      </c>
+      <c r="I358" s="3">
+        <v>0</v>
+      </c>
+      <c r="J358" s="3">
+        <v>0</v>
+      </c>
+      <c r="K358" s="4">
+        <v>1</v>
+      </c>
+      <c r="L358" s="4">
+        <v>1</v>
+      </c>
+      <c r="M358" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A359" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B359">
+        <v>8</v>
+      </c>
+      <c r="C359" t="s">
+        <v>17</v>
+      </c>
+      <c r="D359" t="s">
+        <v>8</v>
+      </c>
+      <c r="E359" t="s">
+        <v>12</v>
+      </c>
+      <c r="F359" s="2">
+        <v>21</v>
+      </c>
+      <c r="G359" s="3">
+        <v>0</v>
+      </c>
+      <c r="H359" s="3">
+        <v>0</v>
+      </c>
+      <c r="I359" s="3">
+        <v>0</v>
+      </c>
+      <c r="J359" s="3">
+        <v>0</v>
+      </c>
+      <c r="K359" s="3">
+        <v>0</v>
+      </c>
+      <c r="L359" s="3">
+        <v>0</v>
+      </c>
+      <c r="M359" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A360" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B360">
+        <v>8</v>
+      </c>
+      <c r="C360" t="s">
+        <v>17</v>
+      </c>
+      <c r="D360" t="s">
+        <v>8</v>
+      </c>
+      <c r="E360" t="s">
+        <v>12</v>
+      </c>
+      <c r="F360" s="2">
+        <v>26</v>
+      </c>
+      <c r="G360" s="3">
+        <v>0</v>
+      </c>
+      <c r="H360" s="3">
+        <v>0</v>
+      </c>
+      <c r="I360" s="3">
+        <v>0</v>
+      </c>
+      <c r="J360" s="4">
+        <v>1</v>
+      </c>
+      <c r="K360" s="4">
+        <v>1</v>
+      </c>
+      <c r="L360" s="4">
+        <v>1</v>
+      </c>
+      <c r="M360" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A361" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B361">
+        <v>8</v>
+      </c>
+      <c r="C361" t="s">
+        <v>17</v>
+      </c>
+      <c r="D361" t="s">
+        <v>8</v>
+      </c>
+      <c r="E361" t="s">
+        <v>12</v>
+      </c>
+      <c r="F361" s="2">
+        <v>5</v>
+      </c>
+      <c r="G361" s="3">
+        <v>0</v>
+      </c>
+      <c r="H361" s="3">
+        <v>0</v>
+      </c>
+      <c r="I361" s="3">
+        <v>0</v>
+      </c>
+      <c r="J361" s="3">
+        <v>0</v>
+      </c>
+      <c r="K361" s="3">
+        <v>0</v>
+      </c>
+      <c r="L361" s="4">
+        <v>1</v>
+      </c>
+      <c r="M361" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A362" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B362">
+        <v>16</v>
+      </c>
+      <c r="C362" t="s">
+        <v>17</v>
+      </c>
+      <c r="D362" t="s">
+        <v>9</v>
+      </c>
+      <c r="E362" t="s">
+        <v>13</v>
+      </c>
+      <c r="F362" s="2">
+        <v>32</v>
+      </c>
+      <c r="G362" s="3">
+        <v>0</v>
+      </c>
+      <c r="H362" s="3">
+        <v>0</v>
+      </c>
+      <c r="I362" s="3">
+        <v>0</v>
+      </c>
+      <c r="J362" s="3">
+        <v>0</v>
+      </c>
+      <c r="K362" s="3">
+        <v>0</v>
+      </c>
+      <c r="L362" s="3">
+        <v>0</v>
+      </c>
+      <c r="M362" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A363" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B363">
+        <v>16</v>
+      </c>
+      <c r="C363" t="s">
+        <v>17</v>
+      </c>
+      <c r="D363" t="s">
+        <v>9</v>
+      </c>
+      <c r="E363" t="s">
+        <v>13</v>
+      </c>
+      <c r="F363" s="2">
+        <v>33</v>
+      </c>
+      <c r="G363" s="3">
+        <v>0</v>
+      </c>
+      <c r="H363" s="3">
+        <v>0</v>
+      </c>
+      <c r="I363" s="3">
+        <v>0</v>
+      </c>
+      <c r="J363" s="3">
+        <v>0</v>
+      </c>
+      <c r="K363" s="3">
+        <v>0</v>
+      </c>
+      <c r="L363" s="3">
+        <v>0</v>
+      </c>
+      <c r="M363" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A364" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B364">
+        <v>16</v>
+      </c>
+      <c r="C364" t="s">
+        <v>17</v>
+      </c>
+      <c r="D364" t="s">
+        <v>9</v>
+      </c>
+      <c r="E364" t="s">
+        <v>13</v>
+      </c>
+      <c r="F364" s="2">
+        <v>17</v>
+      </c>
+      <c r="G364" s="3">
+        <v>0</v>
+      </c>
+      <c r="H364" s="3">
+        <v>0</v>
+      </c>
+      <c r="I364" s="3">
+        <v>0</v>
+      </c>
+      <c r="J364" s="3">
+        <v>0</v>
+      </c>
+      <c r="K364" s="3">
+        <v>0</v>
+      </c>
+      <c r="L364" s="3">
+        <v>0</v>
+      </c>
+      <c r="M364" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A365" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B365">
+        <v>16</v>
+      </c>
+      <c r="C365" t="s">
+        <v>17</v>
+      </c>
+      <c r="D365" t="s">
+        <v>9</v>
+      </c>
+      <c r="E365" t="s">
+        <v>13</v>
+      </c>
+      <c r="F365" s="2">
+        <v>222</v>
+      </c>
+      <c r="G365" s="3">
+        <v>0</v>
+      </c>
+      <c r="H365" s="3">
+        <v>0</v>
+      </c>
+      <c r="I365" s="3">
+        <v>0</v>
+      </c>
+      <c r="J365" s="3">
+        <v>0</v>
+      </c>
+      <c r="K365" s="3">
+        <v>0</v>
+      </c>
+      <c r="L365" s="3">
+        <v>0</v>
+      </c>
+      <c r="M365" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A366" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B366">
+        <v>16</v>
+      </c>
+      <c r="C366" t="s">
+        <v>17</v>
+      </c>
+      <c r="D366" t="s">
+        <v>9</v>
+      </c>
+      <c r="E366" t="s">
+        <v>13</v>
+      </c>
+      <c r="F366" s="2">
+        <v>29</v>
+      </c>
+      <c r="G366" s="3">
+        <v>0</v>
+      </c>
+      <c r="H366" s="3">
+        <v>0</v>
+      </c>
+      <c r="I366" s="3">
+        <v>0</v>
+      </c>
+      <c r="J366" s="3">
+        <v>0</v>
+      </c>
+      <c r="K366" s="3">
+        <v>0</v>
+      </c>
+      <c r="L366" s="3">
+        <v>0</v>
+      </c>
+      <c r="M366" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A367" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B367">
+        <v>16</v>
+      </c>
+      <c r="C367" t="s">
+        <v>17</v>
+      </c>
+      <c r="D367" t="s">
+        <v>9</v>
+      </c>
+      <c r="E367" t="s">
+        <v>13</v>
+      </c>
+      <c r="F367" s="2">
+        <v>152</v>
+      </c>
+      <c r="G367" s="3">
+        <v>0</v>
+      </c>
+      <c r="H367" s="3">
+        <v>0</v>
+      </c>
+      <c r="I367" s="3">
+        <v>0</v>
+      </c>
+      <c r="J367" s="3">
+        <v>0</v>
+      </c>
+      <c r="K367" s="3">
+        <v>0</v>
+      </c>
+      <c r="L367" s="3">
+        <v>0</v>
+      </c>
+      <c r="M367" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A368" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B368">
+        <v>16</v>
+      </c>
+      <c r="C368" t="s">
+        <v>17</v>
+      </c>
+      <c r="D368" t="s">
+        <v>9</v>
+      </c>
+      <c r="E368" t="s">
+        <v>13</v>
+      </c>
+      <c r="F368" s="2">
+        <v>112</v>
+      </c>
+      <c r="G368" s="3">
+        <v>0</v>
+      </c>
+      <c r="H368" s="3">
+        <v>0</v>
+      </c>
+      <c r="I368" s="3">
+        <v>0</v>
+      </c>
+      <c r="J368" s="3">
+        <v>0</v>
+      </c>
+      <c r="K368" s="3">
+        <v>0</v>
+      </c>
+      <c r="L368" s="3">
+        <v>0</v>
+      </c>
+      <c r="M368" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A369" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B369">
+        <v>16</v>
+      </c>
+      <c r="C369" t="s">
+        <v>17</v>
+      </c>
+      <c r="D369" t="s">
+        <v>9</v>
+      </c>
+      <c r="E369" t="s">
+        <v>13</v>
+      </c>
+      <c r="F369" s="2">
+        <v>38</v>
+      </c>
+      <c r="G369" s="3">
+        <v>0</v>
+      </c>
+      <c r="H369" s="3">
+        <v>0</v>
+      </c>
+      <c r="I369" s="3">
+        <v>0</v>
+      </c>
+      <c r="J369" s="3">
+        <v>0</v>
+      </c>
+      <c r="K369" s="3">
+        <v>0</v>
+      </c>
+      <c r="L369" s="3">
+        <v>0</v>
+      </c>
+      <c r="M369" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A370" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B370">
+        <v>16</v>
+      </c>
+      <c r="C370" t="s">
+        <v>17</v>
+      </c>
+      <c r="D370" t="s">
+        <v>9</v>
+      </c>
+      <c r="E370" t="s">
+        <v>13</v>
+      </c>
+      <c r="F370" s="2">
+        <v>18</v>
+      </c>
+      <c r="G370" s="3">
+        <v>0</v>
+      </c>
+      <c r="H370" s="3">
+        <v>0</v>
+      </c>
+      <c r="I370" s="3">
+        <v>0</v>
+      </c>
+      <c r="J370" s="3">
+        <v>0</v>
+      </c>
+      <c r="K370" s="3">
+        <v>0</v>
+      </c>
+      <c r="L370" s="3">
+        <v>0</v>
+      </c>
+      <c r="M370" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A371" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B371">
+        <v>16</v>
+      </c>
+      <c r="C371" t="s">
+        <v>17</v>
+      </c>
+      <c r="D371" t="s">
+        <v>9</v>
+      </c>
+      <c r="E371" t="s">
+        <v>13</v>
+      </c>
+      <c r="F371" s="2">
+        <v>26</v>
+      </c>
+      <c r="G371" s="3">
+        <v>0</v>
+      </c>
+      <c r="H371" s="3">
+        <v>0</v>
+      </c>
+      <c r="I371" s="3">
+        <v>0</v>
+      </c>
+      <c r="J371" s="3">
+        <v>0</v>
+      </c>
+      <c r="K371" s="3">
+        <v>0</v>
+      </c>
+      <c r="L371" s="3">
+        <v>0</v>
+      </c>
+      <c r="M371" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A372" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B372">
+        <v>16</v>
+      </c>
+      <c r="C372" t="s">
+        <v>17</v>
+      </c>
+      <c r="D372" t="s">
+        <v>9</v>
+      </c>
+      <c r="E372" t="s">
+        <v>13</v>
+      </c>
+      <c r="F372" s="2">
+        <v>19</v>
+      </c>
+      <c r="G372" s="3">
+        <v>0</v>
+      </c>
+      <c r="H372" s="3">
+        <v>0</v>
+      </c>
+      <c r="I372" s="3">
+        <v>0</v>
+      </c>
+      <c r="J372" s="3">
+        <v>0</v>
+      </c>
+      <c r="K372" s="3">
+        <v>0</v>
+      </c>
+      <c r="L372" s="3">
+        <v>0</v>
+      </c>
+      <c r="M372" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A373" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B373">
+        <v>16</v>
+      </c>
+      <c r="C373" t="s">
+        <v>17</v>
+      </c>
+      <c r="D373" t="s">
+        <v>9</v>
+      </c>
+      <c r="E373" t="s">
+        <v>13</v>
+      </c>
+      <c r="F373" s="2">
+        <v>2</v>
+      </c>
+      <c r="G373" s="3">
+        <v>0</v>
+      </c>
+      <c r="H373" s="3">
+        <v>0</v>
+      </c>
+      <c r="I373" s="3">
+        <v>0</v>
+      </c>
+      <c r="J373" s="3">
+        <v>0</v>
+      </c>
+      <c r="K373" s="3">
+        <v>0</v>
+      </c>
+      <c r="L373" s="3">
+        <v>0</v>
+      </c>
+      <c r="M373" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A374" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B374">
+        <v>16</v>
+      </c>
+      <c r="C374" t="s">
+        <v>17</v>
+      </c>
+      <c r="D374" t="s">
+        <v>9</v>
+      </c>
+      <c r="E374" t="s">
+        <v>13</v>
+      </c>
+      <c r="F374" s="2">
+        <v>36</v>
+      </c>
+      <c r="G374" s="3">
+        <v>0</v>
+      </c>
+      <c r="H374" s="3">
+        <v>0</v>
+      </c>
+      <c r="I374" s="3">
+        <v>0</v>
+      </c>
+      <c r="J374" s="3">
+        <v>0</v>
+      </c>
+      <c r="K374" s="3">
+        <v>0</v>
+      </c>
+      <c r="L374" s="3">
+        <v>0</v>
+      </c>
+      <c r="M374" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A375" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B375">
+        <v>16</v>
+      </c>
+      <c r="C375" t="s">
+        <v>17</v>
+      </c>
+      <c r="D375" t="s">
+        <v>9</v>
+      </c>
+      <c r="E375" t="s">
+        <v>13</v>
+      </c>
+      <c r="F375" s="2">
+        <v>33</v>
+      </c>
+      <c r="G375" s="3">
+        <v>0</v>
+      </c>
+      <c r="H375" s="3">
+        <v>0</v>
+      </c>
+      <c r="I375" s="3">
+        <v>0</v>
+      </c>
+      <c r="J375" s="3">
+        <v>0</v>
+      </c>
+      <c r="K375" s="3">
+        <v>0</v>
+      </c>
+      <c r="L375" s="3">
+        <v>0</v>
+      </c>
+      <c r="M375" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A376" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B376">
+        <v>16</v>
+      </c>
+      <c r="C376" t="s">
+        <v>17</v>
+      </c>
+      <c r="D376" t="s">
+        <v>9</v>
+      </c>
+      <c r="E376" t="s">
+        <v>13</v>
+      </c>
+      <c r="F376" s="2">
+        <v>10</v>
+      </c>
+      <c r="G376" s="3">
+        <v>0</v>
+      </c>
+      <c r="H376" s="3">
+        <v>0</v>
+      </c>
+      <c r="I376" s="3">
+        <v>0</v>
+      </c>
+      <c r="J376" s="3">
+        <v>0</v>
+      </c>
+      <c r="K376" s="3">
+        <v>0</v>
+      </c>
+      <c r="L376" s="3">
+        <v>0</v>
+      </c>
+      <c r="M376" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A377" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B377">
+        <v>16</v>
+      </c>
+      <c r="C377" t="s">
+        <v>17</v>
+      </c>
+      <c r="D377" t="s">
+        <v>9</v>
+      </c>
+      <c r="E377" t="s">
+        <v>13</v>
+      </c>
+      <c r="F377" s="2">
+        <v>34</v>
+      </c>
+      <c r="G377" s="3">
+        <v>0</v>
+      </c>
+      <c r="H377" s="3">
+        <v>0</v>
+      </c>
+      <c r="I377" s="3">
+        <v>0</v>
+      </c>
+      <c r="J377" s="3">
+        <v>0</v>
+      </c>
+      <c r="K377" s="3">
+        <v>0</v>
+      </c>
+      <c r="L377" s="3">
+        <v>0</v>
+      </c>
+      <c r="M377" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A378" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B378">
+        <v>16</v>
+      </c>
+      <c r="C378" t="s">
+        <v>17</v>
+      </c>
+      <c r="D378" t="s">
+        <v>9</v>
+      </c>
+      <c r="E378" t="s">
+        <v>13</v>
+      </c>
+      <c r="F378" s="2">
+        <v>3</v>
+      </c>
+      <c r="G378" s="3">
+        <v>0</v>
+      </c>
+      <c r="H378" s="3">
+        <v>0</v>
+      </c>
+      <c r="I378" s="3">
+        <v>0</v>
+      </c>
+      <c r="J378" s="3">
+        <v>0</v>
+      </c>
+      <c r="K378" s="3">
+        <v>0</v>
+      </c>
+      <c r="L378" s="3">
+        <v>0</v>
+      </c>
+      <c r="M378" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A379" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B379">
+        <v>16</v>
+      </c>
+      <c r="C379" t="s">
+        <v>17</v>
+      </c>
+      <c r="D379" t="s">
+        <v>9</v>
+      </c>
+      <c r="E379" t="s">
+        <v>13</v>
+      </c>
+      <c r="F379" s="2">
+        <v>31</v>
+      </c>
+      <c r="G379" s="3">
+        <v>0</v>
+      </c>
+      <c r="H379" s="3">
+        <v>0</v>
+      </c>
+      <c r="I379" s="3">
+        <v>0</v>
+      </c>
+      <c r="J379" s="3">
+        <v>0</v>
+      </c>
+      <c r="K379" s="3">
+        <v>0</v>
+      </c>
+      <c r="L379" s="3">
+        <v>0</v>
+      </c>
+      <c r="M379" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A380" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B380">
+        <v>16</v>
+      </c>
+      <c r="C380" t="s">
+        <v>17</v>
+      </c>
+      <c r="D380" t="s">
+        <v>9</v>
+      </c>
+      <c r="E380" t="s">
+        <v>13</v>
+      </c>
+      <c r="F380" s="2">
+        <v>40</v>
+      </c>
+      <c r="G380" s="3">
+        <v>0</v>
+      </c>
+      <c r="H380" s="3">
+        <v>0</v>
+      </c>
+      <c r="I380" s="3">
+        <v>0</v>
+      </c>
+      <c r="J380" s="3">
+        <v>0</v>
+      </c>
+      <c r="K380" s="3">
+        <v>0</v>
+      </c>
+      <c r="L380" s="3">
+        <v>0</v>
+      </c>
+      <c r="M380" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A381" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B381">
+        <v>16</v>
+      </c>
+      <c r="C381" t="s">
+        <v>17</v>
+      </c>
+      <c r="D381" t="s">
+        <v>9</v>
+      </c>
+      <c r="E381" t="s">
+        <v>13</v>
+      </c>
+      <c r="F381" s="2">
+        <v>21</v>
+      </c>
+      <c r="G381" s="3">
+        <v>0</v>
+      </c>
+      <c r="H381" s="3">
+        <v>0</v>
+      </c>
+      <c r="I381" s="3">
+        <v>0</v>
+      </c>
+      <c r="J381" s="3">
+        <v>0</v>
+      </c>
+      <c r="K381" s="3">
+        <v>0</v>
+      </c>
+      <c r="L381" s="3">
+        <v>0</v>
+      </c>
+      <c r="M381" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A382" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B382">
+        <v>16</v>
+      </c>
+      <c r="C382" t="s">
+        <v>17</v>
+      </c>
+      <c r="D382" t="s">
+        <v>9</v>
+      </c>
+      <c r="E382" t="s">
+        <v>12</v>
+      </c>
+      <c r="F382" s="2">
+        <v>36</v>
+      </c>
+      <c r="G382" s="3">
+        <v>0</v>
+      </c>
+      <c r="H382" s="3">
+        <v>0</v>
+      </c>
+      <c r="I382" s="3">
+        <v>0</v>
+      </c>
+      <c r="J382" s="3">
+        <v>0</v>
+      </c>
+      <c r="K382" s="3">
+        <v>0</v>
+      </c>
+      <c r="L382" s="3">
+        <v>0</v>
+      </c>
+      <c r="M382" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A383" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B383">
+        <v>16</v>
+      </c>
+      <c r="C383" t="s">
+        <v>17</v>
+      </c>
+      <c r="D383" t="s">
+        <v>9</v>
+      </c>
+      <c r="E383" t="s">
+        <v>12</v>
+      </c>
+      <c r="F383" s="2">
+        <v>25</v>
+      </c>
+      <c r="G383" s="3">
+        <v>0</v>
+      </c>
+      <c r="H383" s="3">
+        <v>0</v>
+      </c>
+      <c r="I383" s="3">
+        <v>0</v>
+      </c>
+      <c r="J383" s="4">
+        <v>1</v>
+      </c>
+      <c r="K383" s="4">
+        <v>1</v>
+      </c>
+      <c r="L383" s="4">
+        <v>1</v>
+      </c>
+      <c r="M383" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A384" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B384">
+        <v>16</v>
+      </c>
+      <c r="C384" t="s">
+        <v>17</v>
+      </c>
+      <c r="D384" t="s">
+        <v>9</v>
+      </c>
+      <c r="E384" t="s">
+        <v>12</v>
+      </c>
+      <c r="F384" s="2">
+        <v>23</v>
+      </c>
+      <c r="G384" s="3">
+        <v>0</v>
+      </c>
+      <c r="H384" s="3">
+        <v>0</v>
+      </c>
+      <c r="I384" s="3">
+        <v>0</v>
+      </c>
+      <c r="J384" s="4">
+        <v>1</v>
+      </c>
+      <c r="K384" s="4">
+        <v>1</v>
+      </c>
+      <c r="L384" s="4">
+        <v>1</v>
+      </c>
+      <c r="M384" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A385" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B385">
+        <v>16</v>
+      </c>
+      <c r="C385" t="s">
+        <v>17</v>
+      </c>
+      <c r="D385" t="s">
+        <v>9</v>
+      </c>
+      <c r="E385" t="s">
+        <v>12</v>
+      </c>
+      <c r="F385" s="2">
+        <v>22</v>
+      </c>
+      <c r="G385" s="3">
+        <v>0</v>
+      </c>
+      <c r="H385" s="3">
+        <v>0</v>
+      </c>
+      <c r="I385" s="3">
+        <v>0</v>
+      </c>
+      <c r="J385" s="3">
+        <v>0</v>
+      </c>
+      <c r="K385" s="4">
+        <v>1</v>
+      </c>
+      <c r="L385" s="4">
+        <v>1</v>
+      </c>
+      <c r="M385" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A386" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B386">
+        <v>16</v>
+      </c>
+      <c r="C386" t="s">
+        <v>17</v>
+      </c>
+      <c r="D386" t="s">
+        <v>9</v>
+      </c>
+      <c r="E386" t="s">
+        <v>12</v>
+      </c>
+      <c r="F386" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G386" s="3">
+        <v>0</v>
+      </c>
+      <c r="H386" s="3">
+        <v>0</v>
+      </c>
+      <c r="I386" s="4">
+        <v>1</v>
+      </c>
+      <c r="J386" s="4">
+        <v>1</v>
+      </c>
+      <c r="K386" s="4">
+        <v>1</v>
+      </c>
+      <c r="L386" s="4">
+        <v>1</v>
+      </c>
+      <c r="M386" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A387" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B387">
+        <v>16</v>
+      </c>
+      <c r="C387" t="s">
+        <v>17</v>
+      </c>
+      <c r="D387" t="s">
+        <v>9</v>
+      </c>
+      <c r="E387" t="s">
+        <v>12</v>
+      </c>
+      <c r="F387" s="2">
+        <v>1</v>
+      </c>
+      <c r="G387" s="3">
+        <v>0</v>
+      </c>
+      <c r="H387" s="3">
+        <v>0</v>
+      </c>
+      <c r="I387" s="3">
+        <v>0</v>
+      </c>
+      <c r="J387" s="4">
+        <v>1</v>
+      </c>
+      <c r="K387" s="4">
+        <v>1</v>
+      </c>
+      <c r="L387" s="4">
+        <v>1</v>
+      </c>
+      <c r="M387" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A388" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B388">
+        <v>16</v>
+      </c>
+      <c r="C388" t="s">
+        <v>17</v>
+      </c>
+      <c r="D388" t="s">
+        <v>9</v>
+      </c>
+      <c r="E388" t="s">
+        <v>12</v>
+      </c>
+      <c r="F388" s="2">
+        <v>19</v>
+      </c>
+      <c r="G388" s="3">
+        <v>0</v>
+      </c>
+      <c r="H388" s="3">
+        <v>0</v>
+      </c>
+      <c r="I388" s="3">
+        <v>0</v>
+      </c>
+      <c r="J388" s="4">
+        <v>1</v>
+      </c>
+      <c r="K388" s="4">
+        <v>1</v>
+      </c>
+      <c r="L388" s="4">
+        <v>1</v>
+      </c>
+      <c r="M388" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A389" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B389">
+        <v>16</v>
+      </c>
+      <c r="C389" t="s">
+        <v>17</v>
+      </c>
+      <c r="D389" t="s">
+        <v>9</v>
+      </c>
+      <c r="E389" t="s">
+        <v>12</v>
+      </c>
+      <c r="F389" s="2">
+        <v>14</v>
+      </c>
+      <c r="G389" s="3">
+        <v>0</v>
+      </c>
+      <c r="H389" s="3">
+        <v>0</v>
+      </c>
+      <c r="I389" s="4">
+        <v>1</v>
+      </c>
+      <c r="J389" s="4">
+        <v>1</v>
+      </c>
+      <c r="K389" s="4">
+        <v>1</v>
+      </c>
+      <c r="L389" s="4">
+        <v>1</v>
+      </c>
+      <c r="M389" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A390" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B390">
+        <v>16</v>
+      </c>
+      <c r="C390" t="s">
+        <v>17</v>
+      </c>
+      <c r="D390" t="s">
+        <v>9</v>
+      </c>
+      <c r="E390" t="s">
+        <v>12</v>
+      </c>
+      <c r="F390" s="2">
+        <v>28</v>
+      </c>
+      <c r="G390" s="3">
+        <v>0</v>
+      </c>
+      <c r="H390" s="4">
+        <v>1</v>
+      </c>
+      <c r="I390" s="4">
+        <v>1</v>
+      </c>
+      <c r="J390" s="4">
+        <v>1</v>
+      </c>
+      <c r="K390" s="4">
+        <v>1</v>
+      </c>
+      <c r="L390" s="4">
+        <v>1</v>
+      </c>
+      <c r="M390" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A391" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B391">
+        <v>16</v>
+      </c>
+      <c r="C391" t="s">
+        <v>17</v>
+      </c>
+      <c r="D391" t="s">
+        <v>9</v>
+      </c>
+      <c r="E391" t="s">
+        <v>12</v>
+      </c>
+      <c r="F391" s="2">
+        <v>4</v>
+      </c>
+      <c r="G391" s="3">
+        <v>0</v>
+      </c>
+      <c r="H391" s="3">
+        <v>0</v>
+      </c>
+      <c r="I391" s="4">
+        <v>1</v>
+      </c>
+      <c r="J391" s="4">
+        <v>1</v>
+      </c>
+      <c r="K391" s="4">
+        <v>1</v>
+      </c>
+      <c r="L391" s="4">
+        <v>1</v>
+      </c>
+      <c r="M391" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A392" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B392">
+        <v>16</v>
+      </c>
+      <c r="C392" t="s">
+        <v>17</v>
+      </c>
+      <c r="D392" t="s">
+        <v>9</v>
+      </c>
+      <c r="E392" t="s">
+        <v>12</v>
+      </c>
+      <c r="F392" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G392" s="3">
+        <v>0</v>
+      </c>
+      <c r="H392" s="3">
+        <v>0</v>
+      </c>
+      <c r="I392" s="3">
+        <v>0</v>
+      </c>
+      <c r="J392" s="3">
+        <v>0</v>
+      </c>
+      <c r="K392" s="3">
+        <v>0</v>
+      </c>
+      <c r="L392" s="4">
+        <v>1</v>
+      </c>
+      <c r="M392" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A393" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B393">
+        <v>16</v>
+      </c>
+      <c r="C393" t="s">
+        <v>17</v>
+      </c>
+      <c r="D393" t="s">
+        <v>9</v>
+      </c>
+      <c r="E393" t="s">
+        <v>12</v>
+      </c>
+      <c r="F393" s="2">
+        <v>37</v>
+      </c>
+      <c r="G393" s="3">
+        <v>0</v>
+      </c>
+      <c r="H393" s="3">
+        <v>0</v>
+      </c>
+      <c r="I393" s="3">
+        <v>0</v>
+      </c>
+      <c r="J393" s="3">
+        <v>0</v>
+      </c>
+      <c r="K393" s="4">
+        <v>1</v>
+      </c>
+      <c r="L393" s="4">
+        <v>1</v>
+      </c>
+      <c r="M393" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A394" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B394">
+        <v>16</v>
+      </c>
+      <c r="C394" t="s">
+        <v>17</v>
+      </c>
+      <c r="D394" t="s">
+        <v>9</v>
+      </c>
+      <c r="E394" t="s">
+        <v>12</v>
+      </c>
+      <c r="F394" s="2">
+        <v>20</v>
+      </c>
+      <c r="G394" s="3">
+        <v>0</v>
+      </c>
+      <c r="H394" s="3">
+        <v>0</v>
+      </c>
+      <c r="I394" s="4">
+        <v>1</v>
+      </c>
+      <c r="J394" s="4">
+        <v>1</v>
+      </c>
+      <c r="K394" s="4">
+        <v>1</v>
+      </c>
+      <c r="L394" s="4">
+        <v>1</v>
+      </c>
+      <c r="M394" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A395" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B395">
+        <v>16</v>
+      </c>
+      <c r="C395" t="s">
+        <v>17</v>
+      </c>
+      <c r="D395" t="s">
+        <v>9</v>
+      </c>
+      <c r="E395" t="s">
+        <v>12</v>
+      </c>
+      <c r="F395" s="2">
+        <v>6</v>
+      </c>
+      <c r="G395" s="3">
+        <v>0</v>
+      </c>
+      <c r="H395" s="3">
+        <v>0</v>
+      </c>
+      <c r="I395" s="3">
+        <v>0</v>
+      </c>
+      <c r="J395" s="3">
+        <v>0</v>
+      </c>
+      <c r="K395" s="3">
+        <v>0</v>
+      </c>
+      <c r="L395" s="4">
+        <v>1</v>
+      </c>
+      <c r="M395" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A396" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B396">
+        <v>16</v>
+      </c>
+      <c r="C396" t="s">
+        <v>17</v>
+      </c>
+      <c r="D396" t="s">
+        <v>9</v>
+      </c>
+      <c r="E396" t="s">
+        <v>12</v>
+      </c>
+      <c r="F396" s="2">
+        <v>12</v>
+      </c>
+      <c r="G396" s="3">
+        <v>0</v>
+      </c>
+      <c r="H396" s="3">
+        <v>0</v>
+      </c>
+      <c r="I396" s="3">
+        <v>0</v>
+      </c>
+      <c r="J396" s="3">
+        <v>0</v>
+      </c>
+      <c r="K396" s="3">
+        <v>0</v>
+      </c>
+      <c r="L396" s="3">
+        <v>0</v>
+      </c>
+      <c r="M396" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A397" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B397">
+        <v>16</v>
+      </c>
+      <c r="C397" t="s">
+        <v>17</v>
+      </c>
+      <c r="D397" t="s">
+        <v>9</v>
+      </c>
+      <c r="E397" t="s">
+        <v>12</v>
+      </c>
+      <c r="F397" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G397" s="3">
+        <v>0</v>
+      </c>
+      <c r="H397" s="3">
+        <v>0</v>
+      </c>
+      <c r="I397" s="3">
+        <v>0</v>
+      </c>
+      <c r="J397" s="3">
+        <v>0</v>
+      </c>
+      <c r="K397" s="3">
+        <v>0</v>
+      </c>
+      <c r="L397" s="3">
+        <v>0</v>
+      </c>
+      <c r="M397" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A398" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B398">
+        <v>16</v>
+      </c>
+      <c r="C398" t="s">
+        <v>17</v>
+      </c>
+      <c r="D398" t="s">
+        <v>9</v>
+      </c>
+      <c r="E398" t="s">
+        <v>12</v>
+      </c>
+      <c r="F398" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G398" s="3">
+        <v>0</v>
+      </c>
+      <c r="H398" s="3">
+        <v>0</v>
+      </c>
+      <c r="I398" s="3">
+        <v>0</v>
+      </c>
+      <c r="J398" s="3">
+        <v>0</v>
+      </c>
+      <c r="K398" s="4">
+        <v>1</v>
+      </c>
+      <c r="L398" s="4">
+        <v>1</v>
+      </c>
+      <c r="M398" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A399" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B399">
+        <v>16</v>
+      </c>
+      <c r="C399" t="s">
+        <v>17</v>
+      </c>
+      <c r="D399" t="s">
+        <v>9</v>
+      </c>
+      <c r="E399" t="s">
+        <v>12</v>
+      </c>
+      <c r="F399" s="2">
+        <v>6</v>
+      </c>
+      <c r="G399" s="3">
+        <v>0</v>
+      </c>
+      <c r="H399" s="3">
+        <v>0</v>
+      </c>
+      <c r="I399" s="4">
+        <v>1</v>
+      </c>
+      <c r="J399" s="4">
+        <v>1</v>
+      </c>
+      <c r="K399" s="4">
+        <v>1</v>
+      </c>
+      <c r="L399" s="4">
+        <v>1</v>
+      </c>
+      <c r="M399" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A400" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B400">
+        <v>16</v>
+      </c>
+      <c r="C400" t="s">
+        <v>17</v>
+      </c>
+      <c r="D400" t="s">
+        <v>9</v>
+      </c>
+      <c r="E400" t="s">
+        <v>12</v>
+      </c>
+      <c r="F400" s="2">
+        <v>37</v>
+      </c>
+      <c r="G400" s="3">
+        <v>0</v>
+      </c>
+      <c r="H400" s="3">
+        <v>0</v>
+      </c>
+      <c r="I400" s="3">
+        <v>0</v>
+      </c>
+      <c r="J400" s="3">
+        <v>0</v>
+      </c>
+      <c r="K400" s="3">
+        <v>0</v>
+      </c>
+      <c r="L400" s="3">
+        <v>0</v>
+      </c>
+      <c r="M400" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A401" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B401">
+        <v>16</v>
+      </c>
+      <c r="C401" t="s">
+        <v>17</v>
+      </c>
+      <c r="D401" t="s">
+        <v>9</v>
+      </c>
+      <c r="E401" t="s">
+        <v>12</v>
+      </c>
+      <c r="F401" s="2">
+        <v>4</v>
+      </c>
+      <c r="G401" s="3">
+        <v>0</v>
+      </c>
+      <c r="H401" s="3">
+        <v>0</v>
+      </c>
+      <c r="I401" s="4">
+        <v>1</v>
+      </c>
+      <c r="J401" s="4">
+        <v>1</v>
+      </c>
+      <c r="K401" s="4">
+        <v>1</v>
+      </c>
+      <c r="L401" s="4">
+        <v>1</v>
+      </c>
+      <c r="M401" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 10/21 lab survival analysis
</commit_message>
<xml_diff>
--- a/data/survival/lab_survival/lab_survival.xlsx
+++ b/data/survival/lab_survival/lab_survival.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/survival/lab_survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6192593F-75EF-0845-B468-C3496A1A0815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E814CF3-9429-1345-8DDE-37808D148692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33880" yWindow="-1460" windowWidth="20700" windowHeight="18300" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
+    <workbookView xWindow="-31460" yWindow="-1460" windowWidth="20700" windowHeight="18300" xr2:uid="{ADDFC8C8-487B-804E-A169-6B1708E625F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Effort B</t>
+  </si>
+  <si>
+    <t>Effort E</t>
+  </si>
+  <si>
+    <t>Temperature Treated</t>
+  </si>
+  <si>
+    <t>Temperature Control</t>
   </si>
 </sst>
 </file>
@@ -483,11 +492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7ACAA-9959-8D4E-8E48-CFF679AAAAC5}">
-  <dimension ref="A1:N401"/>
+  <dimension ref="A1:N481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J389" sqref="J389"/>
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I467" sqref="I467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16934,6 +16943,3286 @@
         <v>1</v>
       </c>
     </row>
+    <row r="402" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A402" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B402">
+        <v>20</v>
+      </c>
+      <c r="C402" t="s">
+        <v>18</v>
+      </c>
+      <c r="D402" t="s">
+        <v>19</v>
+      </c>
+      <c r="E402" t="s">
+        <v>13</v>
+      </c>
+      <c r="F402" s="2">
+        <v>19</v>
+      </c>
+      <c r="G402" s="3">
+        <v>0</v>
+      </c>
+      <c r="H402" s="3">
+        <v>0</v>
+      </c>
+      <c r="I402" s="3">
+        <v>0</v>
+      </c>
+      <c r="J402" s="3">
+        <v>0</v>
+      </c>
+      <c r="K402" s="3">
+        <v>0</v>
+      </c>
+      <c r="L402" s="3">
+        <v>0</v>
+      </c>
+      <c r="M402" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A403" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B403">
+        <v>20</v>
+      </c>
+      <c r="C403" t="s">
+        <v>18</v>
+      </c>
+      <c r="D403" t="s">
+        <v>19</v>
+      </c>
+      <c r="E403" t="s">
+        <v>13</v>
+      </c>
+      <c r="F403" s="2">
+        <v>4</v>
+      </c>
+      <c r="G403" s="3">
+        <v>0</v>
+      </c>
+      <c r="H403" s="3">
+        <v>0</v>
+      </c>
+      <c r="I403" s="3">
+        <v>0</v>
+      </c>
+      <c r="J403" s="3">
+        <v>0</v>
+      </c>
+      <c r="K403" s="3">
+        <v>0</v>
+      </c>
+      <c r="L403" s="3">
+        <v>0</v>
+      </c>
+      <c r="M403" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A404" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B404">
+        <v>20</v>
+      </c>
+      <c r="C404" t="s">
+        <v>18</v>
+      </c>
+      <c r="D404" t="s">
+        <v>19</v>
+      </c>
+      <c r="E404" t="s">
+        <v>13</v>
+      </c>
+      <c r="F404" s="2">
+        <v>8</v>
+      </c>
+      <c r="G404" s="3">
+        <v>0</v>
+      </c>
+      <c r="H404" s="3">
+        <v>0</v>
+      </c>
+      <c r="I404" s="3">
+        <v>0</v>
+      </c>
+      <c r="J404" s="3">
+        <v>0</v>
+      </c>
+      <c r="K404" s="3">
+        <v>0</v>
+      </c>
+      <c r="L404" s="3">
+        <v>0</v>
+      </c>
+      <c r="M404" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A405" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B405">
+        <v>20</v>
+      </c>
+      <c r="C405" t="s">
+        <v>18</v>
+      </c>
+      <c r="D405" t="s">
+        <v>19</v>
+      </c>
+      <c r="E405" t="s">
+        <v>13</v>
+      </c>
+      <c r="F405" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G405" s="3">
+        <v>0</v>
+      </c>
+      <c r="H405" s="3">
+        <v>0</v>
+      </c>
+      <c r="I405" s="3">
+        <v>0</v>
+      </c>
+      <c r="J405" s="3">
+        <v>0</v>
+      </c>
+      <c r="K405" s="3">
+        <v>0</v>
+      </c>
+      <c r="L405" s="3">
+        <v>0</v>
+      </c>
+      <c r="M405" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A406" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B406">
+        <v>20</v>
+      </c>
+      <c r="C406" t="s">
+        <v>18</v>
+      </c>
+      <c r="D406" t="s">
+        <v>19</v>
+      </c>
+      <c r="E406" t="s">
+        <v>13</v>
+      </c>
+      <c r="F406" s="2">
+        <v>19</v>
+      </c>
+      <c r="G406" s="3">
+        <v>0</v>
+      </c>
+      <c r="H406" s="3">
+        <v>0</v>
+      </c>
+      <c r="I406" s="3">
+        <v>0</v>
+      </c>
+      <c r="J406" s="3">
+        <v>0</v>
+      </c>
+      <c r="K406" s="3">
+        <v>0</v>
+      </c>
+      <c r="L406" s="3">
+        <v>0</v>
+      </c>
+      <c r="M406" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A407" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B407">
+        <v>20</v>
+      </c>
+      <c r="C407" t="s">
+        <v>18</v>
+      </c>
+      <c r="D407" t="s">
+        <v>19</v>
+      </c>
+      <c r="E407" t="s">
+        <v>13</v>
+      </c>
+      <c r="F407" s="2">
+        <v>8</v>
+      </c>
+      <c r="G407" s="3">
+        <v>0</v>
+      </c>
+      <c r="H407" s="3">
+        <v>0</v>
+      </c>
+      <c r="I407" s="3">
+        <v>0</v>
+      </c>
+      <c r="J407" s="3">
+        <v>0</v>
+      </c>
+      <c r="K407" s="3">
+        <v>0</v>
+      </c>
+      <c r="L407" s="3">
+        <v>0</v>
+      </c>
+      <c r="M407" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A408" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B408">
+        <v>20</v>
+      </c>
+      <c r="C408" t="s">
+        <v>18</v>
+      </c>
+      <c r="D408" t="s">
+        <v>19</v>
+      </c>
+      <c r="E408" t="s">
+        <v>13</v>
+      </c>
+      <c r="F408" s="2">
+        <v>2</v>
+      </c>
+      <c r="G408" s="3">
+        <v>0</v>
+      </c>
+      <c r="H408" s="3">
+        <v>0</v>
+      </c>
+      <c r="I408" s="3">
+        <v>0</v>
+      </c>
+      <c r="J408" s="3">
+        <v>0</v>
+      </c>
+      <c r="K408" s="3">
+        <v>0</v>
+      </c>
+      <c r="L408" s="3">
+        <v>0</v>
+      </c>
+      <c r="M408" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A409" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B409">
+        <v>20</v>
+      </c>
+      <c r="C409" t="s">
+        <v>18</v>
+      </c>
+      <c r="D409" t="s">
+        <v>19</v>
+      </c>
+      <c r="E409" t="s">
+        <v>13</v>
+      </c>
+      <c r="F409" s="2">
+        <v>23</v>
+      </c>
+      <c r="G409" s="3">
+        <v>0</v>
+      </c>
+      <c r="H409" s="3">
+        <v>0</v>
+      </c>
+      <c r="I409" s="3">
+        <v>0</v>
+      </c>
+      <c r="J409" s="3">
+        <v>0</v>
+      </c>
+      <c r="K409" s="3">
+        <v>0</v>
+      </c>
+      <c r="L409" s="3">
+        <v>0</v>
+      </c>
+      <c r="M409" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A410" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B410">
+        <v>20</v>
+      </c>
+      <c r="C410" t="s">
+        <v>18</v>
+      </c>
+      <c r="D410" t="s">
+        <v>19</v>
+      </c>
+      <c r="E410" t="s">
+        <v>13</v>
+      </c>
+      <c r="F410" s="2">
+        <v>24</v>
+      </c>
+      <c r="G410" s="3">
+        <v>0</v>
+      </c>
+      <c r="H410" s="3">
+        <v>0</v>
+      </c>
+      <c r="I410" s="3">
+        <v>0</v>
+      </c>
+      <c r="J410" s="3">
+        <v>0</v>
+      </c>
+      <c r="K410" s="3">
+        <v>0</v>
+      </c>
+      <c r="L410" s="3">
+        <v>0</v>
+      </c>
+      <c r="M410" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A411" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B411">
+        <v>20</v>
+      </c>
+      <c r="C411" t="s">
+        <v>18</v>
+      </c>
+      <c r="D411" t="s">
+        <v>19</v>
+      </c>
+      <c r="E411" t="s">
+        <v>13</v>
+      </c>
+      <c r="F411" s="2">
+        <v>5</v>
+      </c>
+      <c r="G411" s="3">
+        <v>0</v>
+      </c>
+      <c r="H411" s="3">
+        <v>0</v>
+      </c>
+      <c r="I411" s="3">
+        <v>0</v>
+      </c>
+      <c r="J411" s="3">
+        <v>0</v>
+      </c>
+      <c r="K411" s="3">
+        <v>0</v>
+      </c>
+      <c r="L411" s="3">
+        <v>0</v>
+      </c>
+      <c r="M411" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A412" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B412">
+        <v>20</v>
+      </c>
+      <c r="C412" t="s">
+        <v>18</v>
+      </c>
+      <c r="D412" t="s">
+        <v>19</v>
+      </c>
+      <c r="E412" t="s">
+        <v>13</v>
+      </c>
+      <c r="F412" s="2">
+        <v>37</v>
+      </c>
+      <c r="G412" s="3">
+        <v>0</v>
+      </c>
+      <c r="H412" s="3">
+        <v>0</v>
+      </c>
+      <c r="I412" s="3">
+        <v>0</v>
+      </c>
+      <c r="J412" s="3">
+        <v>0</v>
+      </c>
+      <c r="K412" s="3">
+        <v>0</v>
+      </c>
+      <c r="L412" s="3">
+        <v>0</v>
+      </c>
+      <c r="M412" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A413" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B413">
+        <v>20</v>
+      </c>
+      <c r="C413" t="s">
+        <v>18</v>
+      </c>
+      <c r="D413" t="s">
+        <v>19</v>
+      </c>
+      <c r="E413" t="s">
+        <v>13</v>
+      </c>
+      <c r="F413" s="2">
+        <v>40</v>
+      </c>
+      <c r="G413" s="3">
+        <v>0</v>
+      </c>
+      <c r="H413" s="3">
+        <v>0</v>
+      </c>
+      <c r="I413" s="3">
+        <v>0</v>
+      </c>
+      <c r="J413" s="3">
+        <v>0</v>
+      </c>
+      <c r="K413" s="3">
+        <v>0</v>
+      </c>
+      <c r="L413" s="3">
+        <v>0</v>
+      </c>
+      <c r="M413" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A414" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B414">
+        <v>20</v>
+      </c>
+      <c r="C414" t="s">
+        <v>18</v>
+      </c>
+      <c r="D414" t="s">
+        <v>19</v>
+      </c>
+      <c r="E414" t="s">
+        <v>13</v>
+      </c>
+      <c r="F414" s="2">
+        <v>2</v>
+      </c>
+      <c r="G414" s="3">
+        <v>0</v>
+      </c>
+      <c r="H414" s="3">
+        <v>0</v>
+      </c>
+      <c r="I414" s="3">
+        <v>0</v>
+      </c>
+      <c r="J414" s="3">
+        <v>0</v>
+      </c>
+      <c r="K414" s="3">
+        <v>0</v>
+      </c>
+      <c r="L414" s="3">
+        <v>0</v>
+      </c>
+      <c r="M414" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A415" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B415">
+        <v>20</v>
+      </c>
+      <c r="C415" t="s">
+        <v>18</v>
+      </c>
+      <c r="D415" t="s">
+        <v>19</v>
+      </c>
+      <c r="E415" t="s">
+        <v>13</v>
+      </c>
+      <c r="F415" s="2">
+        <v>38</v>
+      </c>
+      <c r="G415" s="3">
+        <v>0</v>
+      </c>
+      <c r="H415" s="3">
+        <v>0</v>
+      </c>
+      <c r="I415" s="3">
+        <v>0</v>
+      </c>
+      <c r="J415" s="3">
+        <v>0</v>
+      </c>
+      <c r="K415" s="3">
+        <v>0</v>
+      </c>
+      <c r="L415" s="3">
+        <v>0</v>
+      </c>
+      <c r="M415" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A416" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B416">
+        <v>20</v>
+      </c>
+      <c r="C416" t="s">
+        <v>18</v>
+      </c>
+      <c r="D416" t="s">
+        <v>19</v>
+      </c>
+      <c r="E416" t="s">
+        <v>13</v>
+      </c>
+      <c r="F416" s="2">
+        <v>20</v>
+      </c>
+      <c r="G416" s="3">
+        <v>0</v>
+      </c>
+      <c r="H416" s="3">
+        <v>0</v>
+      </c>
+      <c r="I416" s="3">
+        <v>0</v>
+      </c>
+      <c r="J416" s="3">
+        <v>0</v>
+      </c>
+      <c r="K416" s="3">
+        <v>0</v>
+      </c>
+      <c r="L416" s="3">
+        <v>0</v>
+      </c>
+      <c r="M416" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A417" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B417">
+        <v>20</v>
+      </c>
+      <c r="C417" t="s">
+        <v>18</v>
+      </c>
+      <c r="D417" t="s">
+        <v>19</v>
+      </c>
+      <c r="E417" t="s">
+        <v>13</v>
+      </c>
+      <c r="F417" s="2">
+        <v>24</v>
+      </c>
+      <c r="G417" s="3">
+        <v>0</v>
+      </c>
+      <c r="H417" s="3">
+        <v>0</v>
+      </c>
+      <c r="I417" s="3">
+        <v>0</v>
+      </c>
+      <c r="J417" s="3">
+        <v>0</v>
+      </c>
+      <c r="K417" s="3">
+        <v>0</v>
+      </c>
+      <c r="L417" s="3">
+        <v>0</v>
+      </c>
+      <c r="M417" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A418" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B418">
+        <v>20</v>
+      </c>
+      <c r="C418" t="s">
+        <v>18</v>
+      </c>
+      <c r="D418" t="s">
+        <v>19</v>
+      </c>
+      <c r="E418" t="s">
+        <v>13</v>
+      </c>
+      <c r="F418" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G418" s="3">
+        <v>0</v>
+      </c>
+      <c r="H418" s="3">
+        <v>0</v>
+      </c>
+      <c r="I418" s="3">
+        <v>0</v>
+      </c>
+      <c r="J418" s="3">
+        <v>0</v>
+      </c>
+      <c r="K418" s="3">
+        <v>0</v>
+      </c>
+      <c r="L418" s="3">
+        <v>0</v>
+      </c>
+      <c r="M418" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A419" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B419">
+        <v>20</v>
+      </c>
+      <c r="C419" t="s">
+        <v>18</v>
+      </c>
+      <c r="D419" t="s">
+        <v>19</v>
+      </c>
+      <c r="E419" t="s">
+        <v>13</v>
+      </c>
+      <c r="F419" s="2">
+        <v>15</v>
+      </c>
+      <c r="G419" s="3">
+        <v>0</v>
+      </c>
+      <c r="H419" s="3">
+        <v>0</v>
+      </c>
+      <c r="I419" s="3">
+        <v>0</v>
+      </c>
+      <c r="J419" s="3">
+        <v>0</v>
+      </c>
+      <c r="K419" s="3">
+        <v>0</v>
+      </c>
+      <c r="L419" s="3">
+        <v>0</v>
+      </c>
+      <c r="M419" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A420" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B420">
+        <v>20</v>
+      </c>
+      <c r="C420" t="s">
+        <v>18</v>
+      </c>
+      <c r="D420" t="s">
+        <v>19</v>
+      </c>
+      <c r="E420" t="s">
+        <v>13</v>
+      </c>
+      <c r="F420" s="2">
+        <v>16</v>
+      </c>
+      <c r="G420" s="3">
+        <v>0</v>
+      </c>
+      <c r="H420" s="3">
+        <v>0</v>
+      </c>
+      <c r="I420" s="3">
+        <v>0</v>
+      </c>
+      <c r="J420" s="3">
+        <v>0</v>
+      </c>
+      <c r="K420" s="3">
+        <v>0</v>
+      </c>
+      <c r="L420" s="3">
+        <v>0</v>
+      </c>
+      <c r="M420" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A421" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B421">
+        <v>20</v>
+      </c>
+      <c r="C421" t="s">
+        <v>18</v>
+      </c>
+      <c r="D421" t="s">
+        <v>19</v>
+      </c>
+      <c r="E421" t="s">
+        <v>13</v>
+      </c>
+      <c r="F421" s="2">
+        <v>33</v>
+      </c>
+      <c r="G421" s="3">
+        <v>0</v>
+      </c>
+      <c r="H421" s="3">
+        <v>0</v>
+      </c>
+      <c r="I421" s="3">
+        <v>0</v>
+      </c>
+      <c r="J421" s="3">
+        <v>0</v>
+      </c>
+      <c r="K421" s="3">
+        <v>0</v>
+      </c>
+      <c r="L421" s="3">
+        <v>0</v>
+      </c>
+      <c r="M421" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A422" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B422">
+        <v>20</v>
+      </c>
+      <c r="C422" t="s">
+        <v>18</v>
+      </c>
+      <c r="D422" t="s">
+        <v>19</v>
+      </c>
+      <c r="E422" t="s">
+        <v>12</v>
+      </c>
+      <c r="F422" s="2">
+        <v>3</v>
+      </c>
+      <c r="G422" s="3">
+        <v>0</v>
+      </c>
+      <c r="H422" s="3">
+        <v>0</v>
+      </c>
+      <c r="I422" s="3">
+        <v>0</v>
+      </c>
+      <c r="J422" s="4">
+        <v>1</v>
+      </c>
+      <c r="K422" s="4">
+        <v>1</v>
+      </c>
+      <c r="L422" s="4">
+        <v>1</v>
+      </c>
+      <c r="M422" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A423" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B423">
+        <v>20</v>
+      </c>
+      <c r="C423" t="s">
+        <v>18</v>
+      </c>
+      <c r="D423" t="s">
+        <v>19</v>
+      </c>
+      <c r="E423" t="s">
+        <v>12</v>
+      </c>
+      <c r="F423" s="2">
+        <v>31</v>
+      </c>
+      <c r="G423" s="3">
+        <v>0</v>
+      </c>
+      <c r="H423" s="3">
+        <v>0</v>
+      </c>
+      <c r="I423" s="4">
+        <v>1</v>
+      </c>
+      <c r="J423" s="4">
+        <v>1</v>
+      </c>
+      <c r="K423" s="4">
+        <v>1</v>
+      </c>
+      <c r="L423" s="4">
+        <v>1</v>
+      </c>
+      <c r="M423" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A424" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B424">
+        <v>20</v>
+      </c>
+      <c r="C424" t="s">
+        <v>18</v>
+      </c>
+      <c r="D424" t="s">
+        <v>19</v>
+      </c>
+      <c r="E424" t="s">
+        <v>12</v>
+      </c>
+      <c r="F424" s="2">
+        <v>6</v>
+      </c>
+      <c r="G424" s="3">
+        <v>0</v>
+      </c>
+      <c r="H424" s="3">
+        <v>0</v>
+      </c>
+      <c r="I424" s="4">
+        <v>1</v>
+      </c>
+      <c r="J424" s="4">
+        <v>1</v>
+      </c>
+      <c r="K424" s="4">
+        <v>1</v>
+      </c>
+      <c r="L424" s="4">
+        <v>1</v>
+      </c>
+      <c r="M424" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A425" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B425">
+        <v>20</v>
+      </c>
+      <c r="C425" t="s">
+        <v>18</v>
+      </c>
+      <c r="D425" t="s">
+        <v>19</v>
+      </c>
+      <c r="E425" t="s">
+        <v>12</v>
+      </c>
+      <c r="F425" s="2">
+        <v>16</v>
+      </c>
+      <c r="G425" s="3">
+        <v>0</v>
+      </c>
+      <c r="H425" s="3">
+        <v>0</v>
+      </c>
+      <c r="I425" s="4">
+        <v>1</v>
+      </c>
+      <c r="J425" s="4">
+        <v>1</v>
+      </c>
+      <c r="K425" s="4">
+        <v>1</v>
+      </c>
+      <c r="L425" s="4">
+        <v>1</v>
+      </c>
+      <c r="M425" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A426" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B426">
+        <v>20</v>
+      </c>
+      <c r="C426" t="s">
+        <v>18</v>
+      </c>
+      <c r="D426" t="s">
+        <v>19</v>
+      </c>
+      <c r="E426" t="s">
+        <v>12</v>
+      </c>
+      <c r="F426" s="2">
+        <v>14</v>
+      </c>
+      <c r="G426" s="3">
+        <v>0</v>
+      </c>
+      <c r="H426" s="3">
+        <v>0</v>
+      </c>
+      <c r="I426" s="4">
+        <v>1</v>
+      </c>
+      <c r="J426" s="4">
+        <v>1</v>
+      </c>
+      <c r="K426" s="4">
+        <v>1</v>
+      </c>
+      <c r="L426" s="4">
+        <v>1</v>
+      </c>
+      <c r="M426" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A427" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B427">
+        <v>20</v>
+      </c>
+      <c r="C427" t="s">
+        <v>18</v>
+      </c>
+      <c r="D427" t="s">
+        <v>19</v>
+      </c>
+      <c r="E427" t="s">
+        <v>12</v>
+      </c>
+      <c r="F427" s="2">
+        <v>36</v>
+      </c>
+      <c r="G427" s="3">
+        <v>0</v>
+      </c>
+      <c r="H427" s="3">
+        <v>0</v>
+      </c>
+      <c r="I427" s="4">
+        <v>1</v>
+      </c>
+      <c r="J427" s="4">
+        <v>1</v>
+      </c>
+      <c r="K427" s="4">
+        <v>1</v>
+      </c>
+      <c r="L427" s="4">
+        <v>1</v>
+      </c>
+      <c r="M427" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A428" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B428">
+        <v>20</v>
+      </c>
+      <c r="C428" t="s">
+        <v>18</v>
+      </c>
+      <c r="D428" t="s">
+        <v>19</v>
+      </c>
+      <c r="E428" t="s">
+        <v>12</v>
+      </c>
+      <c r="F428" s="2">
+        <v>4</v>
+      </c>
+      <c r="G428" s="3">
+        <v>0</v>
+      </c>
+      <c r="H428" s="4">
+        <v>1</v>
+      </c>
+      <c r="I428" s="4">
+        <v>1</v>
+      </c>
+      <c r="J428" s="4">
+        <v>1</v>
+      </c>
+      <c r="K428" s="4">
+        <v>1</v>
+      </c>
+      <c r="L428" s="4">
+        <v>1</v>
+      </c>
+      <c r="M428" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A429" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B429">
+        <v>20</v>
+      </c>
+      <c r="C429" t="s">
+        <v>18</v>
+      </c>
+      <c r="D429" t="s">
+        <v>19</v>
+      </c>
+      <c r="E429" t="s">
+        <v>12</v>
+      </c>
+      <c r="F429" s="2">
+        <v>34</v>
+      </c>
+      <c r="G429" s="3">
+        <v>0</v>
+      </c>
+      <c r="H429" s="3">
+        <v>0</v>
+      </c>
+      <c r="I429" s="4">
+        <v>1</v>
+      </c>
+      <c r="J429" s="4">
+        <v>1</v>
+      </c>
+      <c r="K429" s="4">
+        <v>1</v>
+      </c>
+      <c r="L429" s="4">
+        <v>1</v>
+      </c>
+      <c r="M429" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A430" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B430">
+        <v>20</v>
+      </c>
+      <c r="C430" t="s">
+        <v>18</v>
+      </c>
+      <c r="D430" t="s">
+        <v>19</v>
+      </c>
+      <c r="E430" t="s">
+        <v>12</v>
+      </c>
+      <c r="F430" s="2">
+        <v>1</v>
+      </c>
+      <c r="G430" s="3">
+        <v>0</v>
+      </c>
+      <c r="H430" s="3">
+        <v>0</v>
+      </c>
+      <c r="I430" s="3">
+        <v>0</v>
+      </c>
+      <c r="J430" s="4">
+        <v>1</v>
+      </c>
+      <c r="K430" s="4">
+        <v>1</v>
+      </c>
+      <c r="L430" s="4">
+        <v>1</v>
+      </c>
+      <c r="M430" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A431" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B431">
+        <v>20</v>
+      </c>
+      <c r="C431" t="s">
+        <v>18</v>
+      </c>
+      <c r="D431" t="s">
+        <v>19</v>
+      </c>
+      <c r="E431" t="s">
+        <v>12</v>
+      </c>
+      <c r="F431" s="2">
+        <v>26</v>
+      </c>
+      <c r="G431" s="3">
+        <v>0</v>
+      </c>
+      <c r="H431" s="3">
+        <v>0</v>
+      </c>
+      <c r="I431" s="3">
+        <v>0</v>
+      </c>
+      <c r="J431" s="3">
+        <v>0</v>
+      </c>
+      <c r="K431" s="4">
+        <v>1</v>
+      </c>
+      <c r="L431" s="4">
+        <v>1</v>
+      </c>
+      <c r="M431" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A432" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B432">
+        <v>20</v>
+      </c>
+      <c r="C432" t="s">
+        <v>18</v>
+      </c>
+      <c r="D432" t="s">
+        <v>19</v>
+      </c>
+      <c r="E432" t="s">
+        <v>12</v>
+      </c>
+      <c r="F432" s="2">
+        <v>14</v>
+      </c>
+      <c r="G432" s="3">
+        <v>0</v>
+      </c>
+      <c r="H432" s="4">
+        <v>1</v>
+      </c>
+      <c r="I432" s="4">
+        <v>1</v>
+      </c>
+      <c r="J432" s="4">
+        <v>1</v>
+      </c>
+      <c r="K432" s="4">
+        <v>1</v>
+      </c>
+      <c r="L432" s="4">
+        <v>1</v>
+      </c>
+      <c r="M432" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A433" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B433">
+        <v>20</v>
+      </c>
+      <c r="C433" t="s">
+        <v>18</v>
+      </c>
+      <c r="D433" t="s">
+        <v>19</v>
+      </c>
+      <c r="E433" t="s">
+        <v>12</v>
+      </c>
+      <c r="F433" s="2">
+        <v>17</v>
+      </c>
+      <c r="G433" s="3">
+        <v>0</v>
+      </c>
+      <c r="H433" s="4">
+        <v>1</v>
+      </c>
+      <c r="I433" s="4">
+        <v>1</v>
+      </c>
+      <c r="J433" s="4">
+        <v>1</v>
+      </c>
+      <c r="K433" s="4">
+        <v>1</v>
+      </c>
+      <c r="L433" s="4">
+        <v>1</v>
+      </c>
+      <c r="M433" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A434" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B434">
+        <v>20</v>
+      </c>
+      <c r="C434" t="s">
+        <v>18</v>
+      </c>
+      <c r="D434" t="s">
+        <v>19</v>
+      </c>
+      <c r="E434" t="s">
+        <v>12</v>
+      </c>
+      <c r="F434" s="2">
+        <v>23</v>
+      </c>
+      <c r="G434" s="3">
+        <v>0</v>
+      </c>
+      <c r="H434" s="3">
+        <v>0</v>
+      </c>
+      <c r="I434" s="4">
+        <v>1</v>
+      </c>
+      <c r="J434" s="4">
+        <v>1</v>
+      </c>
+      <c r="K434" s="4">
+        <v>1</v>
+      </c>
+      <c r="L434" s="4">
+        <v>1</v>
+      </c>
+      <c r="M434" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A435" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B435">
+        <v>20</v>
+      </c>
+      <c r="C435" t="s">
+        <v>18</v>
+      </c>
+      <c r="D435" t="s">
+        <v>19</v>
+      </c>
+      <c r="E435" t="s">
+        <v>12</v>
+      </c>
+      <c r="F435" s="2">
+        <v>10</v>
+      </c>
+      <c r="G435" s="3">
+        <v>0</v>
+      </c>
+      <c r="H435" s="3">
+        <v>0</v>
+      </c>
+      <c r="I435" s="3">
+        <v>0</v>
+      </c>
+      <c r="J435" s="3">
+        <v>0</v>
+      </c>
+      <c r="K435" s="3">
+        <v>0</v>
+      </c>
+      <c r="L435" s="4">
+        <v>1</v>
+      </c>
+      <c r="M435" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A436" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B436">
+        <v>20</v>
+      </c>
+      <c r="C436" t="s">
+        <v>18</v>
+      </c>
+      <c r="D436" t="s">
+        <v>19</v>
+      </c>
+      <c r="E436" t="s">
+        <v>12</v>
+      </c>
+      <c r="F436" s="2">
+        <v>38</v>
+      </c>
+      <c r="G436" s="3">
+        <v>0</v>
+      </c>
+      <c r="H436" s="3">
+        <v>0</v>
+      </c>
+      <c r="I436" s="4">
+        <v>1</v>
+      </c>
+      <c r="J436" s="4">
+        <v>1</v>
+      </c>
+      <c r="K436" s="4">
+        <v>1</v>
+      </c>
+      <c r="L436" s="4">
+        <v>1</v>
+      </c>
+      <c r="M436" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A437" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B437">
+        <v>20</v>
+      </c>
+      <c r="C437" t="s">
+        <v>18</v>
+      </c>
+      <c r="D437" t="s">
+        <v>19</v>
+      </c>
+      <c r="E437" t="s">
+        <v>12</v>
+      </c>
+      <c r="F437" s="2">
+        <v>15</v>
+      </c>
+      <c r="G437" s="3">
+        <v>0</v>
+      </c>
+      <c r="H437" s="3">
+        <v>0</v>
+      </c>
+      <c r="I437" s="4">
+        <v>1</v>
+      </c>
+      <c r="J437" s="4">
+        <v>1</v>
+      </c>
+      <c r="K437" s="4">
+        <v>1</v>
+      </c>
+      <c r="L437" s="4">
+        <v>1</v>
+      </c>
+      <c r="M437" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A438" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B438">
+        <v>20</v>
+      </c>
+      <c r="C438" t="s">
+        <v>18</v>
+      </c>
+      <c r="D438" t="s">
+        <v>19</v>
+      </c>
+      <c r="E438" t="s">
+        <v>12</v>
+      </c>
+      <c r="F438" s="2">
+        <v>37</v>
+      </c>
+      <c r="G438" s="3">
+        <v>0</v>
+      </c>
+      <c r="H438" s="3">
+        <v>0</v>
+      </c>
+      <c r="I438" s="4">
+        <v>1</v>
+      </c>
+      <c r="J438" s="4">
+        <v>1</v>
+      </c>
+      <c r="K438" s="4">
+        <v>1</v>
+      </c>
+      <c r="L438" s="4">
+        <v>1</v>
+      </c>
+      <c r="M438" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A439" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B439">
+        <v>20</v>
+      </c>
+      <c r="C439" t="s">
+        <v>18</v>
+      </c>
+      <c r="D439" t="s">
+        <v>19</v>
+      </c>
+      <c r="E439" t="s">
+        <v>12</v>
+      </c>
+      <c r="F439" s="2">
+        <v>26</v>
+      </c>
+      <c r="G439" s="3">
+        <v>0</v>
+      </c>
+      <c r="H439" s="3">
+        <v>0</v>
+      </c>
+      <c r="I439" s="4">
+        <v>1</v>
+      </c>
+      <c r="J439" s="4">
+        <v>1</v>
+      </c>
+      <c r="K439" s="4">
+        <v>1</v>
+      </c>
+      <c r="L439" s="4">
+        <v>1</v>
+      </c>
+      <c r="M439" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A440" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B440">
+        <v>20</v>
+      </c>
+      <c r="C440" t="s">
+        <v>18</v>
+      </c>
+      <c r="D440" t="s">
+        <v>19</v>
+      </c>
+      <c r="E440" t="s">
+        <v>12</v>
+      </c>
+      <c r="F440" s="2">
+        <v>8</v>
+      </c>
+      <c r="G440" s="3">
+        <v>0</v>
+      </c>
+      <c r="H440" s="4">
+        <v>1</v>
+      </c>
+      <c r="I440" s="4">
+        <v>1</v>
+      </c>
+      <c r="J440" s="4">
+        <v>1</v>
+      </c>
+      <c r="K440" s="4">
+        <v>1</v>
+      </c>
+      <c r="L440" s="4">
+        <v>1</v>
+      </c>
+      <c r="M440" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A441" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B441">
+        <v>20</v>
+      </c>
+      <c r="C441" t="s">
+        <v>18</v>
+      </c>
+      <c r="D441" t="s">
+        <v>19</v>
+      </c>
+      <c r="E441" t="s">
+        <v>12</v>
+      </c>
+      <c r="F441" s="2">
+        <v>22</v>
+      </c>
+      <c r="G441" s="3">
+        <v>0</v>
+      </c>
+      <c r="H441" s="3">
+        <v>0</v>
+      </c>
+      <c r="I441" s="3">
+        <v>0</v>
+      </c>
+      <c r="J441" s="4">
+        <v>1</v>
+      </c>
+      <c r="K441" s="4">
+        <v>1</v>
+      </c>
+      <c r="L441" s="4">
+        <v>1</v>
+      </c>
+      <c r="M441" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A442" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B442">
+        <v>1</v>
+      </c>
+      <c r="C442" t="s">
+        <v>18</v>
+      </c>
+      <c r="D442" t="s">
+        <v>20</v>
+      </c>
+      <c r="E442" t="s">
+        <v>13</v>
+      </c>
+      <c r="F442" s="2">
+        <v>19</v>
+      </c>
+      <c r="G442" s="3">
+        <v>0</v>
+      </c>
+      <c r="H442" s="3">
+        <v>0</v>
+      </c>
+      <c r="I442" s="3">
+        <v>0</v>
+      </c>
+      <c r="J442" s="3">
+        <v>0</v>
+      </c>
+      <c r="K442" s="3">
+        <v>0</v>
+      </c>
+      <c r="L442" s="3">
+        <v>0</v>
+      </c>
+      <c r="M442" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A443" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B443">
+        <v>1</v>
+      </c>
+      <c r="C443" t="s">
+        <v>18</v>
+      </c>
+      <c r="D443" t="s">
+        <v>20</v>
+      </c>
+      <c r="E443" t="s">
+        <v>13</v>
+      </c>
+      <c r="F443" s="2">
+        <v>4</v>
+      </c>
+      <c r="G443" s="3">
+        <v>0</v>
+      </c>
+      <c r="H443" s="3">
+        <v>0</v>
+      </c>
+      <c r="I443" s="3">
+        <v>0</v>
+      </c>
+      <c r="J443" s="3">
+        <v>0</v>
+      </c>
+      <c r="K443" s="3">
+        <v>0</v>
+      </c>
+      <c r="L443" s="3">
+        <v>0</v>
+      </c>
+      <c r="M443" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A444" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B444">
+        <v>1</v>
+      </c>
+      <c r="C444" t="s">
+        <v>18</v>
+      </c>
+      <c r="D444" t="s">
+        <v>20</v>
+      </c>
+      <c r="E444" t="s">
+        <v>13</v>
+      </c>
+      <c r="F444" s="2">
+        <v>8</v>
+      </c>
+      <c r="G444" s="3">
+        <v>0</v>
+      </c>
+      <c r="H444" s="3">
+        <v>0</v>
+      </c>
+      <c r="I444" s="3">
+        <v>0</v>
+      </c>
+      <c r="J444" s="3">
+        <v>0</v>
+      </c>
+      <c r="K444" s="3">
+        <v>0</v>
+      </c>
+      <c r="L444" s="3">
+        <v>0</v>
+      </c>
+      <c r="M444" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A445" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B445">
+        <v>1</v>
+      </c>
+      <c r="C445" t="s">
+        <v>18</v>
+      </c>
+      <c r="D445" t="s">
+        <v>20</v>
+      </c>
+      <c r="E445" t="s">
+        <v>13</v>
+      </c>
+      <c r="F445" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G445" s="3">
+        <v>0</v>
+      </c>
+      <c r="H445" s="3">
+        <v>0</v>
+      </c>
+      <c r="I445" s="3">
+        <v>0</v>
+      </c>
+      <c r="J445" s="3">
+        <v>0</v>
+      </c>
+      <c r="K445" s="3">
+        <v>0</v>
+      </c>
+      <c r="L445" s="3">
+        <v>0</v>
+      </c>
+      <c r="M445" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A446" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B446">
+        <v>1</v>
+      </c>
+      <c r="C446" t="s">
+        <v>18</v>
+      </c>
+      <c r="D446" t="s">
+        <v>20</v>
+      </c>
+      <c r="E446" t="s">
+        <v>13</v>
+      </c>
+      <c r="F446" s="2">
+        <v>19</v>
+      </c>
+      <c r="G446" s="3">
+        <v>0</v>
+      </c>
+      <c r="H446" s="3">
+        <v>0</v>
+      </c>
+      <c r="I446" s="3">
+        <v>0</v>
+      </c>
+      <c r="J446" s="3">
+        <v>0</v>
+      </c>
+      <c r="K446" s="3">
+        <v>0</v>
+      </c>
+      <c r="L446" s="3">
+        <v>0</v>
+      </c>
+      <c r="M446" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A447" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B447">
+        <v>1</v>
+      </c>
+      <c r="C447" t="s">
+        <v>18</v>
+      </c>
+      <c r="D447" t="s">
+        <v>20</v>
+      </c>
+      <c r="E447" t="s">
+        <v>13</v>
+      </c>
+      <c r="F447" s="2">
+        <v>8</v>
+      </c>
+      <c r="G447" s="3">
+        <v>0</v>
+      </c>
+      <c r="H447" s="3">
+        <v>0</v>
+      </c>
+      <c r="I447" s="3">
+        <v>0</v>
+      </c>
+      <c r="J447" s="3">
+        <v>0</v>
+      </c>
+      <c r="K447" s="3">
+        <v>0</v>
+      </c>
+      <c r="L447" s="3">
+        <v>0</v>
+      </c>
+      <c r="M447" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A448" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B448">
+        <v>1</v>
+      </c>
+      <c r="C448" t="s">
+        <v>18</v>
+      </c>
+      <c r="D448" t="s">
+        <v>20</v>
+      </c>
+      <c r="E448" t="s">
+        <v>13</v>
+      </c>
+      <c r="F448" s="2">
+        <v>2</v>
+      </c>
+      <c r="G448" s="3">
+        <v>0</v>
+      </c>
+      <c r="H448" s="3">
+        <v>0</v>
+      </c>
+      <c r="I448" s="3">
+        <v>0</v>
+      </c>
+      <c r="J448" s="3">
+        <v>0</v>
+      </c>
+      <c r="K448" s="3">
+        <v>0</v>
+      </c>
+      <c r="L448" s="3">
+        <v>0</v>
+      </c>
+      <c r="M448" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A449" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B449">
+        <v>1</v>
+      </c>
+      <c r="C449" t="s">
+        <v>18</v>
+      </c>
+      <c r="D449" t="s">
+        <v>20</v>
+      </c>
+      <c r="E449" t="s">
+        <v>13</v>
+      </c>
+      <c r="F449" s="2">
+        <v>23</v>
+      </c>
+      <c r="G449" s="3">
+        <v>0</v>
+      </c>
+      <c r="H449" s="3">
+        <v>0</v>
+      </c>
+      <c r="I449" s="3">
+        <v>0</v>
+      </c>
+      <c r="J449" s="3">
+        <v>0</v>
+      </c>
+      <c r="K449" s="3">
+        <v>0</v>
+      </c>
+      <c r="L449" s="3">
+        <v>0</v>
+      </c>
+      <c r="M449" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A450" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+      <c r="C450" t="s">
+        <v>18</v>
+      </c>
+      <c r="D450" t="s">
+        <v>20</v>
+      </c>
+      <c r="E450" t="s">
+        <v>13</v>
+      </c>
+      <c r="F450" s="2">
+        <v>24</v>
+      </c>
+      <c r="G450" s="3">
+        <v>0</v>
+      </c>
+      <c r="H450" s="3">
+        <v>0</v>
+      </c>
+      <c r="I450" s="3">
+        <v>0</v>
+      </c>
+      <c r="J450" s="3">
+        <v>0</v>
+      </c>
+      <c r="K450" s="3">
+        <v>0</v>
+      </c>
+      <c r="L450" s="3">
+        <v>0</v>
+      </c>
+      <c r="M450" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A451" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B451">
+        <v>1</v>
+      </c>
+      <c r="C451" t="s">
+        <v>18</v>
+      </c>
+      <c r="D451" t="s">
+        <v>20</v>
+      </c>
+      <c r="E451" t="s">
+        <v>13</v>
+      </c>
+      <c r="F451" s="2">
+        <v>5</v>
+      </c>
+      <c r="G451" s="3">
+        <v>0</v>
+      </c>
+      <c r="H451" s="3">
+        <v>0</v>
+      </c>
+      <c r="I451" s="3">
+        <v>0</v>
+      </c>
+      <c r="J451" s="3">
+        <v>0</v>
+      </c>
+      <c r="K451" s="3">
+        <v>0</v>
+      </c>
+      <c r="L451" s="3">
+        <v>0</v>
+      </c>
+      <c r="M451" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A452" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+      <c r="C452" t="s">
+        <v>18</v>
+      </c>
+      <c r="D452" t="s">
+        <v>20</v>
+      </c>
+      <c r="E452" t="s">
+        <v>13</v>
+      </c>
+      <c r="F452" s="2">
+        <v>37</v>
+      </c>
+      <c r="G452" s="3">
+        <v>0</v>
+      </c>
+      <c r="H452" s="3">
+        <v>0</v>
+      </c>
+      <c r="I452" s="3">
+        <v>0</v>
+      </c>
+      <c r="J452" s="3">
+        <v>0</v>
+      </c>
+      <c r="K452" s="3">
+        <v>0</v>
+      </c>
+      <c r="L452" s="3">
+        <v>0</v>
+      </c>
+      <c r="M452" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A453" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B453">
+        <v>1</v>
+      </c>
+      <c r="C453" t="s">
+        <v>18</v>
+      </c>
+      <c r="D453" t="s">
+        <v>20</v>
+      </c>
+      <c r="E453" t="s">
+        <v>13</v>
+      </c>
+      <c r="F453" s="2">
+        <v>40</v>
+      </c>
+      <c r="G453" s="3">
+        <v>0</v>
+      </c>
+      <c r="H453" s="3">
+        <v>0</v>
+      </c>
+      <c r="I453" s="3">
+        <v>0</v>
+      </c>
+      <c r="J453" s="3">
+        <v>0</v>
+      </c>
+      <c r="K453" s="3">
+        <v>0</v>
+      </c>
+      <c r="L453" s="3">
+        <v>0</v>
+      </c>
+      <c r="M453" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A454" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B454">
+        <v>1</v>
+      </c>
+      <c r="C454" t="s">
+        <v>18</v>
+      </c>
+      <c r="D454" t="s">
+        <v>20</v>
+      </c>
+      <c r="E454" t="s">
+        <v>13</v>
+      </c>
+      <c r="F454" s="2">
+        <v>2</v>
+      </c>
+      <c r="G454" s="3">
+        <v>0</v>
+      </c>
+      <c r="H454" s="3">
+        <v>0</v>
+      </c>
+      <c r="I454" s="3">
+        <v>0</v>
+      </c>
+      <c r="J454" s="3">
+        <v>0</v>
+      </c>
+      <c r="K454" s="3">
+        <v>0</v>
+      </c>
+      <c r="L454" s="3">
+        <v>0</v>
+      </c>
+      <c r="M454" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A455" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B455">
+        <v>1</v>
+      </c>
+      <c r="C455" t="s">
+        <v>18</v>
+      </c>
+      <c r="D455" t="s">
+        <v>20</v>
+      </c>
+      <c r="E455" t="s">
+        <v>13</v>
+      </c>
+      <c r="F455" s="2">
+        <v>38</v>
+      </c>
+      <c r="G455" s="3">
+        <v>0</v>
+      </c>
+      <c r="H455" s="3">
+        <v>0</v>
+      </c>
+      <c r="I455" s="3">
+        <v>0</v>
+      </c>
+      <c r="J455" s="3">
+        <v>0</v>
+      </c>
+      <c r="K455" s="3">
+        <v>0</v>
+      </c>
+      <c r="L455" s="3">
+        <v>0</v>
+      </c>
+      <c r="M455" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A456" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B456">
+        <v>1</v>
+      </c>
+      <c r="C456" t="s">
+        <v>18</v>
+      </c>
+      <c r="D456" t="s">
+        <v>20</v>
+      </c>
+      <c r="E456" t="s">
+        <v>13</v>
+      </c>
+      <c r="F456" s="2">
+        <v>20</v>
+      </c>
+      <c r="G456" s="3">
+        <v>0</v>
+      </c>
+      <c r="H456" s="3">
+        <v>0</v>
+      </c>
+      <c r="I456" s="3">
+        <v>0</v>
+      </c>
+      <c r="J456" s="3">
+        <v>0</v>
+      </c>
+      <c r="K456" s="3">
+        <v>0</v>
+      </c>
+      <c r="L456" s="3">
+        <v>0</v>
+      </c>
+      <c r="M456" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A457" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B457">
+        <v>1</v>
+      </c>
+      <c r="C457" t="s">
+        <v>18</v>
+      </c>
+      <c r="D457" t="s">
+        <v>20</v>
+      </c>
+      <c r="E457" t="s">
+        <v>13</v>
+      </c>
+      <c r="F457" s="2">
+        <v>24</v>
+      </c>
+      <c r="G457" s="3">
+        <v>0</v>
+      </c>
+      <c r="H457" s="3">
+        <v>0</v>
+      </c>
+      <c r="I457" s="3">
+        <v>0</v>
+      </c>
+      <c r="J457" s="3">
+        <v>0</v>
+      </c>
+      <c r="K457" s="3">
+        <v>0</v>
+      </c>
+      <c r="L457" s="3">
+        <v>0</v>
+      </c>
+      <c r="M457" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A458" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B458">
+        <v>1</v>
+      </c>
+      <c r="C458" t="s">
+        <v>18</v>
+      </c>
+      <c r="D458" t="s">
+        <v>20</v>
+      </c>
+      <c r="E458" t="s">
+        <v>13</v>
+      </c>
+      <c r="F458" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G458" s="3">
+        <v>0</v>
+      </c>
+      <c r="H458" s="3">
+        <v>0</v>
+      </c>
+      <c r="I458" s="3">
+        <v>0</v>
+      </c>
+      <c r="J458" s="3">
+        <v>0</v>
+      </c>
+      <c r="K458" s="3">
+        <v>0</v>
+      </c>
+      <c r="L458" s="3">
+        <v>0</v>
+      </c>
+      <c r="M458" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A459" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B459">
+        <v>1</v>
+      </c>
+      <c r="C459" t="s">
+        <v>18</v>
+      </c>
+      <c r="D459" t="s">
+        <v>20</v>
+      </c>
+      <c r="E459" t="s">
+        <v>13</v>
+      </c>
+      <c r="F459" s="2">
+        <v>15</v>
+      </c>
+      <c r="G459" s="3">
+        <v>0</v>
+      </c>
+      <c r="H459" s="3">
+        <v>0</v>
+      </c>
+      <c r="I459" s="3">
+        <v>0</v>
+      </c>
+      <c r="J459" s="3">
+        <v>0</v>
+      </c>
+      <c r="K459" s="3">
+        <v>0</v>
+      </c>
+      <c r="L459" s="3">
+        <v>0</v>
+      </c>
+      <c r="M459" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A460" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B460">
+        <v>1</v>
+      </c>
+      <c r="C460" t="s">
+        <v>18</v>
+      </c>
+      <c r="D460" t="s">
+        <v>20</v>
+      </c>
+      <c r="E460" t="s">
+        <v>13</v>
+      </c>
+      <c r="F460" s="2">
+        <v>16</v>
+      </c>
+      <c r="G460" s="3">
+        <v>0</v>
+      </c>
+      <c r="H460" s="3">
+        <v>0</v>
+      </c>
+      <c r="I460" s="3">
+        <v>0</v>
+      </c>
+      <c r="J460" s="3">
+        <v>0</v>
+      </c>
+      <c r="K460" s="3">
+        <v>0</v>
+      </c>
+      <c r="L460" s="3">
+        <v>0</v>
+      </c>
+      <c r="M460" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A461" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B461">
+        <v>1</v>
+      </c>
+      <c r="C461" t="s">
+        <v>18</v>
+      </c>
+      <c r="D461" t="s">
+        <v>20</v>
+      </c>
+      <c r="E461" t="s">
+        <v>13</v>
+      </c>
+      <c r="F461" s="2">
+        <v>33</v>
+      </c>
+      <c r="G461" s="3">
+        <v>0</v>
+      </c>
+      <c r="H461" s="3">
+        <v>0</v>
+      </c>
+      <c r="I461" s="3">
+        <v>0</v>
+      </c>
+      <c r="J461" s="3">
+        <v>0</v>
+      </c>
+      <c r="K461" s="3">
+        <v>0</v>
+      </c>
+      <c r="L461" s="3">
+        <v>0</v>
+      </c>
+      <c r="M461" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A462" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B462">
+        <v>1</v>
+      </c>
+      <c r="C462" t="s">
+        <v>18</v>
+      </c>
+      <c r="D462" t="s">
+        <v>20</v>
+      </c>
+      <c r="E462" t="s">
+        <v>12</v>
+      </c>
+      <c r="F462" s="2">
+        <v>3</v>
+      </c>
+      <c r="G462" s="3">
+        <v>0</v>
+      </c>
+      <c r="H462" s="3">
+        <v>0</v>
+      </c>
+      <c r="I462" s="4">
+        <v>1</v>
+      </c>
+      <c r="J462" s="4">
+        <v>1</v>
+      </c>
+      <c r="K462" s="4">
+        <v>1</v>
+      </c>
+      <c r="L462" s="4">
+        <v>1</v>
+      </c>
+      <c r="M462" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A463" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B463">
+        <v>1</v>
+      </c>
+      <c r="C463" t="s">
+        <v>18</v>
+      </c>
+      <c r="D463" t="s">
+        <v>20</v>
+      </c>
+      <c r="E463" t="s">
+        <v>12</v>
+      </c>
+      <c r="F463" s="2">
+        <v>2</v>
+      </c>
+      <c r="G463" s="3">
+        <v>0</v>
+      </c>
+      <c r="H463" s="3">
+        <v>0</v>
+      </c>
+      <c r="I463" s="4">
+        <v>1</v>
+      </c>
+      <c r="J463" s="4">
+        <v>1</v>
+      </c>
+      <c r="K463" s="4">
+        <v>1</v>
+      </c>
+      <c r="L463" s="4">
+        <v>1</v>
+      </c>
+      <c r="M463" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A464" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B464">
+        <v>1</v>
+      </c>
+      <c r="C464" t="s">
+        <v>18</v>
+      </c>
+      <c r="D464" t="s">
+        <v>20</v>
+      </c>
+      <c r="E464" t="s">
+        <v>12</v>
+      </c>
+      <c r="F464" s="2">
+        <v>40</v>
+      </c>
+      <c r="G464" s="3">
+        <v>0</v>
+      </c>
+      <c r="H464" s="4">
+        <v>1</v>
+      </c>
+      <c r="I464" s="4">
+        <v>1</v>
+      </c>
+      <c r="J464" s="4">
+        <v>1</v>
+      </c>
+      <c r="K464" s="4">
+        <v>1</v>
+      </c>
+      <c r="L464" s="4">
+        <v>1</v>
+      </c>
+      <c r="M464" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A465" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B465">
+        <v>1</v>
+      </c>
+      <c r="C465" t="s">
+        <v>18</v>
+      </c>
+      <c r="D465" t="s">
+        <v>20</v>
+      </c>
+      <c r="E465" t="s">
+        <v>12</v>
+      </c>
+      <c r="F465" s="2">
+        <v>27</v>
+      </c>
+      <c r="G465" s="3">
+        <v>0</v>
+      </c>
+      <c r="H465" s="3">
+        <v>0</v>
+      </c>
+      <c r="I465" s="3">
+        <v>0</v>
+      </c>
+      <c r="J465" s="3">
+        <v>0</v>
+      </c>
+      <c r="K465" s="4">
+        <v>1</v>
+      </c>
+      <c r="L465" s="4">
+        <v>1</v>
+      </c>
+      <c r="M465" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A466" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B466">
+        <v>1</v>
+      </c>
+      <c r="C466" t="s">
+        <v>18</v>
+      </c>
+      <c r="D466" t="s">
+        <v>20</v>
+      </c>
+      <c r="E466" t="s">
+        <v>12</v>
+      </c>
+      <c r="F466" s="2">
+        <v>35</v>
+      </c>
+      <c r="G466" s="3">
+        <v>0</v>
+      </c>
+      <c r="H466" s="3">
+        <v>0</v>
+      </c>
+      <c r="I466" s="3">
+        <v>0</v>
+      </c>
+      <c r="J466" s="4">
+        <v>1</v>
+      </c>
+      <c r="K466" s="4">
+        <v>1</v>
+      </c>
+      <c r="L466" s="4">
+        <v>1</v>
+      </c>
+      <c r="M466" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A467" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B467">
+        <v>1</v>
+      </c>
+      <c r="C467" t="s">
+        <v>18</v>
+      </c>
+      <c r="D467" t="s">
+        <v>20</v>
+      </c>
+      <c r="E467" t="s">
+        <v>12</v>
+      </c>
+      <c r="F467" s="2">
+        <v>16</v>
+      </c>
+      <c r="G467" s="3">
+        <v>0</v>
+      </c>
+      <c r="H467" s="3">
+        <v>0</v>
+      </c>
+      <c r="I467" s="3">
+        <v>0</v>
+      </c>
+      <c r="J467" s="3">
+        <v>0</v>
+      </c>
+      <c r="K467" s="3">
+        <v>0</v>
+      </c>
+      <c r="L467" s="3">
+        <v>0</v>
+      </c>
+      <c r="M467" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A468" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B468">
+        <v>1</v>
+      </c>
+      <c r="C468" t="s">
+        <v>18</v>
+      </c>
+      <c r="D468" t="s">
+        <v>20</v>
+      </c>
+      <c r="E468" t="s">
+        <v>12</v>
+      </c>
+      <c r="F468" s="2">
+        <v>21</v>
+      </c>
+      <c r="G468" s="3">
+        <v>0</v>
+      </c>
+      <c r="H468" s="3">
+        <v>0</v>
+      </c>
+      <c r="I468" s="4">
+        <v>1</v>
+      </c>
+      <c r="J468" s="4">
+        <v>1</v>
+      </c>
+      <c r="K468" s="4">
+        <v>1</v>
+      </c>
+      <c r="L468" s="4">
+        <v>1</v>
+      </c>
+      <c r="M468" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A469" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B469">
+        <v>1</v>
+      </c>
+      <c r="C469" t="s">
+        <v>18</v>
+      </c>
+      <c r="D469" t="s">
+        <v>20</v>
+      </c>
+      <c r="E469" t="s">
+        <v>12</v>
+      </c>
+      <c r="F469" s="2">
+        <v>8</v>
+      </c>
+      <c r="G469" s="3">
+        <v>0</v>
+      </c>
+      <c r="H469" s="3">
+        <v>0</v>
+      </c>
+      <c r="I469" s="3">
+        <v>0</v>
+      </c>
+      <c r="J469" s="4">
+        <v>1</v>
+      </c>
+      <c r="K469" s="4">
+        <v>1</v>
+      </c>
+      <c r="L469" s="4">
+        <v>1</v>
+      </c>
+      <c r="M469" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A470" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+      <c r="C470" t="s">
+        <v>18</v>
+      </c>
+      <c r="D470" t="s">
+        <v>20</v>
+      </c>
+      <c r="E470" t="s">
+        <v>12</v>
+      </c>
+      <c r="F470" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G470" s="3">
+        <v>0</v>
+      </c>
+      <c r="H470" s="3">
+        <v>0</v>
+      </c>
+      <c r="I470" s="4">
+        <v>1</v>
+      </c>
+      <c r="J470" s="4">
+        <v>1</v>
+      </c>
+      <c r="K470" s="4">
+        <v>1</v>
+      </c>
+      <c r="L470" s="4">
+        <v>1</v>
+      </c>
+      <c r="M470" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A471" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B471">
+        <v>1</v>
+      </c>
+      <c r="C471" t="s">
+        <v>18</v>
+      </c>
+      <c r="D471" t="s">
+        <v>20</v>
+      </c>
+      <c r="E471" t="s">
+        <v>12</v>
+      </c>
+      <c r="F471" s="2">
+        <v>26</v>
+      </c>
+      <c r="G471" s="3">
+        <v>0</v>
+      </c>
+      <c r="H471" s="3">
+        <v>0</v>
+      </c>
+      <c r="I471" s="4">
+        <v>1</v>
+      </c>
+      <c r="J471" s="4">
+        <v>1</v>
+      </c>
+      <c r="K471" s="4">
+        <v>1</v>
+      </c>
+      <c r="L471" s="4">
+        <v>1</v>
+      </c>
+      <c r="M471" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A472" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+      <c r="C472" t="s">
+        <v>18</v>
+      </c>
+      <c r="D472" t="s">
+        <v>20</v>
+      </c>
+      <c r="E472" t="s">
+        <v>12</v>
+      </c>
+      <c r="F472" s="2">
+        <v>24</v>
+      </c>
+      <c r="G472" s="3">
+        <v>0</v>
+      </c>
+      <c r="H472" s="3">
+        <v>0</v>
+      </c>
+      <c r="I472" s="4">
+        <v>1</v>
+      </c>
+      <c r="J472" s="4">
+        <v>1</v>
+      </c>
+      <c r="K472" s="4">
+        <v>1</v>
+      </c>
+      <c r="L472" s="4">
+        <v>1</v>
+      </c>
+      <c r="M472" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A473" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B473">
+        <v>1</v>
+      </c>
+      <c r="C473" t="s">
+        <v>18</v>
+      </c>
+      <c r="D473" t="s">
+        <v>20</v>
+      </c>
+      <c r="E473" t="s">
+        <v>12</v>
+      </c>
+      <c r="F473" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G473" s="3">
+        <v>0</v>
+      </c>
+      <c r="H473" s="3">
+        <v>0</v>
+      </c>
+      <c r="I473" s="4">
+        <v>1</v>
+      </c>
+      <c r="J473" s="4">
+        <v>1</v>
+      </c>
+      <c r="K473" s="4">
+        <v>1</v>
+      </c>
+      <c r="L473" s="4">
+        <v>1</v>
+      </c>
+      <c r="M473" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A474" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B474">
+        <v>1</v>
+      </c>
+      <c r="C474" t="s">
+        <v>18</v>
+      </c>
+      <c r="D474" t="s">
+        <v>20</v>
+      </c>
+      <c r="E474" t="s">
+        <v>12</v>
+      </c>
+      <c r="F474" s="2">
+        <v>36</v>
+      </c>
+      <c r="G474" s="3">
+        <v>0</v>
+      </c>
+      <c r="H474" s="3">
+        <v>0</v>
+      </c>
+      <c r="I474" s="4">
+        <v>1</v>
+      </c>
+      <c r="J474" s="4">
+        <v>1</v>
+      </c>
+      <c r="K474" s="4">
+        <v>1</v>
+      </c>
+      <c r="L474" s="4">
+        <v>1</v>
+      </c>
+      <c r="M474" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A475" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B475">
+        <v>1</v>
+      </c>
+      <c r="C475" t="s">
+        <v>18</v>
+      </c>
+      <c r="D475" t="s">
+        <v>20</v>
+      </c>
+      <c r="E475" t="s">
+        <v>12</v>
+      </c>
+      <c r="F475" s="2">
+        <v>6</v>
+      </c>
+      <c r="G475" s="3">
+        <v>0</v>
+      </c>
+      <c r="H475" s="3">
+        <v>0</v>
+      </c>
+      <c r="I475" s="3">
+        <v>0</v>
+      </c>
+      <c r="J475" s="3">
+        <v>0</v>
+      </c>
+      <c r="K475" s="3">
+        <v>0</v>
+      </c>
+      <c r="L475" s="4">
+        <v>1</v>
+      </c>
+      <c r="M475" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A476" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B476">
+        <v>1</v>
+      </c>
+      <c r="C476" t="s">
+        <v>18</v>
+      </c>
+      <c r="D476" t="s">
+        <v>20</v>
+      </c>
+      <c r="E476" t="s">
+        <v>12</v>
+      </c>
+      <c r="F476" s="2">
+        <v>37</v>
+      </c>
+      <c r="G476" s="3">
+        <v>0</v>
+      </c>
+      <c r="H476" s="3">
+        <v>0</v>
+      </c>
+      <c r="I476" s="4">
+        <v>1</v>
+      </c>
+      <c r="J476" s="4">
+        <v>1</v>
+      </c>
+      <c r="K476" s="4">
+        <v>1</v>
+      </c>
+      <c r="L476" s="4">
+        <v>1</v>
+      </c>
+      <c r="M476" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A477" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B477">
+        <v>1</v>
+      </c>
+      <c r="C477" t="s">
+        <v>18</v>
+      </c>
+      <c r="D477" t="s">
+        <v>20</v>
+      </c>
+      <c r="E477" t="s">
+        <v>12</v>
+      </c>
+      <c r="F477" s="2">
+        <v>2</v>
+      </c>
+      <c r="G477" s="3">
+        <v>0</v>
+      </c>
+      <c r="H477" s="3">
+        <v>0</v>
+      </c>
+      <c r="I477" s="4">
+        <v>1</v>
+      </c>
+      <c r="J477" s="4">
+        <v>1</v>
+      </c>
+      <c r="K477" s="4">
+        <v>1</v>
+      </c>
+      <c r="L477" s="4">
+        <v>1</v>
+      </c>
+      <c r="M477" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A478" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B478">
+        <v>1</v>
+      </c>
+      <c r="C478" t="s">
+        <v>18</v>
+      </c>
+      <c r="D478" t="s">
+        <v>20</v>
+      </c>
+      <c r="E478" t="s">
+        <v>12</v>
+      </c>
+      <c r="F478" s="2">
+        <v>21</v>
+      </c>
+      <c r="G478" s="3">
+        <v>0</v>
+      </c>
+      <c r="H478" s="3">
+        <v>0</v>
+      </c>
+      <c r="I478" s="3">
+        <v>0</v>
+      </c>
+      <c r="J478" s="3">
+        <v>0</v>
+      </c>
+      <c r="K478" s="4">
+        <v>1</v>
+      </c>
+      <c r="L478" s="4">
+        <v>1</v>
+      </c>
+      <c r="M478" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A479" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B479">
+        <v>1</v>
+      </c>
+      <c r="C479" t="s">
+        <v>18</v>
+      </c>
+      <c r="D479" t="s">
+        <v>20</v>
+      </c>
+      <c r="E479" t="s">
+        <v>12</v>
+      </c>
+      <c r="F479" s="2">
+        <v>13</v>
+      </c>
+      <c r="G479" s="3">
+        <v>0</v>
+      </c>
+      <c r="H479" s="4">
+        <v>1</v>
+      </c>
+      <c r="I479" s="4">
+        <v>1</v>
+      </c>
+      <c r="J479" s="4">
+        <v>1</v>
+      </c>
+      <c r="K479" s="4">
+        <v>1</v>
+      </c>
+      <c r="L479" s="4">
+        <v>1</v>
+      </c>
+      <c r="M479" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A480" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B480">
+        <v>1</v>
+      </c>
+      <c r="C480" t="s">
+        <v>18</v>
+      </c>
+      <c r="D480" t="s">
+        <v>20</v>
+      </c>
+      <c r="E480" t="s">
+        <v>12</v>
+      </c>
+      <c r="F480" s="2">
+        <v>27</v>
+      </c>
+      <c r="G480" s="3">
+        <v>0</v>
+      </c>
+      <c r="H480" s="3">
+        <v>0</v>
+      </c>
+      <c r="I480" s="4">
+        <v>1</v>
+      </c>
+      <c r="J480" s="4">
+        <v>1</v>
+      </c>
+      <c r="K480" s="4">
+        <v>1</v>
+      </c>
+      <c r="L480" s="4">
+        <v>1</v>
+      </c>
+      <c r="M480" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A481" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B481">
+        <v>1</v>
+      </c>
+      <c r="C481" t="s">
+        <v>18</v>
+      </c>
+      <c r="D481" t="s">
+        <v>20</v>
+      </c>
+      <c r="E481" t="s">
+        <v>12</v>
+      </c>
+      <c r="F481" s="2">
+        <v>10</v>
+      </c>
+      <c r="G481" s="3">
+        <v>0</v>
+      </c>
+      <c r="H481" s="4">
+        <v>1</v>
+      </c>
+      <c r="I481" s="4">
+        <v>1</v>
+      </c>
+      <c r="J481" s="4">
+        <v>1</v>
+      </c>
+      <c r="K481" s="4">
+        <v>1</v>
+      </c>
+      <c r="L481" s="4">
+        <v>1</v>
+      </c>
+      <c r="M481" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>